<commit_message>
style(excel): se modifican los estilos de los archivos de excel
</commit_message>
<xml_diff>
--- a/GRUPAL-F165.xlsx
+++ b/GRUPAL-F165.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SENA\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\OneDrive\Desktop\sena app\BACKEND_SENA_APP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57E41FD-9174-4059-BC8C-C3CB5EBC1677}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85276C27-3354-4F7A-9EEB-216113F263BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Selección formato - Grupal" sheetId="1" r:id="rId1"/>
@@ -1404,12 +1404,6 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1428,14 +1422,8 @@
     <xf numFmtId="0" fontId="17" fillId="2" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="36" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="2" borderId="34" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="2" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1708,6 +1696,21 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="34" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1744,20 +1747,17 @@
     <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="25" fillId="2" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="2" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="46" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="25" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -2408,611 +2408,611 @@
   </sheetPr>
   <dimension ref="A1:AG48"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="F13" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.25" style="1" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="4.375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="5.25" style="1" customWidth="1"/>
+    <col min="1" max="1" width="28.19921875" style="1" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="4.3984375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="5.19921875" style="1" customWidth="1"/>
     <col min="4" max="4" width="24.5" style="1" customWidth="1"/>
-    <col min="5" max="6" width="21.375" style="1" customWidth="1"/>
+    <col min="5" max="6" width="21.3984375" style="1" customWidth="1"/>
     <col min="7" max="7" width="36.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="31.125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.875" style="1" customWidth="1"/>
-    <col min="10" max="11" width="8.625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="18.125" style="1" customWidth="1"/>
-    <col min="13" max="14" width="7.625" style="1" customWidth="1"/>
-    <col min="15" max="32" width="7.625" style="3" customWidth="1"/>
-    <col min="33" max="33" width="20.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="31.09765625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="20.8984375" style="1" customWidth="1"/>
+    <col min="10" max="11" width="8.59765625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="18.09765625" style="1" customWidth="1"/>
+    <col min="13" max="14" width="7.59765625" style="1" customWidth="1"/>
+    <col min="15" max="32" width="7.59765625" style="3" customWidth="1"/>
+    <col min="33" max="33" width="20.59765625" style="1" customWidth="1"/>
     <col min="34" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="39" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="54"/>
-      <c r="B1" s="54"/>
-      <c r="C1" s="55"/>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
-      <c r="H1" s="55"/>
-      <c r="I1" s="55"/>
-      <c r="J1" s="55"/>
-      <c r="K1" s="55"/>
-      <c r="L1" s="55"/>
-      <c r="M1" s="55"/>
-      <c r="N1" s="55"/>
-      <c r="O1" s="55"/>
-      <c r="P1" s="55"/>
-      <c r="Q1" s="55"/>
-      <c r="R1" s="55"/>
-      <c r="S1" s="55"/>
-      <c r="T1" s="55"/>
-      <c r="U1" s="55"/>
-      <c r="V1" s="55"/>
-      <c r="W1" s="55"/>
-      <c r="X1" s="55"/>
-      <c r="Y1" s="55"/>
-      <c r="Z1" s="55"/>
-      <c r="AA1" s="55"/>
-      <c r="AB1" s="55"/>
-      <c r="AC1" s="55"/>
-      <c r="AD1" s="55"/>
-      <c r="AE1" s="56"/>
-      <c r="AF1" s="56"/>
-      <c r="AG1" s="82" t="s">
+    <row r="1" spans="1:33" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="50"/>
+      <c r="B1" s="50"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="51"/>
+      <c r="G1" s="51"/>
+      <c r="H1" s="51"/>
+      <c r="I1" s="51"/>
+      <c r="J1" s="51"/>
+      <c r="K1" s="51"/>
+      <c r="L1" s="51"/>
+      <c r="M1" s="51"/>
+      <c r="N1" s="51"/>
+      <c r="O1" s="51"/>
+      <c r="P1" s="51"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="51"/>
+      <c r="S1" s="51"/>
+      <c r="T1" s="51"/>
+      <c r="U1" s="51"/>
+      <c r="V1" s="51"/>
+      <c r="W1" s="51"/>
+      <c r="X1" s="51"/>
+      <c r="Y1" s="51"/>
+      <c r="Z1" s="51"/>
+      <c r="AA1" s="51"/>
+      <c r="AB1" s="51"/>
+      <c r="AC1" s="51"/>
+      <c r="AD1" s="51"/>
+      <c r="AE1" s="52"/>
+      <c r="AF1" s="52"/>
+      <c r="AG1" s="78" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="57"/>
-      <c r="B2" s="58"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="59"/>
-      <c r="K2" s="59"/>
-      <c r="L2" s="59"/>
-      <c r="M2" s="59"/>
-      <c r="N2" s="59"/>
-      <c r="O2" s="59"/>
-      <c r="P2" s="59"/>
-      <c r="Q2" s="59"/>
-      <c r="R2" s="59"/>
-      <c r="S2" s="59"/>
-      <c r="T2" s="59"/>
-      <c r="U2" s="59"/>
-      <c r="V2" s="59"/>
-      <c r="W2" s="59"/>
-      <c r="X2" s="59"/>
-      <c r="Y2" s="59"/>
-      <c r="Z2" s="59"/>
-      <c r="AA2" s="59"/>
-      <c r="AB2" s="59"/>
-      <c r="AC2" s="59"/>
-      <c r="AD2" s="59"/>
-      <c r="AE2" s="61"/>
-      <c r="AF2" s="61"/>
-      <c r="AG2" s="82" t="s">
+    <row r="2" spans="1:33" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="53"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="55"/>
+      <c r="W2" s="55"/>
+      <c r="X2" s="55"/>
+      <c r="Y2" s="55"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="55"/>
+      <c r="AC2" s="55"/>
+      <c r="AD2" s="55"/>
+      <c r="AE2" s="57"/>
+      <c r="AF2" s="57"/>
+      <c r="AG2" s="78" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="83"/>
-      <c r="B3" s="160" t="s">
+    <row r="3" spans="1:33" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="79"/>
+      <c r="B3" s="144" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="160"/>
-      <c r="F3" s="160"/>
-      <c r="G3" s="160"/>
-      <c r="H3" s="160"/>
-      <c r="I3" s="160"/>
-      <c r="J3" s="160"/>
-      <c r="K3" s="160"/>
-      <c r="L3" s="160"/>
-      <c r="M3" s="160"/>
-      <c r="N3" s="160"/>
-      <c r="O3" s="160"/>
-      <c r="P3" s="160"/>
-      <c r="Q3" s="160"/>
-      <c r="R3" s="160"/>
-      <c r="S3" s="160"/>
-      <c r="T3" s="160"/>
-      <c r="U3" s="160"/>
-      <c r="V3" s="160"/>
-      <c r="W3" s="160"/>
-      <c r="X3" s="160"/>
-      <c r="Y3" s="160"/>
-      <c r="Z3" s="160"/>
-      <c r="AA3" s="160"/>
-      <c r="AB3" s="160"/>
-      <c r="AC3" s="160"/>
-      <c r="AD3" s="160"/>
-      <c r="AE3" s="160"/>
-      <c r="AF3" s="160"/>
-      <c r="AG3" s="161"/>
-    </row>
-    <row r="4" spans="1:33" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="83"/>
-      <c r="B4" s="162" t="s">
+      <c r="C3" s="144"/>
+      <c r="D3" s="144"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
+      <c r="H3" s="144"/>
+      <c r="I3" s="144"/>
+      <c r="J3" s="144"/>
+      <c r="K3" s="144"/>
+      <c r="L3" s="144"/>
+      <c r="M3" s="144"/>
+      <c r="N3" s="144"/>
+      <c r="O3" s="144"/>
+      <c r="P3" s="144"/>
+      <c r="Q3" s="144"/>
+      <c r="R3" s="144"/>
+      <c r="S3" s="144"/>
+      <c r="T3" s="144"/>
+      <c r="U3" s="144"/>
+      <c r="V3" s="144"/>
+      <c r="W3" s="144"/>
+      <c r="X3" s="144"/>
+      <c r="Y3" s="144"/>
+      <c r="Z3" s="144"/>
+      <c r="AA3" s="144"/>
+      <c r="AB3" s="144"/>
+      <c r="AC3" s="144"/>
+      <c r="AD3" s="144"/>
+      <c r="AE3" s="144"/>
+      <c r="AF3" s="144"/>
+      <c r="AG3" s="145"/>
+    </row>
+    <row r="4" spans="1:33" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="79"/>
+      <c r="B4" s="146" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="162"/>
-      <c r="D4" s="162"/>
-      <c r="E4" s="162"/>
-      <c r="F4" s="162"/>
-      <c r="G4" s="162"/>
-      <c r="H4" s="162"/>
-      <c r="I4" s="162"/>
-      <c r="J4" s="162"/>
-      <c r="K4" s="162"/>
-      <c r="L4" s="162"/>
-      <c r="M4" s="162"/>
-      <c r="N4" s="162"/>
-      <c r="O4" s="162"/>
-      <c r="P4" s="162"/>
-      <c r="Q4" s="162"/>
-      <c r="R4" s="162"/>
-      <c r="S4" s="162"/>
-      <c r="T4" s="162"/>
-      <c r="U4" s="162"/>
-      <c r="V4" s="162"/>
-      <c r="W4" s="162"/>
-      <c r="X4" s="162"/>
-      <c r="Y4" s="162"/>
-      <c r="Z4" s="162"/>
-      <c r="AA4" s="162"/>
-      <c r="AB4" s="162"/>
-      <c r="AC4" s="162"/>
-      <c r="AD4" s="162"/>
-      <c r="AE4" s="162"/>
-      <c r="AF4" s="162"/>
-      <c r="AG4" s="162"/>
-    </row>
-    <row r="5" spans="1:33" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="83"/>
-      <c r="B5" s="160" t="s">
+      <c r="C4" s="146"/>
+      <c r="D4" s="146"/>
+      <c r="E4" s="146"/>
+      <c r="F4" s="146"/>
+      <c r="G4" s="146"/>
+      <c r="H4" s="146"/>
+      <c r="I4" s="146"/>
+      <c r="J4" s="146"/>
+      <c r="K4" s="146"/>
+      <c r="L4" s="146"/>
+      <c r="M4" s="146"/>
+      <c r="N4" s="146"/>
+      <c r="O4" s="146"/>
+      <c r="P4" s="146"/>
+      <c r="Q4" s="146"/>
+      <c r="R4" s="146"/>
+      <c r="S4" s="146"/>
+      <c r="T4" s="146"/>
+      <c r="U4" s="146"/>
+      <c r="V4" s="146"/>
+      <c r="W4" s="146"/>
+      <c r="X4" s="146"/>
+      <c r="Y4" s="146"/>
+      <c r="Z4" s="146"/>
+      <c r="AA4" s="146"/>
+      <c r="AB4" s="146"/>
+      <c r="AC4" s="146"/>
+      <c r="AD4" s="146"/>
+      <c r="AE4" s="146"/>
+      <c r="AF4" s="146"/>
+      <c r="AG4" s="146"/>
+    </row>
+    <row r="5" spans="1:33" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="79"/>
+      <c r="B5" s="144" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="160"/>
-      <c r="D5" s="160"/>
-      <c r="E5" s="160"/>
-      <c r="F5" s="160"/>
-      <c r="G5" s="160"/>
-      <c r="H5" s="160"/>
-      <c r="I5" s="160"/>
-      <c r="J5" s="160"/>
-      <c r="K5" s="160"/>
-      <c r="L5" s="160"/>
-      <c r="M5" s="160"/>
-      <c r="N5" s="160"/>
-      <c r="O5" s="160"/>
-      <c r="P5" s="160"/>
-      <c r="Q5" s="160"/>
-      <c r="R5" s="160"/>
-      <c r="S5" s="160"/>
-      <c r="T5" s="160"/>
-      <c r="U5" s="160"/>
-      <c r="V5" s="160"/>
-      <c r="W5" s="160"/>
-      <c r="X5" s="160"/>
-      <c r="Y5" s="160"/>
-      <c r="Z5" s="160"/>
-      <c r="AA5" s="160"/>
-      <c r="AB5" s="160"/>
-      <c r="AC5" s="160"/>
-      <c r="AD5" s="160"/>
-      <c r="AE5" s="160"/>
-      <c r="AF5" s="160"/>
-      <c r="AG5" s="161"/>
-    </row>
-    <row r="6" spans="1:33" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="83"/>
-      <c r="B6" s="162" t="s">
+      <c r="C5" s="144"/>
+      <c r="D5" s="144"/>
+      <c r="E5" s="144"/>
+      <c r="F5" s="144"/>
+      <c r="G5" s="144"/>
+      <c r="H5" s="144"/>
+      <c r="I5" s="144"/>
+      <c r="J5" s="144"/>
+      <c r="K5" s="144"/>
+      <c r="L5" s="144"/>
+      <c r="M5" s="144"/>
+      <c r="N5" s="144"/>
+      <c r="O5" s="144"/>
+      <c r="P5" s="144"/>
+      <c r="Q5" s="144"/>
+      <c r="R5" s="144"/>
+      <c r="S5" s="144"/>
+      <c r="T5" s="144"/>
+      <c r="U5" s="144"/>
+      <c r="V5" s="144"/>
+      <c r="W5" s="144"/>
+      <c r="X5" s="144"/>
+      <c r="Y5" s="144"/>
+      <c r="Z5" s="144"/>
+      <c r="AA5" s="144"/>
+      <c r="AB5" s="144"/>
+      <c r="AC5" s="144"/>
+      <c r="AD5" s="144"/>
+      <c r="AE5" s="144"/>
+      <c r="AF5" s="144"/>
+      <c r="AG5" s="145"/>
+    </row>
+    <row r="6" spans="1:33" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="79"/>
+      <c r="B6" s="146" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="162"/>
-      <c r="D6" s="162"/>
-      <c r="E6" s="162"/>
-      <c r="F6" s="162"/>
-      <c r="G6" s="162"/>
-      <c r="H6" s="162"/>
-      <c r="I6" s="162"/>
-      <c r="J6" s="162"/>
-      <c r="K6" s="162"/>
-      <c r="L6" s="162"/>
-      <c r="M6" s="162"/>
-      <c r="N6" s="162"/>
-      <c r="O6" s="162"/>
-      <c r="P6" s="162"/>
-      <c r="Q6" s="162"/>
-      <c r="R6" s="162"/>
-      <c r="S6" s="162"/>
-      <c r="T6" s="162"/>
-      <c r="U6" s="162"/>
-      <c r="V6" s="162"/>
-      <c r="W6" s="162"/>
-      <c r="X6" s="162"/>
-      <c r="Y6" s="162"/>
-      <c r="Z6" s="162"/>
-      <c r="AA6" s="162"/>
-      <c r="AB6" s="162"/>
-      <c r="AC6" s="162"/>
-      <c r="AD6" s="162"/>
-      <c r="AE6" s="162"/>
-      <c r="AF6" s="162"/>
-      <c r="AG6" s="162"/>
-    </row>
-    <row r="7" spans="1:33" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="83"/>
-      <c r="B7" s="160" t="s">
+      <c r="C6" s="146"/>
+      <c r="D6" s="146"/>
+      <c r="E6" s="146"/>
+      <c r="F6" s="146"/>
+      <c r="G6" s="146"/>
+      <c r="H6" s="146"/>
+      <c r="I6" s="146"/>
+      <c r="J6" s="146"/>
+      <c r="K6" s="146"/>
+      <c r="L6" s="146"/>
+      <c r="M6" s="146"/>
+      <c r="N6" s="146"/>
+      <c r="O6" s="146"/>
+      <c r="P6" s="146"/>
+      <c r="Q6" s="146"/>
+      <c r="R6" s="146"/>
+      <c r="S6" s="146"/>
+      <c r="T6" s="146"/>
+      <c r="U6" s="146"/>
+      <c r="V6" s="146"/>
+      <c r="W6" s="146"/>
+      <c r="X6" s="146"/>
+      <c r="Y6" s="146"/>
+      <c r="Z6" s="146"/>
+      <c r="AA6" s="146"/>
+      <c r="AB6" s="146"/>
+      <c r="AC6" s="146"/>
+      <c r="AD6" s="146"/>
+      <c r="AE6" s="146"/>
+      <c r="AF6" s="146"/>
+      <c r="AG6" s="146"/>
+    </row>
+    <row r="7" spans="1:33" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="79"/>
+      <c r="B7" s="144" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="160"/>
-      <c r="D7" s="160"/>
-      <c r="E7" s="160"/>
-      <c r="F7" s="160"/>
-      <c r="G7" s="160"/>
-      <c r="H7" s="160"/>
-      <c r="I7" s="160"/>
-      <c r="J7" s="160"/>
-      <c r="K7" s="160"/>
-      <c r="L7" s="160"/>
-      <c r="M7" s="160"/>
-      <c r="N7" s="160"/>
-      <c r="O7" s="160"/>
-      <c r="P7" s="160"/>
-      <c r="Q7" s="160"/>
-      <c r="R7" s="160"/>
-      <c r="S7" s="160"/>
-      <c r="T7" s="160"/>
-      <c r="U7" s="160"/>
-      <c r="V7" s="160"/>
-      <c r="W7" s="160"/>
-      <c r="X7" s="160"/>
-      <c r="Y7" s="160"/>
-      <c r="Z7" s="160"/>
-      <c r="AA7" s="160"/>
-      <c r="AB7" s="160"/>
-      <c r="AC7" s="160"/>
-      <c r="AD7" s="160"/>
-      <c r="AE7" s="160"/>
-      <c r="AF7" s="160"/>
-      <c r="AG7" s="161"/>
-    </row>
-    <row r="8" spans="1:33" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="84"/>
-      <c r="B8" s="141" t="s">
+      <c r="C7" s="144"/>
+      <c r="D7" s="144"/>
+      <c r="E7" s="144"/>
+      <c r="F7" s="144"/>
+      <c r="G7" s="144"/>
+      <c r="H7" s="144"/>
+      <c r="I7" s="144"/>
+      <c r="J7" s="144"/>
+      <c r="K7" s="144"/>
+      <c r="L7" s="144"/>
+      <c r="M7" s="144"/>
+      <c r="N7" s="144"/>
+      <c r="O7" s="144"/>
+      <c r="P7" s="144"/>
+      <c r="Q7" s="144"/>
+      <c r="R7" s="144"/>
+      <c r="S7" s="144"/>
+      <c r="T7" s="144"/>
+      <c r="U7" s="144"/>
+      <c r="V7" s="144"/>
+      <c r="W7" s="144"/>
+      <c r="X7" s="144"/>
+      <c r="Y7" s="144"/>
+      <c r="Z7" s="144"/>
+      <c r="AA7" s="144"/>
+      <c r="AB7" s="144"/>
+      <c r="AC7" s="144"/>
+      <c r="AD7" s="144"/>
+      <c r="AE7" s="144"/>
+      <c r="AF7" s="144"/>
+      <c r="AG7" s="145"/>
+    </row>
+    <row r="8" spans="1:33" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="80"/>
+      <c r="B8" s="137" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="139"/>
-      <c r="D8" s="139"/>
-      <c r="E8" s="139"/>
-      <c r="F8" s="140"/>
-      <c r="G8" s="138" t="s">
+      <c r="C8" s="135"/>
+      <c r="D8" s="135"/>
+      <c r="E8" s="135"/>
+      <c r="F8" s="136"/>
+      <c r="G8" s="134" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="139"/>
-      <c r="I8" s="139"/>
-      <c r="J8" s="139"/>
-      <c r="K8" s="139"/>
-      <c r="L8" s="140"/>
-      <c r="M8" s="127" t="s">
+      <c r="H8" s="135"/>
+      <c r="I8" s="135"/>
+      <c r="J8" s="135"/>
+      <c r="K8" s="135"/>
+      <c r="L8" s="136"/>
+      <c r="M8" s="123" t="s">
         <v>6</v>
       </c>
-      <c r="N8" s="118"/>
-      <c r="O8" s="128"/>
-      <c r="P8" s="128"/>
-      <c r="Q8" s="125"/>
-      <c r="R8" s="125"/>
-      <c r="S8" s="125"/>
-      <c r="T8" s="125"/>
-      <c r="U8" s="125"/>
-      <c r="V8" s="125"/>
-      <c r="W8" s="125"/>
-      <c r="X8" s="125"/>
-      <c r="Y8" s="125"/>
-      <c r="Z8" s="125"/>
-      <c r="AA8" s="125"/>
-      <c r="AB8" s="125"/>
-      <c r="AC8" s="125"/>
-      <c r="AD8" s="125"/>
-      <c r="AE8" s="125"/>
-      <c r="AF8" s="125"/>
-      <c r="AG8" s="126"/>
-    </row>
-    <row r="9" spans="1:33" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="84"/>
-      <c r="B9" s="85"/>
-      <c r="C9" s="85"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="85"/>
-      <c r="I9" s="85"/>
-      <c r="J9" s="85"/>
-      <c r="K9" s="85"/>
-      <c r="L9" s="85"/>
-      <c r="M9" s="85"/>
-      <c r="N9" s="85"/>
-      <c r="O9" s="85"/>
-      <c r="P9" s="85"/>
-      <c r="Q9" s="85"/>
-      <c r="R9" s="85"/>
-      <c r="S9" s="85"/>
-      <c r="T9" s="85"/>
-      <c r="U9" s="85"/>
-      <c r="V9" s="85"/>
-      <c r="W9" s="85"/>
-      <c r="X9" s="85"/>
-      <c r="Y9" s="85"/>
-      <c r="Z9" s="85"/>
-      <c r="AA9" s="85"/>
-      <c r="AB9" s="85"/>
-      <c r="AC9" s="85"/>
-      <c r="AD9" s="85"/>
-      <c r="AE9" s="85"/>
-      <c r="AF9" s="85"/>
-      <c r="AG9" s="86"/>
-    </row>
-    <row r="10" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="83"/>
-      <c r="B10" s="158" t="s">
+      <c r="N8" s="114"/>
+      <c r="O8" s="124"/>
+      <c r="P8" s="124"/>
+      <c r="Q8" s="121"/>
+      <c r="R8" s="121"/>
+      <c r="S8" s="121"/>
+      <c r="T8" s="121"/>
+      <c r="U8" s="121"/>
+      <c r="V8" s="121"/>
+      <c r="W8" s="121"/>
+      <c r="X8" s="121"/>
+      <c r="Y8" s="121"/>
+      <c r="Z8" s="121"/>
+      <c r="AA8" s="121"/>
+      <c r="AB8" s="121"/>
+      <c r="AC8" s="121"/>
+      <c r="AD8" s="121"/>
+      <c r="AE8" s="121"/>
+      <c r="AF8" s="121"/>
+      <c r="AG8" s="122"/>
+    </row>
+    <row r="9" spans="1:33" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="80"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="81"/>
+      <c r="G9" s="81"/>
+      <c r="H9" s="81"/>
+      <c r="I9" s="81"/>
+      <c r="J9" s="81"/>
+      <c r="K9" s="81"/>
+      <c r="L9" s="81"/>
+      <c r="M9" s="81"/>
+      <c r="N9" s="81"/>
+      <c r="O9" s="81"/>
+      <c r="P9" s="81"/>
+      <c r="Q9" s="81"/>
+      <c r="R9" s="81"/>
+      <c r="S9" s="81"/>
+      <c r="T9" s="81"/>
+      <c r="U9" s="81"/>
+      <c r="V9" s="81"/>
+      <c r="W9" s="81"/>
+      <c r="X9" s="81"/>
+      <c r="Y9" s="81"/>
+      <c r="Z9" s="81"/>
+      <c r="AA9" s="81"/>
+      <c r="AB9" s="81"/>
+      <c r="AC9" s="81"/>
+      <c r="AD9" s="81"/>
+      <c r="AE9" s="81"/>
+      <c r="AF9" s="81"/>
+      <c r="AG9" s="82"/>
+    </row>
+    <row r="10" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="79"/>
+      <c r="B10" s="142" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="158"/>
-      <c r="D10" s="158"/>
-      <c r="E10" s="158"/>
-      <c r="F10" s="158"/>
-      <c r="G10" s="158"/>
-      <c r="H10" s="158"/>
-      <c r="I10" s="158"/>
-      <c r="J10" s="158"/>
-      <c r="K10" s="158"/>
-      <c r="L10" s="158"/>
-      <c r="M10" s="158"/>
-      <c r="N10" s="158"/>
-      <c r="O10" s="158"/>
-      <c r="P10" s="158"/>
-      <c r="Q10" s="158"/>
-      <c r="R10" s="158"/>
-      <c r="S10" s="158"/>
-      <c r="T10" s="158"/>
-      <c r="U10" s="158"/>
-      <c r="V10" s="158"/>
-      <c r="W10" s="158"/>
-      <c r="X10" s="158"/>
-      <c r="Y10" s="158"/>
-      <c r="Z10" s="158"/>
-      <c r="AA10" s="158"/>
-      <c r="AB10" s="158"/>
-      <c r="AC10" s="158"/>
-      <c r="AD10" s="158"/>
-      <c r="AE10" s="158"/>
-      <c r="AF10" s="158"/>
-      <c r="AG10" s="158"/>
-    </row>
-    <row r="11" spans="1:33" s="4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="49" t="s">
+      <c r="C10" s="142"/>
+      <c r="D10" s="142"/>
+      <c r="E10" s="142"/>
+      <c r="F10" s="142"/>
+      <c r="G10" s="142"/>
+      <c r="H10" s="142"/>
+      <c r="I10" s="142"/>
+      <c r="J10" s="142"/>
+      <c r="K10" s="142"/>
+      <c r="L10" s="142"/>
+      <c r="M10" s="142"/>
+      <c r="N10" s="142"/>
+      <c r="O10" s="142"/>
+      <c r="P10" s="142"/>
+      <c r="Q10" s="142"/>
+      <c r="R10" s="142"/>
+      <c r="S10" s="142"/>
+      <c r="T10" s="142"/>
+      <c r="U10" s="142"/>
+      <c r="V10" s="142"/>
+      <c r="W10" s="142"/>
+      <c r="X10" s="142"/>
+      <c r="Y10" s="142"/>
+      <c r="Z10" s="142"/>
+      <c r="AA10" s="142"/>
+      <c r="AB10" s="142"/>
+      <c r="AC10" s="142"/>
+      <c r="AD10" s="142"/>
+      <c r="AE10" s="142"/>
+      <c r="AF10" s="142"/>
+      <c r="AG10" s="142"/>
+    </row>
+    <row r="11" spans="1:33" s="4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="50"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="52" t="s">
+      <c r="C11" s="46"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="48" t="s">
         <v>37</v>
       </c>
       <c r="F11" s="8"/>
-      <c r="G11" s="53" t="s">
+      <c r="G11" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="159"/>
-      <c r="I11" s="159"/>
-      <c r="J11" s="159"/>
-      <c r="K11" s="159"/>
-      <c r="L11" s="159"/>
-      <c r="M11" s="119"/>
-      <c r="N11" s="119"/>
-      <c r="O11" s="78" t="s">
+      <c r="H11" s="143"/>
+      <c r="I11" s="143"/>
+      <c r="J11" s="143"/>
+      <c r="K11" s="143"/>
+      <c r="L11" s="143"/>
+      <c r="M11" s="115"/>
+      <c r="N11" s="115"/>
+      <c r="O11" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="P11" s="113"/>
-      <c r="Q11" s="113"/>
-      <c r="R11" s="113"/>
-      <c r="S11" s="113"/>
-      <c r="T11" s="113"/>
-      <c r="U11" s="113"/>
-      <c r="V11" s="113"/>
-      <c r="W11" s="113"/>
-      <c r="X11" s="113"/>
-      <c r="Y11" s="113"/>
-      <c r="Z11" s="113"/>
-      <c r="AA11" s="113"/>
-      <c r="AB11" s="113"/>
-      <c r="AC11" s="113"/>
-      <c r="AD11" s="113"/>
-      <c r="AE11" s="62"/>
-      <c r="AF11" s="123"/>
-      <c r="AG11" s="63"/>
-    </row>
-    <row r="12" spans="1:33" s="4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P11" s="109"/>
+      <c r="Q11" s="109"/>
+      <c r="R11" s="109"/>
+      <c r="S11" s="109"/>
+      <c r="T11" s="109"/>
+      <c r="U11" s="109"/>
+      <c r="V11" s="109"/>
+      <c r="W11" s="109"/>
+      <c r="X11" s="109"/>
+      <c r="Y11" s="109"/>
+      <c r="Z11" s="109"/>
+      <c r="AA11" s="109"/>
+      <c r="AB11" s="109"/>
+      <c r="AC11" s="109"/>
+      <c r="AD11" s="109"/>
+      <c r="AE11" s="58"/>
+      <c r="AF11" s="119"/>
+      <c r="AG11" s="59"/>
+    </row>
+    <row r="12" spans="1:33" s="4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="9"/>
-      <c r="D12" s="40"/>
-      <c r="E12" s="38"/>
-      <c r="F12" s="36"/>
-      <c r="G12" s="37" t="s">
+      <c r="D12" s="38"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="152"/>
-      <c r="I12" s="153"/>
-      <c r="J12" s="152"/>
-      <c r="K12" s="152"/>
-      <c r="L12" s="152"/>
-      <c r="M12" s="120"/>
-      <c r="N12" s="120"/>
+      <c r="H12" s="153"/>
+      <c r="I12" s="154"/>
+      <c r="J12" s="153"/>
+      <c r="K12" s="153"/>
+      <c r="L12" s="153"/>
+      <c r="M12" s="116"/>
+      <c r="N12" s="116"/>
       <c r="O12" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="P12" s="114"/>
-      <c r="Q12" s="114"/>
-      <c r="R12" s="114"/>
-      <c r="S12" s="114"/>
-      <c r="T12" s="114"/>
-      <c r="U12" s="114"/>
-      <c r="V12" s="114"/>
-      <c r="W12" s="114"/>
-      <c r="X12" s="114"/>
-      <c r="Y12" s="114"/>
-      <c r="Z12" s="114"/>
-      <c r="AA12" s="114"/>
-      <c r="AB12" s="114"/>
-      <c r="AC12" s="114"/>
-      <c r="AD12" s="114"/>
+      <c r="P12" s="110"/>
+      <c r="Q12" s="110"/>
+      <c r="R12" s="110"/>
+      <c r="S12" s="110"/>
+      <c r="T12" s="110"/>
+      <c r="U12" s="110"/>
+      <c r="V12" s="110"/>
+      <c r="W12" s="110"/>
+      <c r="X12" s="110"/>
+      <c r="Y12" s="110"/>
+      <c r="Z12" s="110"/>
+      <c r="AA12" s="110"/>
+      <c r="AB12" s="110"/>
+      <c r="AC12" s="110"/>
+      <c r="AD12" s="110"/>
       <c r="AE12" s="11"/>
       <c r="AF12" s="11"/>
       <c r="AG12" s="26"/>
     </row>
-    <row r="13" spans="1:33" s="4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="75" t="s">
+    <row r="13" spans="1:33" s="4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="76"/>
-      <c r="D13" s="77"/>
-      <c r="E13" s="35" t="s">
+      <c r="C13" s="72"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="160" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="36"/>
-      <c r="G13" s="92" t="s">
+      <c r="F13" s="34"/>
+      <c r="G13" s="88" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="34" t="s">
+      <c r="H13" s="162" t="s">
         <v>37</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="154"/>
-      <c r="K13" s="154"/>
-      <c r="L13" s="154"/>
-      <c r="M13" s="121"/>
-      <c r="N13" s="121"/>
+      <c r="J13" s="155"/>
+      <c r="K13" s="155"/>
+      <c r="L13" s="155"/>
+      <c r="M13" s="117"/>
+      <c r="N13" s="117"/>
       <c r="O13" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="P13" s="114"/>
-      <c r="Q13" s="114"/>
-      <c r="R13" s="114"/>
-      <c r="S13" s="114"/>
-      <c r="T13" s="114"/>
-      <c r="U13" s="114"/>
-      <c r="V13" s="114"/>
-      <c r="W13" s="114"/>
-      <c r="X13" s="114"/>
-      <c r="Y13" s="114"/>
-      <c r="Z13" s="114"/>
-      <c r="AA13" s="114"/>
-      <c r="AB13" s="114"/>
-      <c r="AC13" s="114"/>
-      <c r="AD13" s="114"/>
+      <c r="P13" s="110"/>
+      <c r="Q13" s="110"/>
+      <c r="R13" s="110"/>
+      <c r="S13" s="110"/>
+      <c r="T13" s="110"/>
+      <c r="U13" s="110"/>
+      <c r="V13" s="110"/>
+      <c r="W13" s="110"/>
+      <c r="X13" s="110"/>
+      <c r="Y13" s="110"/>
+      <c r="Z13" s="110"/>
+      <c r="AA13" s="110"/>
+      <c r="AB13" s="110"/>
+      <c r="AC13" s="110"/>
+      <c r="AD13" s="110"/>
       <c r="AE13" s="11"/>
       <c r="AF13" s="11"/>
       <c r="AG13" s="26"/>
     </row>
-    <row r="14" spans="1:33" s="4" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" s="4" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="39"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="42" t="s">
+      <c r="C14" s="37"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="159" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="43"/>
-      <c r="G14" s="48" t="s">
+      <c r="F14" s="40"/>
+      <c r="G14" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="44" t="s">
+      <c r="H14" s="161" t="s">
         <v>37</v>
       </c>
       <c r="I14" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="155"/>
-      <c r="K14" s="155"/>
-      <c r="L14" s="155"/>
-      <c r="M14" s="122"/>
-      <c r="N14" s="122"/>
+      <c r="J14" s="156"/>
+      <c r="K14" s="156"/>
+      <c r="L14" s="156"/>
+      <c r="M14" s="118"/>
+      <c r="N14" s="118"/>
       <c r="O14" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="P14" s="115"/>
-      <c r="Q14" s="115"/>
-      <c r="R14" s="115"/>
-      <c r="S14" s="115"/>
-      <c r="T14" s="115"/>
-      <c r="U14" s="115"/>
-      <c r="V14" s="115"/>
-      <c r="W14" s="115"/>
-      <c r="X14" s="115"/>
-      <c r="Y14" s="115"/>
-      <c r="Z14" s="115"/>
-      <c r="AA14" s="115"/>
-      <c r="AB14" s="115"/>
-      <c r="AC14" s="115"/>
-      <c r="AD14" s="115"/>
+      <c r="P14" s="111"/>
+      <c r="Q14" s="111"/>
+      <c r="R14" s="111"/>
+      <c r="S14" s="111"/>
+      <c r="T14" s="111"/>
+      <c r="U14" s="111"/>
+      <c r="V14" s="111"/>
+      <c r="W14" s="111"/>
+      <c r="X14" s="111"/>
+      <c r="Y14" s="111"/>
+      <c r="Z14" s="111"/>
+      <c r="AA14" s="111"/>
+      <c r="AB14" s="111"/>
+      <c r="AC14" s="111"/>
+      <c r="AD14" s="111"/>
       <c r="AE14" s="30"/>
       <c r="AF14" s="30"/>
       <c r="AG14" s="31"/>
     </row>
-    <row r="15" spans="1:33" s="4" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="87"/>
-      <c r="C15" s="88"/>
-      <c r="D15" s="88"/>
-      <c r="E15" s="88"/>
-      <c r="F15" s="88"/>
-      <c r="G15" s="88" t="s">
+    <row r="15" spans="1:33" s="4" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="83"/>
+      <c r="C15" s="84"/>
+      <c r="D15" s="84"/>
+      <c r="E15" s="84"/>
+      <c r="F15" s="84"/>
+      <c r="G15" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="88"/>
-      <c r="I15" s="88"/>
-      <c r="J15" s="89"/>
-      <c r="K15" s="89"/>
-      <c r="L15" s="90"/>
-      <c r="M15" s="88"/>
-      <c r="N15" s="88"/>
-      <c r="O15" s="91"/>
-      <c r="P15" s="91"/>
-      <c r="Q15" s="91"/>
-      <c r="R15" s="91"/>
-      <c r="S15" s="91"/>
-      <c r="T15" s="91"/>
-      <c r="U15" s="91"/>
-      <c r="V15" s="91"/>
-      <c r="W15" s="91"/>
-      <c r="X15" s="91"/>
-      <c r="Y15" s="91"/>
-      <c r="Z15" s="91"/>
-      <c r="AA15" s="91"/>
-      <c r="AB15" s="91"/>
-      <c r="AC15" s="91"/>
-      <c r="AD15" s="91"/>
-      <c r="AE15" s="89"/>
-      <c r="AF15" s="89"/>
-      <c r="AG15" s="90"/>
-    </row>
-    <row r="16" spans="1:33" s="2" customFormat="1" ht="75.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="150" t="s">
+      <c r="H15" s="84"/>
+      <c r="I15" s="84"/>
+      <c r="J15" s="85"/>
+      <c r="K15" s="85"/>
+      <c r="L15" s="86"/>
+      <c r="M15" s="84"/>
+      <c r="N15" s="84"/>
+      <c r="O15" s="87"/>
+      <c r="P15" s="87"/>
+      <c r="Q15" s="87"/>
+      <c r="R15" s="87"/>
+      <c r="S15" s="87"/>
+      <c r="T15" s="87"/>
+      <c r="U15" s="87"/>
+      <c r="V15" s="87"/>
+      <c r="W15" s="87"/>
+      <c r="X15" s="87"/>
+      <c r="Y15" s="87"/>
+      <c r="Z15" s="87"/>
+      <c r="AA15" s="87"/>
+      <c r="AB15" s="87"/>
+      <c r="AC15" s="87"/>
+      <c r="AD15" s="87"/>
+      <c r="AE15" s="85"/>
+      <c r="AF15" s="85"/>
+      <c r="AG15" s="86"/>
+    </row>
+    <row r="16" spans="1:33" s="2" customFormat="1" ht="75.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="151" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="15"/>
@@ -3022,48 +3022,48 @@
       <c r="G16" s="20"/>
       <c r="H16" s="16"/>
       <c r="I16" s="33"/>
-      <c r="J16" s="148" t="s">
+      <c r="J16" s="149" t="s">
         <v>25</v>
       </c>
-      <c r="K16" s="149"/>
-      <c r="L16" s="64"/>
-      <c r="M16" s="137" t="s">
+      <c r="K16" s="150"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="133" t="s">
         <v>75</v>
       </c>
-      <c r="N16" s="129"/>
-      <c r="O16" s="130"/>
-      <c r="P16" s="136" t="s">
+      <c r="N16" s="125"/>
+      <c r="O16" s="126"/>
+      <c r="P16" s="132" t="s">
         <v>28</v>
       </c>
-      <c r="Q16" s="131"/>
-      <c r="R16" s="132" t="s">
+      <c r="Q16" s="127"/>
+      <c r="R16" s="128" t="s">
         <v>27</v>
       </c>
-      <c r="S16" s="132"/>
-      <c r="T16" s="132"/>
-      <c r="U16" s="132"/>
-      <c r="V16" s="132"/>
-      <c r="W16" s="132"/>
-      <c r="X16" s="132"/>
-      <c r="Y16" s="132"/>
-      <c r="Z16" s="133" t="s">
+      <c r="S16" s="128"/>
+      <c r="T16" s="128"/>
+      <c r="U16" s="128"/>
+      <c r="V16" s="128"/>
+      <c r="W16" s="128"/>
+      <c r="X16" s="128"/>
+      <c r="Y16" s="128"/>
+      <c r="Z16" s="129" t="s">
         <v>70</v>
       </c>
-      <c r="AA16" s="134"/>
-      <c r="AB16" s="134"/>
-      <c r="AC16" s="134"/>
-      <c r="AD16" s="135"/>
-      <c r="AE16" s="147" t="s">
+      <c r="AA16" s="130"/>
+      <c r="AB16" s="130"/>
+      <c r="AC16" s="130"/>
+      <c r="AD16" s="131"/>
+      <c r="AE16" s="148" t="s">
         <v>55</v>
       </c>
-      <c r="AF16" s="147"/>
-      <c r="AG16" s="45" t="s">
+      <c r="AF16" s="148"/>
+      <c r="AG16" s="41" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" spans="2:33" s="2" customFormat="1" ht="138.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="151"/>
-      <c r="C17" s="74" t="s">
+      <c r="B17" s="152"/>
+      <c r="C17" s="70" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="17" t="s">
@@ -3081,7 +3081,7 @@
       <c r="H17" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="47" t="s">
+      <c r="I17" s="43" t="s">
         <v>24</v>
       </c>
       <c r="J17" s="14" t="s">
@@ -3132,13 +3132,13 @@
       <c r="Y17" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="Z17" s="116" t="s">
+      <c r="Z17" s="112" t="s">
         <v>31</v>
       </c>
-      <c r="AA17" s="117" t="s">
+      <c r="AA17" s="113" t="s">
         <v>29</v>
       </c>
-      <c r="AB17" s="117" t="s">
+      <c r="AB17" s="113" t="s">
         <v>30</v>
       </c>
       <c r="AC17" s="13" t="s">
@@ -3153,1130 +3153,1123 @@
       <c r="AF17" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="AG17" s="46" t="s">
+      <c r="AG17" s="42" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="2:33" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="93">
+    <row r="18" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="89">
         <v>1</v>
       </c>
-      <c r="C18" s="65"/>
-      <c r="D18" s="65"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="65"/>
-      <c r="G18" s="65"/>
-      <c r="H18" s="65"/>
-      <c r="I18" s="65"/>
-      <c r="J18" s="94"/>
-      <c r="K18" s="95"/>
-      <c r="L18" s="95"/>
-      <c r="M18" s="95"/>
-      <c r="N18" s="95"/>
-      <c r="O18" s="95"/>
-      <c r="P18" s="95"/>
-      <c r="Q18" s="95"/>
-      <c r="R18" s="95"/>
-      <c r="S18" s="95"/>
-      <c r="T18" s="95"/>
-      <c r="U18" s="95"/>
-      <c r="V18" s="95"/>
-      <c r="W18" s="95"/>
-      <c r="X18" s="95"/>
-      <c r="Y18" s="95"/>
-      <c r="Z18" s="95"/>
-      <c r="AA18" s="95"/>
-      <c r="AB18" s="95"/>
-      <c r="AC18" s="95"/>
-      <c r="AD18" s="95"/>
-      <c r="AE18" s="95"/>
-      <c r="AF18" s="95"/>
-      <c r="AG18" s="96"/>
-    </row>
-    <row r="19" spans="2:33" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="97">
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="61"/>
+      <c r="I18" s="61"/>
+      <c r="J18" s="90"/>
+      <c r="K18" s="91"/>
+      <c r="L18" s="91"/>
+      <c r="M18" s="91"/>
+      <c r="N18" s="91"/>
+      <c r="O18" s="91"/>
+      <c r="P18" s="91"/>
+      <c r="Q18" s="91"/>
+      <c r="R18" s="91"/>
+      <c r="S18" s="91"/>
+      <c r="T18" s="91"/>
+      <c r="U18" s="91"/>
+      <c r="V18" s="91"/>
+      <c r="W18" s="91"/>
+      <c r="X18" s="91"/>
+      <c r="Y18" s="91"/>
+      <c r="Z18" s="91"/>
+      <c r="AA18" s="91"/>
+      <c r="AB18" s="91"/>
+      <c r="AC18" s="91"/>
+      <c r="AD18" s="91"/>
+      <c r="AE18" s="91"/>
+      <c r="AF18" s="91"/>
+      <c r="AG18" s="92"/>
+    </row>
+    <row r="19" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="93">
         <v>2</v>
       </c>
-      <c r="C19" s="66"/>
-      <c r="D19" s="66"/>
-      <c r="E19" s="66"/>
-      <c r="F19" s="66"/>
-      <c r="G19" s="66"/>
-      <c r="H19" s="66"/>
-      <c r="I19" s="66"/>
-      <c r="J19" s="98"/>
-      <c r="K19" s="99"/>
-      <c r="L19" s="95"/>
-      <c r="M19" s="95"/>
-      <c r="N19" s="95"/>
-      <c r="O19" s="99"/>
-      <c r="P19" s="99"/>
-      <c r="Q19" s="99"/>
-      <c r="R19" s="99"/>
-      <c r="S19" s="99"/>
-      <c r="T19" s="99"/>
-      <c r="U19" s="99"/>
-      <c r="V19" s="99"/>
-      <c r="W19" s="99"/>
-      <c r="X19" s="99"/>
-      <c r="Y19" s="99"/>
-      <c r="Z19" s="99"/>
-      <c r="AA19" s="99"/>
-      <c r="AB19" s="99"/>
-      <c r="AC19" s="99"/>
-      <c r="AD19" s="99"/>
-      <c r="AE19" s="99"/>
-      <c r="AF19" s="99"/>
-      <c r="AG19" s="100"/>
-    </row>
-    <row r="20" spans="2:33" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="97">
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="62"/>
+      <c r="F19" s="62"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="62"/>
+      <c r="J19" s="94"/>
+      <c r="K19" s="95"/>
+      <c r="L19" s="91"/>
+      <c r="M19" s="91"/>
+      <c r="N19" s="91"/>
+      <c r="O19" s="95"/>
+      <c r="P19" s="95"/>
+      <c r="Q19" s="95"/>
+      <c r="R19" s="95"/>
+      <c r="S19" s="95"/>
+      <c r="T19" s="95"/>
+      <c r="U19" s="95"/>
+      <c r="V19" s="95"/>
+      <c r="W19" s="95"/>
+      <c r="X19" s="95"/>
+      <c r="Y19" s="95"/>
+      <c r="Z19" s="95"/>
+      <c r="AA19" s="95"/>
+      <c r="AB19" s="95"/>
+      <c r="AC19" s="95"/>
+      <c r="AD19" s="95"/>
+      <c r="AE19" s="95"/>
+      <c r="AF19" s="95"/>
+      <c r="AG19" s="96"/>
+    </row>
+    <row r="20" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="93">
         <v>3</v>
       </c>
-      <c r="C20" s="66"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="66"/>
-      <c r="F20" s="66"/>
-      <c r="G20" s="66"/>
-      <c r="H20" s="66"/>
-      <c r="I20" s="66"/>
-      <c r="J20" s="98"/>
-      <c r="K20" s="99"/>
-      <c r="L20" s="95"/>
-      <c r="M20" s="95"/>
-      <c r="N20" s="95"/>
-      <c r="O20" s="99"/>
-      <c r="P20" s="99"/>
-      <c r="Q20" s="99"/>
-      <c r="R20" s="99"/>
-      <c r="S20" s="99"/>
-      <c r="T20" s="99"/>
-      <c r="U20" s="99"/>
-      <c r="V20" s="99"/>
-      <c r="W20" s="99"/>
-      <c r="X20" s="99"/>
-      <c r="Y20" s="99"/>
-      <c r="Z20" s="99"/>
-      <c r="AA20" s="99"/>
-      <c r="AB20" s="99"/>
-      <c r="AC20" s="99"/>
-      <c r="AD20" s="99"/>
-      <c r="AE20" s="99"/>
-      <c r="AF20" s="99"/>
-      <c r="AG20" s="100"/>
-    </row>
-    <row r="21" spans="2:33" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="93">
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="62"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="62"/>
+      <c r="J20" s="94"/>
+      <c r="K20" s="95"/>
+      <c r="L20" s="91"/>
+      <c r="M20" s="91"/>
+      <c r="N20" s="91"/>
+      <c r="O20" s="95"/>
+      <c r="P20" s="95"/>
+      <c r="Q20" s="95"/>
+      <c r="R20" s="95"/>
+      <c r="S20" s="95"/>
+      <c r="T20" s="95"/>
+      <c r="U20" s="95"/>
+      <c r="V20" s="95"/>
+      <c r="W20" s="95"/>
+      <c r="X20" s="95"/>
+      <c r="Y20" s="95"/>
+      <c r="Z20" s="95"/>
+      <c r="AA20" s="95"/>
+      <c r="AB20" s="95"/>
+      <c r="AC20" s="95"/>
+      <c r="AD20" s="95"/>
+      <c r="AE20" s="95"/>
+      <c r="AF20" s="95"/>
+      <c r="AG20" s="96"/>
+    </row>
+    <row r="21" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="89">
         <v>4</v>
       </c>
-      <c r="C21" s="66"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="66"/>
-      <c r="F21" s="66"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="66"/>
-      <c r="I21" s="66"/>
-      <c r="J21" s="98"/>
-      <c r="K21" s="99"/>
-      <c r="L21" s="95"/>
-      <c r="M21" s="95"/>
-      <c r="N21" s="95"/>
-      <c r="O21" s="99"/>
-      <c r="P21" s="99"/>
-      <c r="Q21" s="99"/>
-      <c r="R21" s="99"/>
-      <c r="S21" s="99"/>
-      <c r="T21" s="99"/>
-      <c r="U21" s="99"/>
-      <c r="V21" s="99"/>
-      <c r="W21" s="99"/>
-      <c r="X21" s="99"/>
-      <c r="Y21" s="99"/>
-      <c r="Z21" s="99"/>
-      <c r="AA21" s="99"/>
-      <c r="AB21" s="99"/>
-      <c r="AC21" s="99"/>
-      <c r="AD21" s="99"/>
-      <c r="AE21" s="99"/>
-      <c r="AF21" s="99"/>
-      <c r="AG21" s="100"/>
-    </row>
-    <row r="22" spans="2:33" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="97">
+      <c r="C21" s="62"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="62"/>
+      <c r="F21" s="62"/>
+      <c r="G21" s="62"/>
+      <c r="H21" s="62"/>
+      <c r="I21" s="62"/>
+      <c r="J21" s="94"/>
+      <c r="K21" s="95"/>
+      <c r="L21" s="91"/>
+      <c r="M21" s="91"/>
+      <c r="N21" s="91"/>
+      <c r="O21" s="95"/>
+      <c r="P21" s="95"/>
+      <c r="Q21" s="95"/>
+      <c r="R21" s="95"/>
+      <c r="S21" s="95"/>
+      <c r="T21" s="95"/>
+      <c r="U21" s="95"/>
+      <c r="V21" s="95"/>
+      <c r="W21" s="95"/>
+      <c r="X21" s="95"/>
+      <c r="Y21" s="95"/>
+      <c r="Z21" s="95"/>
+      <c r="AA21" s="95"/>
+      <c r="AB21" s="95"/>
+      <c r="AC21" s="95"/>
+      <c r="AD21" s="95"/>
+      <c r="AE21" s="95"/>
+      <c r="AF21" s="95"/>
+      <c r="AG21" s="96"/>
+    </row>
+    <row r="22" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="93">
         <v>5</v>
       </c>
-      <c r="C22" s="66"/>
-      <c r="D22" s="66"/>
-      <c r="E22" s="66"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="66"/>
-      <c r="H22" s="66"/>
-      <c r="I22" s="66"/>
-      <c r="J22" s="98"/>
-      <c r="K22" s="99"/>
-      <c r="L22" s="95"/>
-      <c r="M22" s="95"/>
-      <c r="N22" s="95"/>
-      <c r="O22" s="99"/>
-      <c r="P22" s="99"/>
-      <c r="Q22" s="99"/>
-      <c r="R22" s="99"/>
-      <c r="S22" s="99"/>
-      <c r="T22" s="99"/>
-      <c r="U22" s="99"/>
-      <c r="V22" s="99"/>
-      <c r="W22" s="99"/>
-      <c r="X22" s="99"/>
-      <c r="Y22" s="99"/>
-      <c r="Z22" s="99"/>
-      <c r="AA22" s="99"/>
-      <c r="AB22" s="99"/>
-      <c r="AC22" s="99"/>
-      <c r="AD22" s="99"/>
-      <c r="AE22" s="99"/>
-      <c r="AF22" s="99"/>
-      <c r="AG22" s="100"/>
-    </row>
-    <row r="23" spans="2:33" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="97">
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="62"/>
+      <c r="G22" s="62"/>
+      <c r="H22" s="62"/>
+      <c r="I22" s="62"/>
+      <c r="J22" s="94"/>
+      <c r="K22" s="95"/>
+      <c r="L22" s="91"/>
+      <c r="M22" s="91"/>
+      <c r="N22" s="91"/>
+      <c r="O22" s="95"/>
+      <c r="P22" s="95"/>
+      <c r="Q22" s="95"/>
+      <c r="R22" s="95"/>
+      <c r="S22" s="95"/>
+      <c r="T22" s="95"/>
+      <c r="U22" s="95"/>
+      <c r="V22" s="95"/>
+      <c r="W22" s="95"/>
+      <c r="X22" s="95"/>
+      <c r="Y22" s="95"/>
+      <c r="Z22" s="95"/>
+      <c r="AA22" s="95"/>
+      <c r="AB22" s="95"/>
+      <c r="AC22" s="95"/>
+      <c r="AD22" s="95"/>
+      <c r="AE22" s="95"/>
+      <c r="AF22" s="95"/>
+      <c r="AG22" s="96"/>
+    </row>
+    <row r="23" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="93">
         <v>6</v>
       </c>
-      <c r="C23" s="66"/>
-      <c r="D23" s="66"/>
-      <c r="E23" s="66"/>
-      <c r="F23" s="66"/>
-      <c r="G23" s="66"/>
-      <c r="H23" s="66"/>
-      <c r="I23" s="66"/>
-      <c r="J23" s="98"/>
-      <c r="K23" s="67"/>
-      <c r="L23" s="95"/>
-      <c r="M23" s="95"/>
-      <c r="N23" s="95"/>
-      <c r="O23" s="67"/>
-      <c r="P23" s="67"/>
-      <c r="Q23" s="67"/>
-      <c r="R23" s="67"/>
-      <c r="S23" s="67"/>
-      <c r="T23" s="67"/>
-      <c r="U23" s="67"/>
-      <c r="V23" s="67"/>
-      <c r="W23" s="67"/>
-      <c r="X23" s="67"/>
-      <c r="Y23" s="67"/>
-      <c r="Z23" s="67"/>
-      <c r="AA23" s="67"/>
-      <c r="AB23" s="67"/>
-      <c r="AC23" s="67"/>
-      <c r="AD23" s="67"/>
-      <c r="AE23" s="67"/>
-      <c r="AF23" s="67"/>
-      <c r="AG23" s="68"/>
-    </row>
-    <row r="24" spans="2:33" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="93">
+      <c r="C23" s="62"/>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="94"/>
+      <c r="K23" s="63"/>
+      <c r="L23" s="91"/>
+      <c r="M23" s="91"/>
+      <c r="N23" s="91"/>
+      <c r="O23" s="63"/>
+      <c r="P23" s="63"/>
+      <c r="Q23" s="63"/>
+      <c r="R23" s="63"/>
+      <c r="S23" s="63"/>
+      <c r="T23" s="63"/>
+      <c r="U23" s="63"/>
+      <c r="V23" s="63"/>
+      <c r="W23" s="63"/>
+      <c r="X23" s="63"/>
+      <c r="Y23" s="63"/>
+      <c r="Z23" s="63"/>
+      <c r="AA23" s="63"/>
+      <c r="AB23" s="63"/>
+      <c r="AC23" s="63"/>
+      <c r="AD23" s="63"/>
+      <c r="AE23" s="63"/>
+      <c r="AF23" s="63"/>
+      <c r="AG23" s="64"/>
+    </row>
+    <row r="24" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="89">
         <v>7</v>
       </c>
-      <c r="C24" s="66"/>
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="66"/>
-      <c r="I24" s="66"/>
-      <c r="J24" s="98"/>
-      <c r="K24" s="99"/>
-      <c r="L24" s="95"/>
-      <c r="M24" s="95"/>
-      <c r="N24" s="95"/>
-      <c r="O24" s="99"/>
-      <c r="P24" s="99"/>
-      <c r="Q24" s="99"/>
-      <c r="R24" s="99"/>
-      <c r="S24" s="99"/>
-      <c r="T24" s="99"/>
-      <c r="U24" s="99"/>
-      <c r="V24" s="99"/>
-      <c r="W24" s="99"/>
-      <c r="X24" s="99"/>
-      <c r="Y24" s="99"/>
-      <c r="Z24" s="99"/>
-      <c r="AA24" s="99"/>
-      <c r="AB24" s="99"/>
-      <c r="AC24" s="99"/>
-      <c r="AD24" s="99"/>
-      <c r="AE24" s="99"/>
-      <c r="AF24" s="99"/>
-      <c r="AG24" s="100"/>
-    </row>
-    <row r="25" spans="2:33" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="97">
+      <c r="C24" s="62"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="62"/>
+      <c r="H24" s="62"/>
+      <c r="I24" s="62"/>
+      <c r="J24" s="94"/>
+      <c r="K24" s="95"/>
+      <c r="L24" s="91"/>
+      <c r="M24" s="91"/>
+      <c r="N24" s="91"/>
+      <c r="O24" s="95"/>
+      <c r="P24" s="95"/>
+      <c r="Q24" s="95"/>
+      <c r="R24" s="95"/>
+      <c r="S24" s="95"/>
+      <c r="T24" s="95"/>
+      <c r="U24" s="95"/>
+      <c r="V24" s="95"/>
+      <c r="W24" s="95"/>
+      <c r="X24" s="95"/>
+      <c r="Y24" s="95"/>
+      <c r="Z24" s="95"/>
+      <c r="AA24" s="95"/>
+      <c r="AB24" s="95"/>
+      <c r="AC24" s="95"/>
+      <c r="AD24" s="95"/>
+      <c r="AE24" s="95"/>
+      <c r="AF24" s="95"/>
+      <c r="AG24" s="96"/>
+    </row>
+    <row r="25" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="93">
         <v>8</v>
       </c>
-      <c r="C25" s="66"/>
-      <c r="D25" s="66"/>
-      <c r="E25" s="66"/>
-      <c r="F25" s="66"/>
-      <c r="G25" s="66"/>
-      <c r="H25" s="66"/>
-      <c r="I25" s="66"/>
-      <c r="J25" s="98"/>
-      <c r="K25" s="99"/>
-      <c r="L25" s="95"/>
-      <c r="M25" s="95"/>
-      <c r="N25" s="95"/>
-      <c r="O25" s="99"/>
-      <c r="P25" s="99"/>
-      <c r="Q25" s="99"/>
-      <c r="R25" s="99"/>
-      <c r="S25" s="99"/>
-      <c r="T25" s="99"/>
-      <c r="U25" s="99"/>
-      <c r="V25" s="99"/>
-      <c r="W25" s="99"/>
-      <c r="X25" s="99"/>
-      <c r="Y25" s="99"/>
-      <c r="Z25" s="99"/>
-      <c r="AA25" s="99"/>
-      <c r="AB25" s="99"/>
-      <c r="AC25" s="99"/>
-      <c r="AD25" s="99"/>
-      <c r="AE25" s="99"/>
-      <c r="AF25" s="99"/>
-      <c r="AG25" s="100"/>
-    </row>
-    <row r="26" spans="2:33" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="97">
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="62"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="62"/>
+      <c r="J25" s="94"/>
+      <c r="K25" s="95"/>
+      <c r="L25" s="91"/>
+      <c r="M25" s="91"/>
+      <c r="N25" s="91"/>
+      <c r="O25" s="95"/>
+      <c r="P25" s="95"/>
+      <c r="Q25" s="95"/>
+      <c r="R25" s="95"/>
+      <c r="S25" s="95"/>
+      <c r="T25" s="95"/>
+      <c r="U25" s="95"/>
+      <c r="V25" s="95"/>
+      <c r="W25" s="95"/>
+      <c r="X25" s="95"/>
+      <c r="Y25" s="95"/>
+      <c r="Z25" s="95"/>
+      <c r="AA25" s="95"/>
+      <c r="AB25" s="95"/>
+      <c r="AC25" s="95"/>
+      <c r="AD25" s="95"/>
+      <c r="AE25" s="95"/>
+      <c r="AF25" s="95"/>
+      <c r="AG25" s="96"/>
+    </row>
+    <row r="26" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="93">
         <v>9</v>
       </c>
-      <c r="C26" s="66"/>
-      <c r="D26" s="66"/>
-      <c r="E26" s="66"/>
-      <c r="F26" s="66"/>
-      <c r="G26" s="66"/>
-      <c r="H26" s="66"/>
-      <c r="I26" s="66"/>
-      <c r="J26" s="98"/>
-      <c r="K26" s="99"/>
-      <c r="L26" s="95"/>
-      <c r="M26" s="95"/>
-      <c r="N26" s="95"/>
-      <c r="O26" s="99"/>
-      <c r="P26" s="99"/>
-      <c r="Q26" s="99"/>
-      <c r="R26" s="99"/>
-      <c r="S26" s="99"/>
-      <c r="T26" s="99"/>
-      <c r="U26" s="99"/>
-      <c r="V26" s="99"/>
-      <c r="W26" s="99"/>
-      <c r="X26" s="99"/>
-      <c r="Y26" s="99"/>
-      <c r="Z26" s="99"/>
-      <c r="AA26" s="99"/>
-      <c r="AB26" s="99"/>
-      <c r="AC26" s="99"/>
-      <c r="AD26" s="99"/>
-      <c r="AE26" s="99"/>
-      <c r="AF26" s="99"/>
-      <c r="AG26" s="100"/>
-    </row>
-    <row r="27" spans="2:33" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="93">
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="62"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="62"/>
+      <c r="I26" s="62"/>
+      <c r="J26" s="94"/>
+      <c r="K26" s="95"/>
+      <c r="L26" s="91"/>
+      <c r="M26" s="91"/>
+      <c r="N26" s="91"/>
+      <c r="O26" s="95"/>
+      <c r="P26" s="95"/>
+      <c r="Q26" s="95"/>
+      <c r="R26" s="95"/>
+      <c r="S26" s="95"/>
+      <c r="T26" s="95"/>
+      <c r="U26" s="95"/>
+      <c r="V26" s="95"/>
+      <c r="W26" s="95"/>
+      <c r="X26" s="95"/>
+      <c r="Y26" s="95"/>
+      <c r="Z26" s="95"/>
+      <c r="AA26" s="95"/>
+      <c r="AB26" s="95"/>
+      <c r="AC26" s="95"/>
+      <c r="AD26" s="95"/>
+      <c r="AE26" s="95"/>
+      <c r="AF26" s="95"/>
+      <c r="AG26" s="96"/>
+    </row>
+    <row r="27" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="89">
         <v>10</v>
       </c>
-      <c r="C27" s="66"/>
-      <c r="D27" s="66"/>
-      <c r="E27" s="66"/>
-      <c r="F27" s="66"/>
-      <c r="G27" s="66"/>
-      <c r="H27" s="66"/>
-      <c r="I27" s="66"/>
-      <c r="J27" s="98"/>
-      <c r="K27" s="99"/>
-      <c r="L27" s="95"/>
-      <c r="M27" s="95"/>
-      <c r="N27" s="95"/>
-      <c r="O27" s="99"/>
-      <c r="P27" s="99"/>
-      <c r="Q27" s="99"/>
-      <c r="R27" s="99"/>
-      <c r="S27" s="99"/>
-      <c r="T27" s="99"/>
-      <c r="U27" s="99"/>
-      <c r="V27" s="99"/>
-      <c r="W27" s="99"/>
-      <c r="X27" s="99"/>
-      <c r="Y27" s="99"/>
-      <c r="Z27" s="99"/>
-      <c r="AA27" s="99"/>
-      <c r="AB27" s="99"/>
-      <c r="AC27" s="99"/>
-      <c r="AD27" s="99"/>
-      <c r="AE27" s="99"/>
-      <c r="AF27" s="99"/>
-      <c r="AG27" s="100"/>
-    </row>
-    <row r="28" spans="2:33" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="97">
+      <c r="C27" s="62"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="62"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="62"/>
+      <c r="J27" s="94"/>
+      <c r="K27" s="95"/>
+      <c r="L27" s="91"/>
+      <c r="M27" s="91"/>
+      <c r="N27" s="91"/>
+      <c r="O27" s="95"/>
+      <c r="P27" s="95"/>
+      <c r="Q27" s="95"/>
+      <c r="R27" s="95"/>
+      <c r="S27" s="95"/>
+      <c r="T27" s="95"/>
+      <c r="U27" s="95"/>
+      <c r="V27" s="95"/>
+      <c r="W27" s="95"/>
+      <c r="X27" s="95"/>
+      <c r="Y27" s="95"/>
+      <c r="Z27" s="95"/>
+      <c r="AA27" s="95"/>
+      <c r="AB27" s="95"/>
+      <c r="AC27" s="95"/>
+      <c r="AD27" s="95"/>
+      <c r="AE27" s="95"/>
+      <c r="AF27" s="95"/>
+      <c r="AG27" s="96"/>
+    </row>
+    <row r="28" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="93">
         <v>11</v>
       </c>
-      <c r="C28" s="66"/>
-      <c r="D28" s="66"/>
-      <c r="E28" s="66"/>
-      <c r="F28" s="66"/>
-      <c r="G28" s="66"/>
-      <c r="H28" s="66"/>
-      <c r="I28" s="66"/>
-      <c r="J28" s="98"/>
-      <c r="K28" s="99"/>
-      <c r="L28" s="95"/>
-      <c r="M28" s="95"/>
-      <c r="N28" s="95"/>
-      <c r="O28" s="99"/>
-      <c r="P28" s="99"/>
-      <c r="Q28" s="99"/>
-      <c r="R28" s="99"/>
-      <c r="S28" s="99"/>
-      <c r="T28" s="99"/>
-      <c r="U28" s="99"/>
-      <c r="V28" s="99"/>
-      <c r="W28" s="99"/>
-      <c r="X28" s="99"/>
-      <c r="Y28" s="99"/>
-      <c r="Z28" s="99"/>
-      <c r="AA28" s="99"/>
-      <c r="AB28" s="99"/>
-      <c r="AC28" s="99"/>
-      <c r="AD28" s="99"/>
-      <c r="AE28" s="99"/>
-      <c r="AF28" s="99"/>
-      <c r="AG28" s="100"/>
-    </row>
-    <row r="29" spans="2:33" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="97">
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="62"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="62"/>
+      <c r="J28" s="94"/>
+      <c r="K28" s="95"/>
+      <c r="L28" s="91"/>
+      <c r="M28" s="91"/>
+      <c r="N28" s="91"/>
+      <c r="O28" s="95"/>
+      <c r="P28" s="95"/>
+      <c r="Q28" s="95"/>
+      <c r="R28" s="95"/>
+      <c r="S28" s="95"/>
+      <c r="T28" s="95"/>
+      <c r="U28" s="95"/>
+      <c r="V28" s="95"/>
+      <c r="W28" s="95"/>
+      <c r="X28" s="95"/>
+      <c r="Y28" s="95"/>
+      <c r="Z28" s="95"/>
+      <c r="AA28" s="95"/>
+      <c r="AB28" s="95"/>
+      <c r="AC28" s="95"/>
+      <c r="AD28" s="95"/>
+      <c r="AE28" s="95"/>
+      <c r="AF28" s="95"/>
+      <c r="AG28" s="96"/>
+    </row>
+    <row r="29" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="93">
         <v>12</v>
       </c>
-      <c r="C29" s="66"/>
-      <c r="D29" s="66"/>
-      <c r="E29" s="66"/>
-      <c r="F29" s="66"/>
-      <c r="G29" s="66"/>
-      <c r="H29" s="66"/>
-      <c r="I29" s="66"/>
-      <c r="J29" s="98"/>
-      <c r="K29" s="99"/>
-      <c r="L29" s="95"/>
-      <c r="M29" s="95"/>
-      <c r="N29" s="95"/>
-      <c r="O29" s="99"/>
-      <c r="P29" s="99"/>
-      <c r="Q29" s="99"/>
-      <c r="R29" s="99"/>
-      <c r="S29" s="99"/>
-      <c r="T29" s="99"/>
-      <c r="U29" s="99"/>
-      <c r="V29" s="99"/>
-      <c r="W29" s="99"/>
-      <c r="X29" s="99"/>
-      <c r="Y29" s="99"/>
-      <c r="Z29" s="99"/>
-      <c r="AA29" s="99"/>
-      <c r="AB29" s="99"/>
-      <c r="AC29" s="99"/>
-      <c r="AD29" s="99"/>
-      <c r="AE29" s="99"/>
-      <c r="AF29" s="99"/>
-      <c r="AG29" s="100"/>
-    </row>
-    <row r="30" spans="2:33" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="93">
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="62"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="62"/>
+      <c r="J29" s="94"/>
+      <c r="K29" s="95"/>
+      <c r="L29" s="91"/>
+      <c r="M29" s="91"/>
+      <c r="N29" s="91"/>
+      <c r="O29" s="95"/>
+      <c r="P29" s="95"/>
+      <c r="Q29" s="95"/>
+      <c r="R29" s="95"/>
+      <c r="S29" s="95"/>
+      <c r="T29" s="95"/>
+      <c r="U29" s="95"/>
+      <c r="V29" s="95"/>
+      <c r="W29" s="95"/>
+      <c r="X29" s="95"/>
+      <c r="Y29" s="95"/>
+      <c r="Z29" s="95"/>
+      <c r="AA29" s="95"/>
+      <c r="AB29" s="95"/>
+      <c r="AC29" s="95"/>
+      <c r="AD29" s="95"/>
+      <c r="AE29" s="95"/>
+      <c r="AF29" s="95"/>
+      <c r="AG29" s="96"/>
+    </row>
+    <row r="30" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="89">
         <v>13</v>
       </c>
-      <c r="C30" s="66"/>
-      <c r="D30" s="66"/>
-      <c r="E30" s="66"/>
-      <c r="F30" s="66"/>
-      <c r="G30" s="66"/>
-      <c r="H30" s="66"/>
-      <c r="I30" s="66"/>
-      <c r="J30" s="98"/>
-      <c r="K30" s="99"/>
-      <c r="L30" s="95"/>
-      <c r="M30" s="95"/>
-      <c r="N30" s="95"/>
-      <c r="O30" s="99"/>
-      <c r="P30" s="99"/>
-      <c r="Q30" s="99"/>
-      <c r="R30" s="99"/>
-      <c r="S30" s="99"/>
-      <c r="T30" s="99"/>
-      <c r="U30" s="99"/>
-      <c r="V30" s="99"/>
-      <c r="W30" s="99"/>
-      <c r="X30" s="99"/>
-      <c r="Y30" s="99"/>
-      <c r="Z30" s="99"/>
-      <c r="AA30" s="99"/>
-      <c r="AB30" s="99"/>
-      <c r="AC30" s="99"/>
-      <c r="AD30" s="99"/>
-      <c r="AE30" s="99"/>
-      <c r="AF30" s="99"/>
-      <c r="AG30" s="100"/>
-    </row>
-    <row r="31" spans="2:33" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="97">
+      <c r="C30" s="62"/>
+      <c r="D30" s="62"/>
+      <c r="E30" s="62"/>
+      <c r="F30" s="62"/>
+      <c r="G30" s="62"/>
+      <c r="H30" s="62"/>
+      <c r="I30" s="62"/>
+      <c r="J30" s="94"/>
+      <c r="K30" s="95"/>
+      <c r="L30" s="91"/>
+      <c r="M30" s="91"/>
+      <c r="N30" s="91"/>
+      <c r="O30" s="95"/>
+      <c r="P30" s="95"/>
+      <c r="Q30" s="95"/>
+      <c r="R30" s="95"/>
+      <c r="S30" s="95"/>
+      <c r="T30" s="95"/>
+      <c r="U30" s="95"/>
+      <c r="V30" s="95"/>
+      <c r="W30" s="95"/>
+      <c r="X30" s="95"/>
+      <c r="Y30" s="95"/>
+      <c r="Z30" s="95"/>
+      <c r="AA30" s="95"/>
+      <c r="AB30" s="95"/>
+      <c r="AC30" s="95"/>
+      <c r="AD30" s="95"/>
+      <c r="AE30" s="95"/>
+      <c r="AF30" s="95"/>
+      <c r="AG30" s="96"/>
+    </row>
+    <row r="31" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="93">
         <v>14</v>
       </c>
-      <c r="C31" s="66"/>
-      <c r="D31" s="66"/>
-      <c r="E31" s="66"/>
-      <c r="F31" s="66"/>
-      <c r="G31" s="66"/>
-      <c r="H31" s="66"/>
-      <c r="I31" s="66"/>
-      <c r="J31" s="98"/>
-      <c r="K31" s="99"/>
-      <c r="L31" s="95"/>
-      <c r="M31" s="95"/>
-      <c r="N31" s="95"/>
-      <c r="O31" s="99"/>
-      <c r="P31" s="99"/>
-      <c r="Q31" s="99"/>
-      <c r="R31" s="99"/>
-      <c r="S31" s="99"/>
-      <c r="T31" s="99"/>
-      <c r="U31" s="99"/>
-      <c r="V31" s="99"/>
-      <c r="W31" s="99"/>
-      <c r="X31" s="99"/>
-      <c r="Y31" s="99"/>
-      <c r="Z31" s="99"/>
-      <c r="AA31" s="99"/>
-      <c r="AB31" s="99"/>
-      <c r="AC31" s="99"/>
-      <c r="AD31" s="99"/>
-      <c r="AE31" s="99"/>
-      <c r="AF31" s="99"/>
-      <c r="AG31" s="100"/>
-    </row>
-    <row r="32" spans="2:33" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="97">
+      <c r="C31" s="62"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="62"/>
+      <c r="F31" s="62"/>
+      <c r="G31" s="62"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="62"/>
+      <c r="J31" s="94"/>
+      <c r="K31" s="95"/>
+      <c r="L31" s="91"/>
+      <c r="M31" s="91"/>
+      <c r="N31" s="91"/>
+      <c r="O31" s="95"/>
+      <c r="P31" s="95"/>
+      <c r="Q31" s="95"/>
+      <c r="R31" s="95"/>
+      <c r="S31" s="95"/>
+      <c r="T31" s="95"/>
+      <c r="U31" s="95"/>
+      <c r="V31" s="95"/>
+      <c r="W31" s="95"/>
+      <c r="X31" s="95"/>
+      <c r="Y31" s="95"/>
+      <c r="Z31" s="95"/>
+      <c r="AA31" s="95"/>
+      <c r="AB31" s="95"/>
+      <c r="AC31" s="95"/>
+      <c r="AD31" s="95"/>
+      <c r="AE31" s="95"/>
+      <c r="AF31" s="95"/>
+      <c r="AG31" s="96"/>
+    </row>
+    <row r="32" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="93">
         <v>15</v>
       </c>
-      <c r="C32" s="66"/>
-      <c r="D32" s="66"/>
-      <c r="E32" s="66"/>
-      <c r="F32" s="66"/>
-      <c r="G32" s="66"/>
-      <c r="H32" s="66"/>
-      <c r="I32" s="66"/>
-      <c r="J32" s="98"/>
-      <c r="K32" s="99"/>
-      <c r="L32" s="95"/>
-      <c r="M32" s="95"/>
-      <c r="N32" s="95"/>
-      <c r="O32" s="99"/>
-      <c r="P32" s="99"/>
-      <c r="Q32" s="99"/>
-      <c r="R32" s="99"/>
-      <c r="S32" s="99"/>
-      <c r="T32" s="99"/>
-      <c r="U32" s="99"/>
-      <c r="V32" s="99"/>
-      <c r="W32" s="99"/>
-      <c r="X32" s="99"/>
-      <c r="Y32" s="99"/>
-      <c r="Z32" s="99"/>
-      <c r="AA32" s="99"/>
-      <c r="AB32" s="99"/>
-      <c r="AC32" s="99"/>
-      <c r="AD32" s="99"/>
-      <c r="AE32" s="99"/>
-      <c r="AF32" s="99"/>
-      <c r="AG32" s="100"/>
-    </row>
-    <row r="33" spans="2:33" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="93">
+      <c r="C32" s="62"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="62"/>
+      <c r="H32" s="62"/>
+      <c r="I32" s="62"/>
+      <c r="J32" s="94"/>
+      <c r="K32" s="95"/>
+      <c r="L32" s="91"/>
+      <c r="M32" s="91"/>
+      <c r="N32" s="91"/>
+      <c r="O32" s="95"/>
+      <c r="P32" s="95"/>
+      <c r="Q32" s="95"/>
+      <c r="R32" s="95"/>
+      <c r="S32" s="95"/>
+      <c r="T32" s="95"/>
+      <c r="U32" s="95"/>
+      <c r="V32" s="95"/>
+      <c r="W32" s="95"/>
+      <c r="X32" s="95"/>
+      <c r="Y32" s="95"/>
+      <c r="Z32" s="95"/>
+      <c r="AA32" s="95"/>
+      <c r="AB32" s="95"/>
+      <c r="AC32" s="95"/>
+      <c r="AD32" s="95"/>
+      <c r="AE32" s="95"/>
+      <c r="AF32" s="95"/>
+      <c r="AG32" s="96"/>
+    </row>
+    <row r="33" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="89">
         <v>16</v>
       </c>
-      <c r="C33" s="66"/>
-      <c r="D33" s="66"/>
-      <c r="E33" s="66"/>
-      <c r="F33" s="66"/>
-      <c r="G33" s="66"/>
-      <c r="H33" s="66"/>
-      <c r="I33" s="66"/>
-      <c r="J33" s="98"/>
-      <c r="K33" s="99"/>
-      <c r="L33" s="95"/>
-      <c r="M33" s="95"/>
-      <c r="N33" s="95"/>
-      <c r="O33" s="99"/>
-      <c r="P33" s="99"/>
-      <c r="Q33" s="99"/>
-      <c r="R33" s="99"/>
-      <c r="S33" s="99"/>
-      <c r="T33" s="99"/>
-      <c r="U33" s="99"/>
-      <c r="V33" s="99"/>
-      <c r="W33" s="99"/>
-      <c r="X33" s="99"/>
-      <c r="Y33" s="99"/>
-      <c r="Z33" s="99"/>
-      <c r="AA33" s="99"/>
-      <c r="AB33" s="99"/>
-      <c r="AC33" s="99"/>
-      <c r="AD33" s="99"/>
-      <c r="AE33" s="99"/>
-      <c r="AF33" s="99"/>
-      <c r="AG33" s="100"/>
-    </row>
-    <row r="34" spans="2:33" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="97">
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="62"/>
+      <c r="F33" s="62"/>
+      <c r="G33" s="62"/>
+      <c r="H33" s="62"/>
+      <c r="I33" s="62"/>
+      <c r="J33" s="94"/>
+      <c r="K33" s="95"/>
+      <c r="L33" s="91"/>
+      <c r="M33" s="91"/>
+      <c r="N33" s="91"/>
+      <c r="O33" s="95"/>
+      <c r="P33" s="95"/>
+      <c r="Q33" s="95"/>
+      <c r="R33" s="95"/>
+      <c r="S33" s="95"/>
+      <c r="T33" s="95"/>
+      <c r="U33" s="95"/>
+      <c r="V33" s="95"/>
+      <c r="W33" s="95"/>
+      <c r="X33" s="95"/>
+      <c r="Y33" s="95"/>
+      <c r="Z33" s="95"/>
+      <c r="AA33" s="95"/>
+      <c r="AB33" s="95"/>
+      <c r="AC33" s="95"/>
+      <c r="AD33" s="95"/>
+      <c r="AE33" s="95"/>
+      <c r="AF33" s="95"/>
+      <c r="AG33" s="96"/>
+    </row>
+    <row r="34" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="93">
         <v>17</v>
       </c>
-      <c r="C34" s="66"/>
-      <c r="D34" s="66"/>
-      <c r="E34" s="66"/>
-      <c r="F34" s="66"/>
-      <c r="G34" s="66"/>
-      <c r="H34" s="66"/>
-      <c r="I34" s="66"/>
-      <c r="J34" s="101"/>
-      <c r="K34" s="101"/>
-      <c r="L34" s="95"/>
-      <c r="M34" s="95"/>
-      <c r="N34" s="95"/>
-      <c r="O34" s="99"/>
-      <c r="P34" s="99"/>
-      <c r="Q34" s="99"/>
-      <c r="R34" s="99"/>
-      <c r="S34" s="99"/>
-      <c r="T34" s="99"/>
-      <c r="U34" s="99"/>
-      <c r="V34" s="99"/>
-      <c r="W34" s="99"/>
-      <c r="X34" s="99"/>
-      <c r="Y34" s="99"/>
-      <c r="Z34" s="99"/>
-      <c r="AA34" s="99"/>
-      <c r="AB34" s="99"/>
-      <c r="AC34" s="99"/>
-      <c r="AD34" s="99"/>
-      <c r="AE34" s="99"/>
-      <c r="AF34" s="99"/>
-      <c r="AG34" s="100"/>
-    </row>
-    <row r="35" spans="2:33" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="97">
+      <c r="C34" s="62"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="62"/>
+      <c r="F34" s="62"/>
+      <c r="G34" s="62"/>
+      <c r="H34" s="62"/>
+      <c r="I34" s="62"/>
+      <c r="J34" s="97"/>
+      <c r="K34" s="97"/>
+      <c r="L34" s="91"/>
+      <c r="M34" s="91"/>
+      <c r="N34" s="91"/>
+      <c r="O34" s="95"/>
+      <c r="P34" s="95"/>
+      <c r="Q34" s="95"/>
+      <c r="R34" s="95"/>
+      <c r="S34" s="95"/>
+      <c r="T34" s="95"/>
+      <c r="U34" s="95"/>
+      <c r="V34" s="95"/>
+      <c r="W34" s="95"/>
+      <c r="X34" s="95"/>
+      <c r="Y34" s="95"/>
+      <c r="Z34" s="95"/>
+      <c r="AA34" s="95"/>
+      <c r="AB34" s="95"/>
+      <c r="AC34" s="95"/>
+      <c r="AD34" s="95"/>
+      <c r="AE34" s="95"/>
+      <c r="AF34" s="95"/>
+      <c r="AG34" s="96"/>
+    </row>
+    <row r="35" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="93">
         <v>18</v>
       </c>
-      <c r="C35" s="66"/>
-      <c r="D35" s="66"/>
-      <c r="E35" s="66"/>
-      <c r="F35" s="66"/>
-      <c r="G35" s="66"/>
-      <c r="H35" s="66"/>
-      <c r="I35" s="66"/>
-      <c r="J35" s="101"/>
-      <c r="K35" s="101"/>
-      <c r="L35" s="95"/>
-      <c r="M35" s="95"/>
-      <c r="N35" s="95"/>
-      <c r="O35" s="99"/>
-      <c r="P35" s="99"/>
-      <c r="Q35" s="99"/>
-      <c r="R35" s="99"/>
-      <c r="S35" s="99"/>
-      <c r="T35" s="99"/>
-      <c r="U35" s="99"/>
-      <c r="V35" s="99"/>
-      <c r="W35" s="99"/>
-      <c r="X35" s="99"/>
-      <c r="Y35" s="99"/>
-      <c r="Z35" s="99"/>
-      <c r="AA35" s="99"/>
-      <c r="AB35" s="99"/>
-      <c r="AC35" s="99"/>
-      <c r="AD35" s="99"/>
-      <c r="AE35" s="99"/>
-      <c r="AF35" s="99"/>
-      <c r="AG35" s="100"/>
-    </row>
-    <row r="36" spans="2:33" ht="26.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="93">
+      <c r="C35" s="62"/>
+      <c r="D35" s="62"/>
+      <c r="E35" s="62"/>
+      <c r="F35" s="62"/>
+      <c r="G35" s="62"/>
+      <c r="H35" s="62"/>
+      <c r="I35" s="62"/>
+      <c r="J35" s="97"/>
+      <c r="K35" s="97"/>
+      <c r="L35" s="91"/>
+      <c r="M35" s="91"/>
+      <c r="N35" s="91"/>
+      <c r="O35" s="95"/>
+      <c r="P35" s="95"/>
+      <c r="Q35" s="95"/>
+      <c r="R35" s="95"/>
+      <c r="S35" s="95"/>
+      <c r="T35" s="95"/>
+      <c r="U35" s="95"/>
+      <c r="V35" s="95"/>
+      <c r="W35" s="95"/>
+      <c r="X35" s="95"/>
+      <c r="Y35" s="95"/>
+      <c r="Z35" s="95"/>
+      <c r="AA35" s="95"/>
+      <c r="AB35" s="95"/>
+      <c r="AC35" s="95"/>
+      <c r="AD35" s="95"/>
+      <c r="AE35" s="95"/>
+      <c r="AF35" s="95"/>
+      <c r="AG35" s="96"/>
+    </row>
+    <row r="36" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="89">
         <v>19</v>
       </c>
-      <c r="C36" s="66"/>
-      <c r="D36" s="69"/>
-      <c r="E36" s="69"/>
-      <c r="F36" s="69"/>
-      <c r="G36" s="69"/>
-      <c r="H36" s="69"/>
-      <c r="I36" s="69"/>
-      <c r="J36" s="102"/>
-      <c r="K36" s="102"/>
-      <c r="L36" s="95"/>
-      <c r="M36" s="124"/>
-      <c r="N36" s="124"/>
-      <c r="O36" s="103"/>
-      <c r="P36" s="103"/>
-      <c r="Q36" s="103"/>
-      <c r="R36" s="103"/>
-      <c r="S36" s="103"/>
-      <c r="T36" s="103"/>
-      <c r="U36" s="103"/>
-      <c r="V36" s="103"/>
-      <c r="W36" s="103"/>
-      <c r="X36" s="103"/>
-      <c r="Y36" s="103"/>
-      <c r="Z36" s="103"/>
-      <c r="AA36" s="103"/>
-      <c r="AB36" s="103"/>
-      <c r="AC36" s="103"/>
-      <c r="AD36" s="103"/>
-      <c r="AE36" s="103"/>
-      <c r="AF36" s="103"/>
-      <c r="AG36" s="104"/>
-    </row>
-    <row r="37" spans="2:33" ht="26.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B37" s="105">
+      <c r="C36" s="62"/>
+      <c r="D36" s="65"/>
+      <c r="E36" s="65"/>
+      <c r="F36" s="65"/>
+      <c r="G36" s="65"/>
+      <c r="H36" s="65"/>
+      <c r="I36" s="65"/>
+      <c r="J36" s="98"/>
+      <c r="K36" s="98"/>
+      <c r="L36" s="91"/>
+      <c r="M36" s="120"/>
+      <c r="N36" s="120"/>
+      <c r="O36" s="99"/>
+      <c r="P36" s="99"/>
+      <c r="Q36" s="99"/>
+      <c r="R36" s="99"/>
+      <c r="S36" s="99"/>
+      <c r="T36" s="99"/>
+      <c r="U36" s="99"/>
+      <c r="V36" s="99"/>
+      <c r="W36" s="99"/>
+      <c r="X36" s="99"/>
+      <c r="Y36" s="99"/>
+      <c r="Z36" s="99"/>
+      <c r="AA36" s="99"/>
+      <c r="AB36" s="99"/>
+      <c r="AC36" s="99"/>
+      <c r="AD36" s="99"/>
+      <c r="AE36" s="99"/>
+      <c r="AF36" s="99"/>
+      <c r="AG36" s="100"/>
+    </row>
+    <row r="37" spans="2:33" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="101">
         <v>20</v>
       </c>
-      <c r="C37" s="70"/>
-      <c r="D37" s="70"/>
-      <c r="E37" s="70"/>
-      <c r="F37" s="70"/>
-      <c r="G37" s="70"/>
-      <c r="H37" s="70"/>
-      <c r="I37" s="70"/>
-      <c r="J37" s="106"/>
-      <c r="K37" s="106"/>
-      <c r="L37" s="107"/>
-      <c r="M37" s="107"/>
-      <c r="N37" s="107"/>
-      <c r="O37" s="108"/>
-      <c r="P37" s="108"/>
-      <c r="Q37" s="108"/>
-      <c r="R37" s="108"/>
-      <c r="S37" s="108"/>
-      <c r="T37" s="108"/>
-      <c r="U37" s="108"/>
-      <c r="V37" s="108"/>
-      <c r="W37" s="108"/>
-      <c r="X37" s="108"/>
-      <c r="Y37" s="108"/>
-      <c r="Z37" s="108"/>
-      <c r="AA37" s="108"/>
-      <c r="AB37" s="108"/>
-      <c r="AC37" s="108"/>
-      <c r="AD37" s="108"/>
-      <c r="AE37" s="108"/>
-      <c r="AF37" s="108"/>
-      <c r="AG37" s="109"/>
-    </row>
-    <row r="38" spans="2:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="145" t="s">
+      <c r="C37" s="66"/>
+      <c r="D37" s="66"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
+      <c r="G37" s="66"/>
+      <c r="H37" s="66"/>
+      <c r="I37" s="66"/>
+      <c r="J37" s="102"/>
+      <c r="K37" s="102"/>
+      <c r="L37" s="103"/>
+      <c r="M37" s="103"/>
+      <c r="N37" s="103"/>
+      <c r="O37" s="104"/>
+      <c r="P37" s="104"/>
+      <c r="Q37" s="104"/>
+      <c r="R37" s="104"/>
+      <c r="S37" s="104"/>
+      <c r="T37" s="104"/>
+      <c r="U37" s="104"/>
+      <c r="V37" s="104"/>
+      <c r="W37" s="104"/>
+      <c r="X37" s="104"/>
+      <c r="Y37" s="104"/>
+      <c r="Z37" s="104"/>
+      <c r="AA37" s="104"/>
+      <c r="AB37" s="104"/>
+      <c r="AC37" s="104"/>
+      <c r="AD37" s="104"/>
+      <c r="AE37" s="104"/>
+      <c r="AF37" s="104"/>
+      <c r="AG37" s="105"/>
+    </row>
+    <row r="38" spans="2:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="141" t="s">
         <v>80</v>
       </c>
-      <c r="C38" s="110"/>
-      <c r="D38" s="110"/>
-      <c r="E38" s="110"/>
-      <c r="F38" s="110"/>
-      <c r="G38" s="110"/>
-      <c r="H38" s="110"/>
-      <c r="I38" s="110"/>
-      <c r="J38" s="110"/>
-      <c r="K38" s="110"/>
-      <c r="L38" s="110"/>
-      <c r="M38" s="110"/>
-      <c r="N38" s="110"/>
-      <c r="O38" s="111"/>
-      <c r="P38" s="111"/>
-      <c r="Q38" s="111"/>
-      <c r="R38" s="111"/>
-      <c r="S38" s="111"/>
-      <c r="T38" s="111"/>
-      <c r="U38" s="111"/>
-      <c r="V38" s="111"/>
-      <c r="W38" s="111"/>
-      <c r="X38" s="111"/>
-      <c r="Y38" s="111"/>
-      <c r="Z38" s="111"/>
-      <c r="AA38" s="111"/>
-      <c r="AB38" s="111"/>
-      <c r="AC38" s="111"/>
-      <c r="AD38" s="111"/>
-      <c r="AE38" s="111"/>
-      <c r="AF38" s="111"/>
-      <c r="AG38" s="110"/>
-    </row>
-    <row r="39" spans="2:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="110"/>
-      <c r="C39" s="110"/>
-      <c r="D39" s="110"/>
-      <c r="E39" s="110"/>
-      <c r="F39" s="110"/>
-      <c r="G39" s="110"/>
-      <c r="H39" s="110"/>
-      <c r="I39" s="110"/>
-      <c r="J39" s="110"/>
-      <c r="K39" s="110"/>
-      <c r="L39" s="110"/>
-      <c r="M39" s="110"/>
-      <c r="N39" s="110"/>
-      <c r="O39" s="111"/>
-      <c r="P39" s="111"/>
-      <c r="Q39" s="111"/>
-      <c r="R39" s="111"/>
-      <c r="S39" s="111"/>
-      <c r="T39" s="111"/>
-      <c r="U39" s="111"/>
-      <c r="V39" s="111"/>
-      <c r="W39" s="111"/>
-      <c r="X39" s="111"/>
-      <c r="Y39" s="111"/>
-      <c r="Z39" s="111"/>
-      <c r="AA39" s="111"/>
-      <c r="AB39" s="111"/>
-      <c r="AC39" s="111"/>
-      <c r="AD39" s="111"/>
-      <c r="AE39" s="111"/>
-      <c r="AF39" s="111"/>
-      <c r="AG39" s="110"/>
-    </row>
-    <row r="40" spans="2:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="110"/>
-      <c r="C40" s="110"/>
-      <c r="D40" s="110"/>
-      <c r="E40" s="110"/>
-      <c r="F40" s="110"/>
-      <c r="G40" s="110"/>
-      <c r="H40" s="110"/>
-      <c r="I40" s="110"/>
-      <c r="J40" s="110"/>
-      <c r="K40" s="110"/>
-      <c r="L40" s="110"/>
-      <c r="M40" s="110"/>
-      <c r="N40" s="110"/>
-      <c r="O40" s="111"/>
-      <c r="P40" s="111"/>
-      <c r="Q40" s="111"/>
-      <c r="R40" s="111"/>
-      <c r="S40" s="111"/>
-      <c r="T40" s="111"/>
-      <c r="U40" s="111"/>
-      <c r="V40" s="111"/>
-      <c r="W40" s="111"/>
-      <c r="X40" s="111"/>
-      <c r="Y40" s="111"/>
-      <c r="Z40" s="111"/>
-      <c r="AA40" s="111"/>
-      <c r="AB40" s="111"/>
-      <c r="AC40" s="111"/>
-      <c r="AD40" s="111"/>
-      <c r="AE40" s="111"/>
-      <c r="AF40" s="111"/>
-      <c r="AG40" s="110"/>
-    </row>
-    <row r="41" spans="2:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="110"/>
-      <c r="C41" s="71"/>
-      <c r="D41" s="71"/>
-      <c r="E41" s="71"/>
-      <c r="F41" s="110"/>
-      <c r="G41" s="110"/>
-      <c r="H41" s="110"/>
-      <c r="I41" s="110"/>
-      <c r="J41" s="110"/>
-      <c r="K41" s="110"/>
-      <c r="L41" s="110"/>
-      <c r="M41" s="110"/>
-      <c r="N41" s="110"/>
-      <c r="O41" s="111"/>
-      <c r="P41" s="111"/>
-      <c r="Q41" s="111"/>
-      <c r="R41" s="111"/>
-      <c r="S41" s="111"/>
-      <c r="T41" s="111"/>
-      <c r="U41" s="111"/>
-      <c r="V41" s="111"/>
-      <c r="W41" s="111"/>
-      <c r="X41" s="111"/>
-      <c r="Y41" s="111"/>
-      <c r="Z41" s="111"/>
-      <c r="AA41" s="111"/>
-      <c r="AB41" s="111"/>
-      <c r="AC41" s="111"/>
-      <c r="AD41" s="111"/>
-      <c r="AE41" s="111"/>
-      <c r="AF41" s="111"/>
-      <c r="AG41" s="110"/>
-    </row>
-    <row r="42" spans="2:33" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="71"/>
-      <c r="C42" s="71"/>
-      <c r="D42" s="71"/>
-      <c r="E42" s="71"/>
-      <c r="F42" s="156" t="s">
+      <c r="C38" s="106"/>
+      <c r="D38" s="106"/>
+      <c r="E38" s="106"/>
+      <c r="F38" s="106"/>
+      <c r="G38" s="106"/>
+      <c r="H38" s="106"/>
+      <c r="I38" s="106"/>
+      <c r="J38" s="106"/>
+      <c r="K38" s="106"/>
+      <c r="L38" s="106"/>
+      <c r="M38" s="106"/>
+      <c r="N38" s="106"/>
+      <c r="O38" s="107"/>
+      <c r="P38" s="107"/>
+      <c r="Q38" s="107"/>
+      <c r="R38" s="107"/>
+      <c r="S38" s="107"/>
+      <c r="T38" s="107"/>
+      <c r="U38" s="107"/>
+      <c r="V38" s="107"/>
+      <c r="W38" s="107"/>
+      <c r="X38" s="107"/>
+      <c r="Y38" s="107"/>
+      <c r="Z38" s="107"/>
+      <c r="AA38" s="107"/>
+      <c r="AB38" s="107"/>
+      <c r="AC38" s="107"/>
+      <c r="AD38" s="107"/>
+      <c r="AE38" s="107"/>
+      <c r="AF38" s="107"/>
+      <c r="AG38" s="106"/>
+    </row>
+    <row r="39" spans="2:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="106"/>
+      <c r="C39" s="106"/>
+      <c r="D39" s="106"/>
+      <c r="E39" s="106"/>
+      <c r="F39" s="106"/>
+      <c r="G39" s="106"/>
+      <c r="H39" s="106"/>
+      <c r="I39" s="106"/>
+      <c r="J39" s="106"/>
+      <c r="K39" s="106"/>
+      <c r="L39" s="106"/>
+      <c r="M39" s="106"/>
+      <c r="N39" s="106"/>
+      <c r="O39" s="107"/>
+      <c r="P39" s="107"/>
+      <c r="Q39" s="107"/>
+      <c r="R39" s="107"/>
+      <c r="S39" s="107"/>
+      <c r="T39" s="107"/>
+      <c r="U39" s="107"/>
+      <c r="V39" s="107"/>
+      <c r="W39" s="107"/>
+      <c r="X39" s="107"/>
+      <c r="Y39" s="107"/>
+      <c r="Z39" s="107"/>
+      <c r="AA39" s="107"/>
+      <c r="AB39" s="107"/>
+      <c r="AC39" s="107"/>
+      <c r="AD39" s="107"/>
+      <c r="AE39" s="107"/>
+      <c r="AF39" s="107"/>
+      <c r="AG39" s="106"/>
+    </row>
+    <row r="40" spans="2:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="106"/>
+      <c r="C40" s="106"/>
+      <c r="D40" s="106"/>
+      <c r="E40" s="106"/>
+      <c r="F40" s="106"/>
+      <c r="G40" s="106"/>
+      <c r="H40" s="106"/>
+      <c r="I40" s="106"/>
+      <c r="J40" s="106"/>
+      <c r="K40" s="106"/>
+      <c r="L40" s="106"/>
+      <c r="M40" s="106"/>
+      <c r="N40" s="106"/>
+      <c r="O40" s="107"/>
+      <c r="P40" s="107"/>
+      <c r="Q40" s="107"/>
+      <c r="R40" s="107"/>
+      <c r="S40" s="107"/>
+      <c r="T40" s="107"/>
+      <c r="U40" s="107"/>
+      <c r="V40" s="107"/>
+      <c r="W40" s="107"/>
+      <c r="X40" s="107"/>
+      <c r="Y40" s="107"/>
+      <c r="Z40" s="107"/>
+      <c r="AA40" s="107"/>
+      <c r="AB40" s="107"/>
+      <c r="AC40" s="107"/>
+      <c r="AD40" s="107"/>
+      <c r="AE40" s="107"/>
+      <c r="AF40" s="107"/>
+      <c r="AG40" s="106"/>
+    </row>
+    <row r="41" spans="2:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="106"/>
+      <c r="C41" s="67"/>
+      <c r="D41" s="67"/>
+      <c r="E41" s="67"/>
+      <c r="F41" s="106"/>
+      <c r="G41" s="106"/>
+      <c r="H41" s="106"/>
+      <c r="I41" s="106"/>
+      <c r="J41" s="106"/>
+      <c r="K41" s="106"/>
+      <c r="L41" s="106"/>
+      <c r="M41" s="106"/>
+      <c r="N41" s="106"/>
+      <c r="O41" s="107"/>
+      <c r="P41" s="107"/>
+      <c r="Q41" s="107"/>
+      <c r="R41" s="107"/>
+      <c r="S41" s="107"/>
+      <c r="T41" s="107"/>
+      <c r="U41" s="107"/>
+      <c r="V41" s="107"/>
+      <c r="W41" s="107"/>
+      <c r="X41" s="107"/>
+      <c r="Y41" s="107"/>
+      <c r="Z41" s="107"/>
+      <c r="AA41" s="107"/>
+      <c r="AB41" s="107"/>
+      <c r="AC41" s="107"/>
+      <c r="AD41" s="107"/>
+      <c r="AE41" s="107"/>
+      <c r="AF41" s="107"/>
+      <c r="AG41" s="106"/>
+    </row>
+    <row r="42" spans="2:33" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B42" s="67"/>
+      <c r="C42" s="67"/>
+      <c r="D42" s="67"/>
+      <c r="E42" s="67"/>
+      <c r="F42" s="157" t="s">
         <v>48</v>
       </c>
-      <c r="G42" s="156"/>
-      <c r="H42" s="72"/>
-      <c r="I42" s="73"/>
-      <c r="J42" s="110"/>
-      <c r="K42" s="142"/>
-      <c r="L42" s="142"/>
-      <c r="M42" s="142"/>
-      <c r="N42" s="142"/>
-      <c r="O42" s="72" t="s">
+      <c r="G42" s="157"/>
+      <c r="H42" s="68"/>
+      <c r="I42" s="69"/>
+      <c r="J42" s="106"/>
+      <c r="K42" s="138"/>
+      <c r="L42" s="138"/>
+      <c r="M42" s="138"/>
+      <c r="N42" s="138"/>
+      <c r="O42" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="P42" s="81"/>
-      <c r="Q42" s="81"/>
-      <c r="R42" s="81"/>
-      <c r="S42" s="81"/>
-      <c r="T42" s="81"/>
-      <c r="U42" s="81"/>
-      <c r="V42" s="81"/>
-      <c r="W42" s="81"/>
-      <c r="X42" s="142"/>
-      <c r="Y42" s="142"/>
-      <c r="Z42" s="142"/>
-      <c r="AA42" s="142"/>
-      <c r="AB42" s="142"/>
-      <c r="AC42" s="142"/>
-      <c r="AD42" s="142"/>
-      <c r="AE42" s="142"/>
-      <c r="AF42" s="142"/>
-      <c r="AG42" s="142"/>
-    </row>
-    <row r="43" spans="2:33" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="71"/>
-      <c r="C43" s="71"/>
-      <c r="D43" s="71"/>
-      <c r="E43" s="71"/>
-      <c r="F43" s="79"/>
-      <c r="G43" s="73"/>
-      <c r="H43" s="73"/>
-      <c r="I43" s="73"/>
-      <c r="J43" s="110"/>
-      <c r="K43" s="80"/>
-      <c r="L43" s="80"/>
-      <c r="M43" s="80"/>
-      <c r="N43" s="80"/>
-      <c r="O43" s="80"/>
-      <c r="P43" s="80"/>
-      <c r="Q43" s="80"/>
-      <c r="R43" s="80"/>
-      <c r="S43" s="80"/>
-      <c r="T43" s="80"/>
-      <c r="U43" s="80"/>
-      <c r="V43" s="157" t="s">
+      <c r="P42" s="77"/>
+      <c r="Q42" s="77"/>
+      <c r="R42" s="77"/>
+      <c r="S42" s="77"/>
+      <c r="T42" s="77"/>
+      <c r="U42" s="77"/>
+      <c r="V42" s="77"/>
+      <c r="W42" s="77"/>
+      <c r="X42" s="138"/>
+      <c r="Y42" s="138"/>
+      <c r="Z42" s="138"/>
+      <c r="AA42" s="138"/>
+      <c r="AB42" s="138"/>
+      <c r="AC42" s="138"/>
+      <c r="AD42" s="138"/>
+      <c r="AE42" s="138"/>
+      <c r="AF42" s="138"/>
+      <c r="AG42" s="138"/>
+    </row>
+    <row r="43" spans="2:33" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="67"/>
+      <c r="C43" s="67"/>
+      <c r="D43" s="67"/>
+      <c r="E43" s="67"/>
+      <c r="F43" s="75"/>
+      <c r="G43" s="69"/>
+      <c r="H43" s="69"/>
+      <c r="I43" s="69"/>
+      <c r="J43" s="106"/>
+      <c r="K43" s="76"/>
+      <c r="L43" s="76"/>
+      <c r="M43" s="76"/>
+      <c r="N43" s="76"/>
+      <c r="O43" s="76"/>
+      <c r="P43" s="76"/>
+      <c r="Q43" s="76"/>
+      <c r="R43" s="76"/>
+      <c r="S43" s="76"/>
+      <c r="T43" s="76"/>
+      <c r="U43" s="76"/>
+      <c r="V43" s="158" t="s">
         <v>49</v>
       </c>
-      <c r="W43" s="157"/>
-      <c r="X43" s="157"/>
-      <c r="Y43" s="157"/>
-      <c r="Z43" s="144" t="s">
+      <c r="W43" s="158"/>
+      <c r="X43" s="158"/>
+      <c r="Y43" s="158"/>
+      <c r="Z43" s="140" t="s">
         <v>71</v>
       </c>
-      <c r="AA43" s="143"/>
-      <c r="AB43" s="80"/>
-      <c r="AC43" s="80"/>
-      <c r="AD43" s="80"/>
-    </row>
-    <row r="44" spans="2:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA43" s="139"/>
+      <c r="AB43" s="76"/>
+      <c r="AC43" s="76"/>
+      <c r="AD43" s="76"/>
+    </row>
+    <row r="44" spans="2:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="5" t="s">
         <v>50</v>
       </c>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
-      <c r="E44" s="110"/>
-      <c r="F44" s="110"/>
-      <c r="G44" s="110"/>
-      <c r="H44" s="110"/>
-      <c r="I44" s="110"/>
-      <c r="J44" s="110"/>
-      <c r="K44" s="110"/>
-      <c r="L44" s="110"/>
-      <c r="M44" s="110"/>
-      <c r="N44" s="110"/>
-      <c r="O44" s="111"/>
-      <c r="P44" s="111"/>
-      <c r="Q44" s="111"/>
-      <c r="R44" s="111"/>
-      <c r="S44" s="111"/>
-      <c r="T44" s="111"/>
-      <c r="U44" s="111"/>
-      <c r="V44" s="111"/>
-      <c r="W44" s="111"/>
-      <c r="X44" s="111"/>
-      <c r="Y44" s="111"/>
-      <c r="Z44" s="111"/>
-      <c r="AA44" s="111"/>
-      <c r="AB44" s="111"/>
-      <c r="AC44" s="111"/>
-      <c r="AD44" s="111"/>
-      <c r="AE44" s="111"/>
-      <c r="AF44" s="111"/>
-      <c r="AG44" s="110"/>
-    </row>
-    <row r="45" spans="2:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="146" t="s">
+      <c r="E44" s="106"/>
+      <c r="F44" s="106"/>
+      <c r="G44" s="106"/>
+      <c r="H44" s="106"/>
+      <c r="I44" s="106"/>
+      <c r="J44" s="106"/>
+      <c r="K44" s="106"/>
+      <c r="L44" s="106"/>
+      <c r="M44" s="106"/>
+      <c r="N44" s="106"/>
+      <c r="O44" s="107"/>
+      <c r="P44" s="107"/>
+      <c r="Q44" s="107"/>
+      <c r="R44" s="107"/>
+      <c r="S44" s="107"/>
+      <c r="T44" s="107"/>
+      <c r="U44" s="107"/>
+      <c r="V44" s="107"/>
+      <c r="W44" s="107"/>
+      <c r="X44" s="107"/>
+      <c r="Y44" s="107"/>
+      <c r="Z44" s="107"/>
+      <c r="AA44" s="107"/>
+      <c r="AB44" s="107"/>
+      <c r="AC44" s="107"/>
+      <c r="AD44" s="107"/>
+      <c r="AE44" s="107"/>
+      <c r="AF44" s="107"/>
+      <c r="AG44" s="106"/>
+    </row>
+    <row r="45" spans="2:33" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="147" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="146"/>
+      <c r="C45" s="147"/>
       <c r="D45" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="112"/>
-      <c r="F45" s="112"/>
-      <c r="G45" s="112"/>
-      <c r="H45" s="112"/>
-      <c r="I45" s="112"/>
-      <c r="J45" s="112"/>
-      <c r="K45" s="112"/>
-      <c r="L45" s="112"/>
-      <c r="M45" s="112"/>
-      <c r="N45" s="112"/>
-      <c r="O45" s="112"/>
-      <c r="P45" s="112"/>
-      <c r="Q45" s="112"/>
-      <c r="R45" s="112"/>
-      <c r="S45" s="112"/>
-      <c r="T45" s="112"/>
-      <c r="U45" s="112"/>
-      <c r="V45" s="112"/>
-      <c r="W45" s="112"/>
-      <c r="X45" s="112"/>
-      <c r="Y45" s="112"/>
-      <c r="Z45" s="112"/>
-      <c r="AA45" s="112"/>
-      <c r="AB45" s="112"/>
-      <c r="AC45" s="112"/>
-      <c r="AD45" s="112"/>
-      <c r="AE45" s="112"/>
-      <c r="AF45" s="112"/>
-      <c r="AG45" s="112"/>
-    </row>
-    <row r="46" spans="2:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E45" s="108"/>
+      <c r="F45" s="108"/>
+      <c r="G45" s="108"/>
+      <c r="H45" s="108"/>
+      <c r="I45" s="108"/>
+      <c r="J45" s="108"/>
+      <c r="K45" s="108"/>
+      <c r="L45" s="108"/>
+      <c r="M45" s="108"/>
+      <c r="N45" s="108"/>
+      <c r="O45" s="108"/>
+      <c r="P45" s="108"/>
+      <c r="Q45" s="108"/>
+      <c r="R45" s="108"/>
+      <c r="S45" s="108"/>
+      <c r="T45" s="108"/>
+      <c r="U45" s="108"/>
+      <c r="V45" s="108"/>
+      <c r="W45" s="108"/>
+      <c r="X45" s="108"/>
+      <c r="Y45" s="108"/>
+      <c r="Z45" s="108"/>
+      <c r="AA45" s="108"/>
+      <c r="AB45" s="108"/>
+      <c r="AC45" s="108"/>
+      <c r="AD45" s="108"/>
+      <c r="AE45" s="108"/>
+      <c r="AF45" s="108"/>
+      <c r="AG45" s="108"/>
+    </row>
+    <row r="46" spans="2:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E46" s="110"/>
-      <c r="F46" s="110"/>
-      <c r="G46" s="110"/>
-      <c r="H46" s="110"/>
-      <c r="I46" s="110"/>
-      <c r="J46" s="110"/>
-      <c r="K46" s="110"/>
-      <c r="L46" s="110"/>
-      <c r="M46" s="110"/>
-      <c r="N46" s="110"/>
-      <c r="O46" s="111"/>
-      <c r="P46" s="111"/>
-      <c r="Q46" s="111"/>
-      <c r="R46" s="111"/>
-      <c r="S46" s="111"/>
-      <c r="T46" s="111"/>
-      <c r="U46" s="111"/>
-      <c r="V46" s="111"/>
-      <c r="W46" s="111"/>
-      <c r="X46" s="111"/>
-      <c r="Y46" s="111"/>
-      <c r="Z46" s="111"/>
-      <c r="AA46" s="111"/>
-      <c r="AB46" s="111"/>
-      <c r="AC46" s="111"/>
-      <c r="AD46" s="111"/>
-      <c r="AE46" s="111"/>
-      <c r="AF46" s="111"/>
-      <c r="AG46" s="110"/>
-    </row>
-    <row r="47" spans="2:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E46" s="106"/>
+      <c r="F46" s="106"/>
+      <c r="G46" s="106"/>
+      <c r="H46" s="106"/>
+      <c r="I46" s="106"/>
+      <c r="J46" s="106"/>
+      <c r="K46" s="106"/>
+      <c r="L46" s="106"/>
+      <c r="M46" s="106"/>
+      <c r="N46" s="106"/>
+      <c r="O46" s="107"/>
+      <c r="P46" s="107"/>
+      <c r="Q46" s="107"/>
+      <c r="R46" s="107"/>
+      <c r="S46" s="107"/>
+      <c r="T46" s="107"/>
+      <c r="U46" s="107"/>
+      <c r="V46" s="107"/>
+      <c r="W46" s="107"/>
+      <c r="X46" s="107"/>
+      <c r="Y46" s="107"/>
+      <c r="Z46" s="107"/>
+      <c r="AA46" s="107"/>
+      <c r="AB46" s="107"/>
+      <c r="AC46" s="107"/>
+      <c r="AD46" s="107"/>
+      <c r="AE46" s="107"/>
+      <c r="AF46" s="107"/>
+      <c r="AG46" s="106"/>
+    </row>
+    <row r="47" spans="2:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
       <c r="D47" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E47" s="110"/>
-      <c r="F47" s="110"/>
-      <c r="G47" s="110"/>
-      <c r="H47" s="110"/>
-      <c r="I47" s="110"/>
-      <c r="J47" s="110"/>
-      <c r="K47" s="110"/>
-      <c r="L47" s="110"/>
-      <c r="M47" s="110"/>
-      <c r="N47" s="110"/>
-      <c r="O47" s="111"/>
-      <c r="P47" s="111"/>
-      <c r="Q47" s="111"/>
-      <c r="R47" s="111"/>
-      <c r="S47" s="111"/>
-      <c r="T47" s="111"/>
-      <c r="U47" s="111"/>
-      <c r="V47" s="111"/>
-      <c r="W47" s="111"/>
-      <c r="X47" s="111"/>
-      <c r="Y47" s="111"/>
-      <c r="Z47" s="111"/>
-      <c r="AA47" s="111"/>
-      <c r="AB47" s="111"/>
-      <c r="AC47" s="111"/>
-      <c r="AD47" s="111"/>
-      <c r="AE47" s="111"/>
-      <c r="AF47" s="111"/>
-      <c r="AG47" s="110"/>
-    </row>
-    <row r="48" spans="2:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="110"/>
-      <c r="C48" s="110"/>
-      <c r="D48" s="110"/>
-      <c r="E48" s="110"/>
-      <c r="F48" s="110"/>
-      <c r="G48" s="110"/>
-      <c r="H48" s="110"/>
-      <c r="I48" s="110"/>
-      <c r="J48" s="110"/>
-      <c r="K48" s="110"/>
-      <c r="L48" s="110"/>
-      <c r="M48" s="110"/>
-      <c r="N48" s="110"/>
-      <c r="O48" s="111"/>
-      <c r="P48" s="111"/>
-      <c r="Q48" s="111"/>
-      <c r="R48" s="111"/>
-      <c r="S48" s="111"/>
-      <c r="T48" s="111"/>
-      <c r="U48" s="111"/>
-      <c r="V48" s="111"/>
-      <c r="W48" s="111"/>
-      <c r="X48" s="111"/>
-      <c r="Y48" s="111"/>
-      <c r="Z48" s="111"/>
-      <c r="AA48" s="111"/>
-      <c r="AB48" s="111"/>
-      <c r="AC48" s="111"/>
-      <c r="AD48" s="111"/>
-      <c r="AE48" s="111"/>
-      <c r="AF48" s="111"/>
-      <c r="AG48" s="110"/>
+      <c r="E47" s="106"/>
+      <c r="F47" s="106"/>
+      <c r="G47" s="106"/>
+      <c r="H47" s="106"/>
+      <c r="I47" s="106"/>
+      <c r="J47" s="106"/>
+      <c r="K47" s="106"/>
+      <c r="L47" s="106"/>
+      <c r="M47" s="106"/>
+      <c r="N47" s="106"/>
+      <c r="O47" s="107"/>
+      <c r="P47" s="107"/>
+      <c r="Q47" s="107"/>
+      <c r="R47" s="107"/>
+      <c r="S47" s="107"/>
+      <c r="T47" s="107"/>
+      <c r="U47" s="107"/>
+      <c r="V47" s="107"/>
+      <c r="W47" s="107"/>
+      <c r="X47" s="107"/>
+      <c r="Y47" s="107"/>
+      <c r="Z47" s="107"/>
+      <c r="AA47" s="107"/>
+      <c r="AB47" s="107"/>
+      <c r="AC47" s="107"/>
+      <c r="AD47" s="107"/>
+      <c r="AE47" s="107"/>
+      <c r="AF47" s="107"/>
+      <c r="AG47" s="106"/>
+    </row>
+    <row r="48" spans="2:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B48" s="106"/>
+      <c r="C48" s="106"/>
+      <c r="D48" s="106"/>
+      <c r="E48" s="106"/>
+      <c r="F48" s="106"/>
+      <c r="G48" s="106"/>
+      <c r="H48" s="106"/>
+      <c r="I48" s="106"/>
+      <c r="J48" s="106"/>
+      <c r="K48" s="106"/>
+      <c r="L48" s="106"/>
+      <c r="M48" s="106"/>
+      <c r="N48" s="106"/>
+      <c r="O48" s="107"/>
+      <c r="P48" s="107"/>
+      <c r="Q48" s="107"/>
+      <c r="R48" s="107"/>
+      <c r="S48" s="107"/>
+      <c r="T48" s="107"/>
+      <c r="U48" s="107"/>
+      <c r="V48" s="107"/>
+      <c r="W48" s="107"/>
+      <c r="X48" s="107"/>
+      <c r="Y48" s="107"/>
+      <c r="Z48" s="107"/>
+      <c r="AA48" s="107"/>
+      <c r="AB48" s="107"/>
+      <c r="AC48" s="107"/>
+      <c r="AD48" s="107"/>
+      <c r="AE48" s="107"/>
+      <c r="AF48" s="107"/>
+      <c r="AG48" s="106"/>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="B10:AG10"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="B3:AG3"/>
-    <mergeCell ref="B4:AG4"/>
-    <mergeCell ref="B5:AG5"/>
-    <mergeCell ref="B6:AG6"/>
-    <mergeCell ref="B7:AG7"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="AE16:AF16"/>
     <mergeCell ref="J16:K16"/>
@@ -4286,6 +4279,13 @@
     <mergeCell ref="J14:L14"/>
     <mergeCell ref="F42:G42"/>
     <mergeCell ref="V43:Y43"/>
+    <mergeCell ref="B10:AG10"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="B3:AG3"/>
+    <mergeCell ref="B4:AG4"/>
+    <mergeCell ref="B5:AG5"/>
+    <mergeCell ref="B6:AG6"/>
+    <mergeCell ref="B7:AG7"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="1.299212598425197" right="0.70866141732283472" top="0.35433070866141736" bottom="0.35433070866141736" header="0.51181102362204722" footer="0.31496062992125984"/>
@@ -4323,12 +4323,12 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="17.75" customWidth="1"/>
+    <col min="3" max="3" width="17.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>56</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>58</v>
       </c>
@@ -4344,7 +4344,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>60</v>
       </c>
@@ -4352,7 +4352,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>62</v>
       </c>
@@ -4360,7 +4360,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>64</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>66</v>
       </c>

</xml_diff>

<commit_message>
style(excel): se ajustan estilos de las celdas en las plantillas
</commit_message>
<xml_diff>
--- a/GRUPAL-F165.xlsx
+++ b/GRUPAL-F165.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johan\OneDrive\Desktop\sena app\BACKEND_SENA_APP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85276C27-3354-4F7A-9EEB-216113F263BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A89A932-3535-4B67-8277-EC9B45A5BF75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1410,9 +1410,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1696,6 +1693,54 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="25" fillId="2" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="2" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="25" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="34" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1711,52 +1756,7 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="59" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="52" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="43" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="2" borderId="36" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="2" borderId="43" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2409,7 +2409,7 @@
   <dimension ref="A1:AG48"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2431,500 +2431,500 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="50"/>
-      <c r="B1" s="50"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="51"/>
-      <c r="J1" s="51"/>
-      <c r="K1" s="51"/>
-      <c r="L1" s="51"/>
-      <c r="M1" s="51"/>
-      <c r="N1" s="51"/>
-      <c r="O1" s="51"/>
-      <c r="P1" s="51"/>
-      <c r="Q1" s="51"/>
-      <c r="R1" s="51"/>
-      <c r="S1" s="51"/>
-      <c r="T1" s="51"/>
-      <c r="U1" s="51"/>
-      <c r="V1" s="51"/>
-      <c r="W1" s="51"/>
-      <c r="X1" s="51"/>
-      <c r="Y1" s="51"/>
-      <c r="Z1" s="51"/>
-      <c r="AA1" s="51"/>
-      <c r="AB1" s="51"/>
-      <c r="AC1" s="51"/>
-      <c r="AD1" s="51"/>
-      <c r="AE1" s="52"/>
-      <c r="AF1" s="52"/>
-      <c r="AG1" s="78" t="s">
+      <c r="A1" s="49"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="50"/>
+      <c r="G1" s="50"/>
+      <c r="H1" s="50"/>
+      <c r="I1" s="50"/>
+      <c r="J1" s="50"/>
+      <c r="K1" s="50"/>
+      <c r="L1" s="50"/>
+      <c r="M1" s="50"/>
+      <c r="N1" s="50"/>
+      <c r="O1" s="50"/>
+      <c r="P1" s="50"/>
+      <c r="Q1" s="50"/>
+      <c r="R1" s="50"/>
+      <c r="S1" s="50"/>
+      <c r="T1" s="50"/>
+      <c r="U1" s="50"/>
+      <c r="V1" s="50"/>
+      <c r="W1" s="50"/>
+      <c r="X1" s="50"/>
+      <c r="Y1" s="50"/>
+      <c r="Z1" s="50"/>
+      <c r="AA1" s="50"/>
+      <c r="AB1" s="50"/>
+      <c r="AC1" s="50"/>
+      <c r="AD1" s="50"/>
+      <c r="AE1" s="51"/>
+      <c r="AF1" s="51"/>
+      <c r="AG1" s="77" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:33" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="55"/>
-      <c r="P2" s="55"/>
-      <c r="Q2" s="55"/>
-      <c r="R2" s="55"/>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="55"/>
-      <c r="W2" s="55"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="55"/>
-      <c r="Z2" s="55"/>
-      <c r="AA2" s="55"/>
-      <c r="AB2" s="55"/>
-      <c r="AC2" s="55"/>
-      <c r="AD2" s="55"/>
-      <c r="AE2" s="57"/>
-      <c r="AF2" s="57"/>
-      <c r="AG2" s="78" t="s">
+      <c r="A2" s="52"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
+      <c r="V2" s="54"/>
+      <c r="W2" s="54"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="54"/>
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="54"/>
+      <c r="AD2" s="54"/>
+      <c r="AE2" s="56"/>
+      <c r="AF2" s="56"/>
+      <c r="AG2" s="77" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:33" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="79"/>
-      <c r="B3" s="144" t="s">
+      <c r="A3" s="78"/>
+      <c r="B3" s="159" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="144"/>
-      <c r="D3" s="144"/>
-      <c r="E3" s="144"/>
-      <c r="F3" s="144"/>
-      <c r="G3" s="144"/>
-      <c r="H3" s="144"/>
-      <c r="I3" s="144"/>
-      <c r="J3" s="144"/>
-      <c r="K3" s="144"/>
-      <c r="L3" s="144"/>
-      <c r="M3" s="144"/>
-      <c r="N3" s="144"/>
-      <c r="O3" s="144"/>
-      <c r="P3" s="144"/>
-      <c r="Q3" s="144"/>
-      <c r="R3" s="144"/>
-      <c r="S3" s="144"/>
-      <c r="T3" s="144"/>
-      <c r="U3" s="144"/>
-      <c r="V3" s="144"/>
-      <c r="W3" s="144"/>
-      <c r="X3" s="144"/>
-      <c r="Y3" s="144"/>
-      <c r="Z3" s="144"/>
-      <c r="AA3" s="144"/>
-      <c r="AB3" s="144"/>
-      <c r="AC3" s="144"/>
-      <c r="AD3" s="144"/>
-      <c r="AE3" s="144"/>
-      <c r="AF3" s="144"/>
-      <c r="AG3" s="145"/>
+      <c r="C3" s="159"/>
+      <c r="D3" s="159"/>
+      <c r="E3" s="159"/>
+      <c r="F3" s="159"/>
+      <c r="G3" s="159"/>
+      <c r="H3" s="159"/>
+      <c r="I3" s="159"/>
+      <c r="J3" s="159"/>
+      <c r="K3" s="159"/>
+      <c r="L3" s="159"/>
+      <c r="M3" s="159"/>
+      <c r="N3" s="159"/>
+      <c r="O3" s="159"/>
+      <c r="P3" s="159"/>
+      <c r="Q3" s="159"/>
+      <c r="R3" s="159"/>
+      <c r="S3" s="159"/>
+      <c r="T3" s="159"/>
+      <c r="U3" s="159"/>
+      <c r="V3" s="159"/>
+      <c r="W3" s="159"/>
+      <c r="X3" s="159"/>
+      <c r="Y3" s="159"/>
+      <c r="Z3" s="159"/>
+      <c r="AA3" s="159"/>
+      <c r="AB3" s="159"/>
+      <c r="AC3" s="159"/>
+      <c r="AD3" s="159"/>
+      <c r="AE3" s="159"/>
+      <c r="AF3" s="159"/>
+      <c r="AG3" s="160"/>
     </row>
     <row r="4" spans="1:33" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="79"/>
-      <c r="B4" s="146" t="s">
+      <c r="A4" s="78"/>
+      <c r="B4" s="161" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="146"/>
-      <c r="D4" s="146"/>
-      <c r="E4" s="146"/>
-      <c r="F4" s="146"/>
-      <c r="G4" s="146"/>
-      <c r="H4" s="146"/>
-      <c r="I4" s="146"/>
-      <c r="J4" s="146"/>
-      <c r="K4" s="146"/>
-      <c r="L4" s="146"/>
-      <c r="M4" s="146"/>
-      <c r="N4" s="146"/>
-      <c r="O4" s="146"/>
-      <c r="P4" s="146"/>
-      <c r="Q4" s="146"/>
-      <c r="R4" s="146"/>
-      <c r="S4" s="146"/>
-      <c r="T4" s="146"/>
-      <c r="U4" s="146"/>
-      <c r="V4" s="146"/>
-      <c r="W4" s="146"/>
-      <c r="X4" s="146"/>
-      <c r="Y4" s="146"/>
-      <c r="Z4" s="146"/>
-      <c r="AA4" s="146"/>
-      <c r="AB4" s="146"/>
-      <c r="AC4" s="146"/>
-      <c r="AD4" s="146"/>
-      <c r="AE4" s="146"/>
-      <c r="AF4" s="146"/>
-      <c r="AG4" s="146"/>
+      <c r="C4" s="161"/>
+      <c r="D4" s="161"/>
+      <c r="E4" s="161"/>
+      <c r="F4" s="161"/>
+      <c r="G4" s="161"/>
+      <c r="H4" s="161"/>
+      <c r="I4" s="161"/>
+      <c r="J4" s="161"/>
+      <c r="K4" s="161"/>
+      <c r="L4" s="161"/>
+      <c r="M4" s="161"/>
+      <c r="N4" s="161"/>
+      <c r="O4" s="161"/>
+      <c r="P4" s="161"/>
+      <c r="Q4" s="161"/>
+      <c r="R4" s="161"/>
+      <c r="S4" s="161"/>
+      <c r="T4" s="161"/>
+      <c r="U4" s="161"/>
+      <c r="V4" s="161"/>
+      <c r="W4" s="161"/>
+      <c r="X4" s="161"/>
+      <c r="Y4" s="161"/>
+      <c r="Z4" s="161"/>
+      <c r="AA4" s="161"/>
+      <c r="AB4" s="161"/>
+      <c r="AC4" s="161"/>
+      <c r="AD4" s="161"/>
+      <c r="AE4" s="161"/>
+      <c r="AF4" s="161"/>
+      <c r="AG4" s="161"/>
     </row>
     <row r="5" spans="1:33" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="79"/>
-      <c r="B5" s="144" t="s">
+      <c r="A5" s="78"/>
+      <c r="B5" s="159" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="144"/>
-      <c r="D5" s="144"/>
-      <c r="E5" s="144"/>
-      <c r="F5" s="144"/>
-      <c r="G5" s="144"/>
-      <c r="H5" s="144"/>
-      <c r="I5" s="144"/>
-      <c r="J5" s="144"/>
-      <c r="K5" s="144"/>
-      <c r="L5" s="144"/>
-      <c r="M5" s="144"/>
-      <c r="N5" s="144"/>
-      <c r="O5" s="144"/>
-      <c r="P5" s="144"/>
-      <c r="Q5" s="144"/>
-      <c r="R5" s="144"/>
-      <c r="S5" s="144"/>
-      <c r="T5" s="144"/>
-      <c r="U5" s="144"/>
-      <c r="V5" s="144"/>
-      <c r="W5" s="144"/>
-      <c r="X5" s="144"/>
-      <c r="Y5" s="144"/>
-      <c r="Z5" s="144"/>
-      <c r="AA5" s="144"/>
-      <c r="AB5" s="144"/>
-      <c r="AC5" s="144"/>
-      <c r="AD5" s="144"/>
-      <c r="AE5" s="144"/>
-      <c r="AF5" s="144"/>
-      <c r="AG5" s="145"/>
+      <c r="C5" s="159"/>
+      <c r="D5" s="159"/>
+      <c r="E5" s="159"/>
+      <c r="F5" s="159"/>
+      <c r="G5" s="159"/>
+      <c r="H5" s="159"/>
+      <c r="I5" s="159"/>
+      <c r="J5" s="159"/>
+      <c r="K5" s="159"/>
+      <c r="L5" s="159"/>
+      <c r="M5" s="159"/>
+      <c r="N5" s="159"/>
+      <c r="O5" s="159"/>
+      <c r="P5" s="159"/>
+      <c r="Q5" s="159"/>
+      <c r="R5" s="159"/>
+      <c r="S5" s="159"/>
+      <c r="T5" s="159"/>
+      <c r="U5" s="159"/>
+      <c r="V5" s="159"/>
+      <c r="W5" s="159"/>
+      <c r="X5" s="159"/>
+      <c r="Y5" s="159"/>
+      <c r="Z5" s="159"/>
+      <c r="AA5" s="159"/>
+      <c r="AB5" s="159"/>
+      <c r="AC5" s="159"/>
+      <c r="AD5" s="159"/>
+      <c r="AE5" s="159"/>
+      <c r="AF5" s="159"/>
+      <c r="AG5" s="160"/>
     </row>
     <row r="6" spans="1:33" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="79"/>
-      <c r="B6" s="146" t="s">
+      <c r="A6" s="78"/>
+      <c r="B6" s="161" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="146"/>
-      <c r="D6" s="146"/>
-      <c r="E6" s="146"/>
-      <c r="F6" s="146"/>
-      <c r="G6" s="146"/>
-      <c r="H6" s="146"/>
-      <c r="I6" s="146"/>
-      <c r="J6" s="146"/>
-      <c r="K6" s="146"/>
-      <c r="L6" s="146"/>
-      <c r="M6" s="146"/>
-      <c r="N6" s="146"/>
-      <c r="O6" s="146"/>
-      <c r="P6" s="146"/>
-      <c r="Q6" s="146"/>
-      <c r="R6" s="146"/>
-      <c r="S6" s="146"/>
-      <c r="T6" s="146"/>
-      <c r="U6" s="146"/>
-      <c r="V6" s="146"/>
-      <c r="W6" s="146"/>
-      <c r="X6" s="146"/>
-      <c r="Y6" s="146"/>
-      <c r="Z6" s="146"/>
-      <c r="AA6" s="146"/>
-      <c r="AB6" s="146"/>
-      <c r="AC6" s="146"/>
-      <c r="AD6" s="146"/>
-      <c r="AE6" s="146"/>
-      <c r="AF6" s="146"/>
-      <c r="AG6" s="146"/>
+      <c r="C6" s="161"/>
+      <c r="D6" s="161"/>
+      <c r="E6" s="161"/>
+      <c r="F6" s="161"/>
+      <c r="G6" s="161"/>
+      <c r="H6" s="161"/>
+      <c r="I6" s="161"/>
+      <c r="J6" s="161"/>
+      <c r="K6" s="161"/>
+      <c r="L6" s="161"/>
+      <c r="M6" s="161"/>
+      <c r="N6" s="161"/>
+      <c r="O6" s="161"/>
+      <c r="P6" s="161"/>
+      <c r="Q6" s="161"/>
+      <c r="R6" s="161"/>
+      <c r="S6" s="161"/>
+      <c r="T6" s="161"/>
+      <c r="U6" s="161"/>
+      <c r="V6" s="161"/>
+      <c r="W6" s="161"/>
+      <c r="X6" s="161"/>
+      <c r="Y6" s="161"/>
+      <c r="Z6" s="161"/>
+      <c r="AA6" s="161"/>
+      <c r="AB6" s="161"/>
+      <c r="AC6" s="161"/>
+      <c r="AD6" s="161"/>
+      <c r="AE6" s="161"/>
+      <c r="AF6" s="161"/>
+      <c r="AG6" s="161"/>
     </row>
     <row r="7" spans="1:33" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="79"/>
-      <c r="B7" s="144" t="s">
+      <c r="A7" s="78"/>
+      <c r="B7" s="159" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="144"/>
-      <c r="D7" s="144"/>
-      <c r="E7" s="144"/>
-      <c r="F7" s="144"/>
-      <c r="G7" s="144"/>
-      <c r="H7" s="144"/>
-      <c r="I7" s="144"/>
-      <c r="J7" s="144"/>
-      <c r="K7" s="144"/>
-      <c r="L7" s="144"/>
-      <c r="M7" s="144"/>
-      <c r="N7" s="144"/>
-      <c r="O7" s="144"/>
-      <c r="P7" s="144"/>
-      <c r="Q7" s="144"/>
-      <c r="R7" s="144"/>
-      <c r="S7" s="144"/>
-      <c r="T7" s="144"/>
-      <c r="U7" s="144"/>
-      <c r="V7" s="144"/>
-      <c r="W7" s="144"/>
-      <c r="X7" s="144"/>
-      <c r="Y7" s="144"/>
-      <c r="Z7" s="144"/>
-      <c r="AA7" s="144"/>
-      <c r="AB7" s="144"/>
-      <c r="AC7" s="144"/>
-      <c r="AD7" s="144"/>
-      <c r="AE7" s="144"/>
-      <c r="AF7" s="144"/>
-      <c r="AG7" s="145"/>
+      <c r="C7" s="159"/>
+      <c r="D7" s="159"/>
+      <c r="E7" s="159"/>
+      <c r="F7" s="159"/>
+      <c r="G7" s="159"/>
+      <c r="H7" s="159"/>
+      <c r="I7" s="159"/>
+      <c r="J7" s="159"/>
+      <c r="K7" s="159"/>
+      <c r="L7" s="159"/>
+      <c r="M7" s="159"/>
+      <c r="N7" s="159"/>
+      <c r="O7" s="159"/>
+      <c r="P7" s="159"/>
+      <c r="Q7" s="159"/>
+      <c r="R7" s="159"/>
+      <c r="S7" s="159"/>
+      <c r="T7" s="159"/>
+      <c r="U7" s="159"/>
+      <c r="V7" s="159"/>
+      <c r="W7" s="159"/>
+      <c r="X7" s="159"/>
+      <c r="Y7" s="159"/>
+      <c r="Z7" s="159"/>
+      <c r="AA7" s="159"/>
+      <c r="AB7" s="159"/>
+      <c r="AC7" s="159"/>
+      <c r="AD7" s="159"/>
+      <c r="AE7" s="159"/>
+      <c r="AF7" s="159"/>
+      <c r="AG7" s="160"/>
     </row>
     <row r="8" spans="1:33" s="4" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="80"/>
-      <c r="B8" s="137" t="s">
+      <c r="A8" s="79"/>
+      <c r="B8" s="136" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="135"/>
-      <c r="D8" s="135"/>
-      <c r="E8" s="135"/>
-      <c r="F8" s="136"/>
-      <c r="G8" s="134" t="s">
+      <c r="C8" s="134"/>
+      <c r="D8" s="134"/>
+      <c r="E8" s="134"/>
+      <c r="F8" s="135"/>
+      <c r="G8" s="133" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="135"/>
-      <c r="I8" s="135"/>
-      <c r="J8" s="135"/>
-      <c r="K8" s="135"/>
-      <c r="L8" s="136"/>
-      <c r="M8" s="123" t="s">
+      <c r="H8" s="134"/>
+      <c r="I8" s="134"/>
+      <c r="J8" s="134"/>
+      <c r="K8" s="134"/>
+      <c r="L8" s="135"/>
+      <c r="M8" s="122" t="s">
         <v>6</v>
       </c>
-      <c r="N8" s="114"/>
-      <c r="O8" s="124"/>
-      <c r="P8" s="124"/>
-      <c r="Q8" s="121"/>
-      <c r="R8" s="121"/>
-      <c r="S8" s="121"/>
-      <c r="T8" s="121"/>
-      <c r="U8" s="121"/>
-      <c r="V8" s="121"/>
-      <c r="W8" s="121"/>
-      <c r="X8" s="121"/>
-      <c r="Y8" s="121"/>
-      <c r="Z8" s="121"/>
-      <c r="AA8" s="121"/>
-      <c r="AB8" s="121"/>
-      <c r="AC8" s="121"/>
-      <c r="AD8" s="121"/>
-      <c r="AE8" s="121"/>
-      <c r="AF8" s="121"/>
-      <c r="AG8" s="122"/>
+      <c r="N8" s="113"/>
+      <c r="O8" s="123"/>
+      <c r="P8" s="123"/>
+      <c r="Q8" s="120"/>
+      <c r="R8" s="120"/>
+      <c r="S8" s="120"/>
+      <c r="T8" s="120"/>
+      <c r="U8" s="120"/>
+      <c r="V8" s="120"/>
+      <c r="W8" s="120"/>
+      <c r="X8" s="120"/>
+      <c r="Y8" s="120"/>
+      <c r="Z8" s="120"/>
+      <c r="AA8" s="120"/>
+      <c r="AB8" s="120"/>
+      <c r="AC8" s="120"/>
+      <c r="AD8" s="120"/>
+      <c r="AE8" s="120"/>
+      <c r="AF8" s="120"/>
+      <c r="AG8" s="121"/>
     </row>
     <row r="9" spans="1:33" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="80"/>
-      <c r="B9" s="81"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="81"/>
-      <c r="E9" s="81"/>
-      <c r="F9" s="81"/>
-      <c r="G9" s="81"/>
-      <c r="H9" s="81"/>
-      <c r="I9" s="81"/>
-      <c r="J9" s="81"/>
-      <c r="K9" s="81"/>
-      <c r="L9" s="81"/>
-      <c r="M9" s="81"/>
-      <c r="N9" s="81"/>
-      <c r="O9" s="81"/>
-      <c r="P9" s="81"/>
-      <c r="Q9" s="81"/>
-      <c r="R9" s="81"/>
-      <c r="S9" s="81"/>
-      <c r="T9" s="81"/>
-      <c r="U9" s="81"/>
-      <c r="V9" s="81"/>
-      <c r="W9" s="81"/>
-      <c r="X9" s="81"/>
-      <c r="Y9" s="81"/>
-      <c r="Z9" s="81"/>
-      <c r="AA9" s="81"/>
-      <c r="AB9" s="81"/>
-      <c r="AC9" s="81"/>
-      <c r="AD9" s="81"/>
-      <c r="AE9" s="81"/>
-      <c r="AF9" s="81"/>
-      <c r="AG9" s="82"/>
+      <c r="A9" s="79"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="80"/>
+      <c r="E9" s="80"/>
+      <c r="F9" s="80"/>
+      <c r="G9" s="80"/>
+      <c r="H9" s="80"/>
+      <c r="I9" s="80"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="80"/>
+      <c r="L9" s="80"/>
+      <c r="M9" s="80"/>
+      <c r="N9" s="80"/>
+      <c r="O9" s="80"/>
+      <c r="P9" s="80"/>
+      <c r="Q9" s="80"/>
+      <c r="R9" s="80"/>
+      <c r="S9" s="80"/>
+      <c r="T9" s="80"/>
+      <c r="U9" s="80"/>
+      <c r="V9" s="80"/>
+      <c r="W9" s="80"/>
+      <c r="X9" s="80"/>
+      <c r="Y9" s="80"/>
+      <c r="Z9" s="80"/>
+      <c r="AA9" s="80"/>
+      <c r="AB9" s="80"/>
+      <c r="AC9" s="80"/>
+      <c r="AD9" s="80"/>
+      <c r="AE9" s="80"/>
+      <c r="AF9" s="80"/>
+      <c r="AG9" s="81"/>
     </row>
     <row r="10" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="79"/>
-      <c r="B10" s="142" t="s">
+      <c r="A10" s="78"/>
+      <c r="B10" s="157" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="142"/>
-      <c r="D10" s="142"/>
-      <c r="E10" s="142"/>
-      <c r="F10" s="142"/>
-      <c r="G10" s="142"/>
-      <c r="H10" s="142"/>
-      <c r="I10" s="142"/>
-      <c r="J10" s="142"/>
-      <c r="K10" s="142"/>
-      <c r="L10" s="142"/>
-      <c r="M10" s="142"/>
-      <c r="N10" s="142"/>
-      <c r="O10" s="142"/>
-      <c r="P10" s="142"/>
-      <c r="Q10" s="142"/>
-      <c r="R10" s="142"/>
-      <c r="S10" s="142"/>
-      <c r="T10" s="142"/>
-      <c r="U10" s="142"/>
-      <c r="V10" s="142"/>
-      <c r="W10" s="142"/>
-      <c r="X10" s="142"/>
-      <c r="Y10" s="142"/>
-      <c r="Z10" s="142"/>
-      <c r="AA10" s="142"/>
-      <c r="AB10" s="142"/>
-      <c r="AC10" s="142"/>
-      <c r="AD10" s="142"/>
-      <c r="AE10" s="142"/>
-      <c r="AF10" s="142"/>
-      <c r="AG10" s="142"/>
+      <c r="C10" s="157"/>
+      <c r="D10" s="157"/>
+      <c r="E10" s="157"/>
+      <c r="F10" s="157"/>
+      <c r="G10" s="157"/>
+      <c r="H10" s="157"/>
+      <c r="I10" s="157"/>
+      <c r="J10" s="157"/>
+      <c r="K10" s="157"/>
+      <c r="L10" s="157"/>
+      <c r="M10" s="157"/>
+      <c r="N10" s="157"/>
+      <c r="O10" s="157"/>
+      <c r="P10" s="157"/>
+      <c r="Q10" s="157"/>
+      <c r="R10" s="157"/>
+      <c r="S10" s="157"/>
+      <c r="T10" s="157"/>
+      <c r="U10" s="157"/>
+      <c r="V10" s="157"/>
+      <c r="W10" s="157"/>
+      <c r="X10" s="157"/>
+      <c r="Y10" s="157"/>
+      <c r="Z10" s="157"/>
+      <c r="AA10" s="157"/>
+      <c r="AB10" s="157"/>
+      <c r="AC10" s="157"/>
+      <c r="AD10" s="157"/>
+      <c r="AE10" s="157"/>
+      <c r="AF10" s="157"/>
+      <c r="AG10" s="157"/>
     </row>
     <row r="11" spans="1:33" s="4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="45" t="s">
+      <c r="B11" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="46"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="48" t="s">
+      <c r="C11" s="45"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="47" t="s">
         <v>37</v>
       </c>
       <c r="F11" s="8"/>
-      <c r="G11" s="49" t="s">
+      <c r="G11" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="143"/>
-      <c r="I11" s="143"/>
-      <c r="J11" s="143"/>
-      <c r="K11" s="143"/>
-      <c r="L11" s="143"/>
-      <c r="M11" s="115"/>
-      <c r="N11" s="115"/>
-      <c r="O11" s="74" t="s">
+      <c r="H11" s="158"/>
+      <c r="I11" s="158"/>
+      <c r="J11" s="158"/>
+      <c r="K11" s="158"/>
+      <c r="L11" s="158"/>
+      <c r="M11" s="114"/>
+      <c r="N11" s="114"/>
+      <c r="O11" s="73" t="s">
         <v>38</v>
       </c>
-      <c r="P11" s="109"/>
-      <c r="Q11" s="109"/>
-      <c r="R11" s="109"/>
-      <c r="S11" s="109"/>
-      <c r="T11" s="109"/>
-      <c r="U11" s="109"/>
-      <c r="V11" s="109"/>
-      <c r="W11" s="109"/>
-      <c r="X11" s="109"/>
-      <c r="Y11" s="109"/>
-      <c r="Z11" s="109"/>
-      <c r="AA11" s="109"/>
-      <c r="AB11" s="109"/>
-      <c r="AC11" s="109"/>
-      <c r="AD11" s="109"/>
-      <c r="AE11" s="58"/>
-      <c r="AF11" s="119"/>
-      <c r="AG11" s="59"/>
+      <c r="P11" s="108"/>
+      <c r="Q11" s="108"/>
+      <c r="R11" s="108"/>
+      <c r="S11" s="108"/>
+      <c r="T11" s="108"/>
+      <c r="U11" s="108"/>
+      <c r="V11" s="108"/>
+      <c r="W11" s="108"/>
+      <c r="X11" s="108"/>
+      <c r="Y11" s="108"/>
+      <c r="Z11" s="108"/>
+      <c r="AA11" s="108"/>
+      <c r="AB11" s="108"/>
+      <c r="AC11" s="108"/>
+      <c r="AD11" s="108"/>
+      <c r="AE11" s="57"/>
+      <c r="AF11" s="118"/>
+      <c r="AG11" s="58"/>
     </row>
     <row r="12" spans="1:33" s="4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="25" t="s">
         <v>8</v>
       </c>
       <c r="C12" s="9"/>
-      <c r="D12" s="38"/>
-      <c r="E12" s="36"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="162"/>
       <c r="F12" s="34"/>
       <c r="G12" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="153"/>
-      <c r="I12" s="154"/>
-      <c r="J12" s="153"/>
-      <c r="K12" s="153"/>
-      <c r="L12" s="153"/>
-      <c r="M12" s="116"/>
-      <c r="N12" s="116"/>
+      <c r="H12" s="151"/>
+      <c r="I12" s="152"/>
+      <c r="J12" s="151"/>
+      <c r="K12" s="151"/>
+      <c r="L12" s="151"/>
+      <c r="M12" s="115"/>
+      <c r="N12" s="115"/>
       <c r="O12" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="P12" s="110"/>
-      <c r="Q12" s="110"/>
-      <c r="R12" s="110"/>
-      <c r="S12" s="110"/>
-      <c r="T12" s="110"/>
-      <c r="U12" s="110"/>
-      <c r="V12" s="110"/>
-      <c r="W12" s="110"/>
-      <c r="X12" s="110"/>
-      <c r="Y12" s="110"/>
-      <c r="Z12" s="110"/>
-      <c r="AA12" s="110"/>
-      <c r="AB12" s="110"/>
-      <c r="AC12" s="110"/>
-      <c r="AD12" s="110"/>
+      <c r="P12" s="109"/>
+      <c r="Q12" s="109"/>
+      <c r="R12" s="109"/>
+      <c r="S12" s="109"/>
+      <c r="T12" s="109"/>
+      <c r="U12" s="109"/>
+      <c r="V12" s="109"/>
+      <c r="W12" s="109"/>
+      <c r="X12" s="109"/>
+      <c r="Y12" s="109"/>
+      <c r="Z12" s="109"/>
+      <c r="AA12" s="109"/>
+      <c r="AB12" s="109"/>
+      <c r="AC12" s="109"/>
+      <c r="AD12" s="109"/>
       <c r="AE12" s="11"/>
       <c r="AF12" s="11"/>
       <c r="AG12" s="26"/>
     </row>
     <row r="13" spans="1:33" s="4" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="71" t="s">
+      <c r="B13" s="70" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="72"/>
-      <c r="D13" s="73"/>
-      <c r="E13" s="160" t="s">
+      <c r="C13" s="71"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="142" t="s">
         <v>37</v>
       </c>
       <c r="F13" s="34"/>
-      <c r="G13" s="88" t="s">
+      <c r="G13" s="87" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="162" t="s">
+      <c r="H13" s="144" t="s">
         <v>37</v>
       </c>
       <c r="I13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="J13" s="155"/>
-      <c r="K13" s="155"/>
-      <c r="L13" s="155"/>
-      <c r="M13" s="117"/>
-      <c r="N13" s="117"/>
+      <c r="J13" s="153"/>
+      <c r="K13" s="153"/>
+      <c r="L13" s="153"/>
+      <c r="M13" s="116"/>
+      <c r="N13" s="116"/>
       <c r="O13" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="P13" s="110"/>
-      <c r="Q13" s="110"/>
-      <c r="R13" s="110"/>
-      <c r="S13" s="110"/>
-      <c r="T13" s="110"/>
-      <c r="U13" s="110"/>
-      <c r="V13" s="110"/>
-      <c r="W13" s="110"/>
-      <c r="X13" s="110"/>
-      <c r="Y13" s="110"/>
-      <c r="Z13" s="110"/>
-      <c r="AA13" s="110"/>
-      <c r="AB13" s="110"/>
-      <c r="AC13" s="110"/>
-      <c r="AD13" s="110"/>
+      <c r="P13" s="109"/>
+      <c r="Q13" s="109"/>
+      <c r="R13" s="109"/>
+      <c r="S13" s="109"/>
+      <c r="T13" s="109"/>
+      <c r="U13" s="109"/>
+      <c r="V13" s="109"/>
+      <c r="W13" s="109"/>
+      <c r="X13" s="109"/>
+      <c r="Y13" s="109"/>
+      <c r="Z13" s="109"/>
+      <c r="AA13" s="109"/>
+      <c r="AB13" s="109"/>
+      <c r="AC13" s="109"/>
+      <c r="AD13" s="109"/>
       <c r="AE13" s="11"/>
       <c r="AF13" s="11"/>
       <c r="AG13" s="26"/>
@@ -2933,86 +2933,86 @@
       <c r="B14" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="39"/>
-      <c r="E14" s="159" t="s">
+      <c r="C14" s="36"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="141" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="40"/>
-      <c r="G14" s="44" t="s">
+      <c r="F14" s="39"/>
+      <c r="G14" s="43" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="161" t="s">
+      <c r="H14" s="143" t="s">
         <v>37</v>
       </c>
       <c r="I14" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="156"/>
-      <c r="K14" s="156"/>
-      <c r="L14" s="156"/>
-      <c r="M14" s="118"/>
-      <c r="N14" s="118"/>
+      <c r="J14" s="154"/>
+      <c r="K14" s="154"/>
+      <c r="L14" s="154"/>
+      <c r="M14" s="117"/>
+      <c r="N14" s="117"/>
       <c r="O14" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="P14" s="111"/>
-      <c r="Q14" s="111"/>
-      <c r="R14" s="111"/>
-      <c r="S14" s="111"/>
-      <c r="T14" s="111"/>
-      <c r="U14" s="111"/>
-      <c r="V14" s="111"/>
-      <c r="W14" s="111"/>
-      <c r="X14" s="111"/>
-      <c r="Y14" s="111"/>
-      <c r="Z14" s="111"/>
-      <c r="AA14" s="111"/>
-      <c r="AB14" s="111"/>
-      <c r="AC14" s="111"/>
-      <c r="AD14" s="111"/>
+      <c r="P14" s="110"/>
+      <c r="Q14" s="110"/>
+      <c r="R14" s="110"/>
+      <c r="S14" s="110"/>
+      <c r="T14" s="110"/>
+      <c r="U14" s="110"/>
+      <c r="V14" s="110"/>
+      <c r="W14" s="110"/>
+      <c r="X14" s="110"/>
+      <c r="Y14" s="110"/>
+      <c r="Z14" s="110"/>
+      <c r="AA14" s="110"/>
+      <c r="AB14" s="110"/>
+      <c r="AC14" s="110"/>
+      <c r="AD14" s="110"/>
       <c r="AE14" s="30"/>
       <c r="AF14" s="30"/>
       <c r="AG14" s="31"/>
     </row>
     <row r="15" spans="1:33" s="4" customFormat="1" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="83"/>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="84"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="84" t="s">
+      <c r="B15" s="82"/>
+      <c r="C15" s="83"/>
+      <c r="D15" s="83"/>
+      <c r="E15" s="83"/>
+      <c r="F15" s="83"/>
+      <c r="G15" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="H15" s="84"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="85"/>
-      <c r="K15" s="85"/>
-      <c r="L15" s="86"/>
-      <c r="M15" s="84"/>
-      <c r="N15" s="84"/>
-      <c r="O15" s="87"/>
-      <c r="P15" s="87"/>
-      <c r="Q15" s="87"/>
-      <c r="R15" s="87"/>
-      <c r="S15" s="87"/>
-      <c r="T15" s="87"/>
-      <c r="U15" s="87"/>
-      <c r="V15" s="87"/>
-      <c r="W15" s="87"/>
-      <c r="X15" s="87"/>
-      <c r="Y15" s="87"/>
-      <c r="Z15" s="87"/>
-      <c r="AA15" s="87"/>
-      <c r="AB15" s="87"/>
-      <c r="AC15" s="87"/>
-      <c r="AD15" s="87"/>
-      <c r="AE15" s="85"/>
-      <c r="AF15" s="85"/>
-      <c r="AG15" s="86"/>
+      <c r="H15" s="83"/>
+      <c r="I15" s="83"/>
+      <c r="J15" s="84"/>
+      <c r="K15" s="84"/>
+      <c r="L15" s="85"/>
+      <c r="M15" s="83"/>
+      <c r="N15" s="83"/>
+      <c r="O15" s="86"/>
+      <c r="P15" s="86"/>
+      <c r="Q15" s="86"/>
+      <c r="R15" s="86"/>
+      <c r="S15" s="86"/>
+      <c r="T15" s="86"/>
+      <c r="U15" s="86"/>
+      <c r="V15" s="86"/>
+      <c r="W15" s="86"/>
+      <c r="X15" s="86"/>
+      <c r="Y15" s="86"/>
+      <c r="Z15" s="86"/>
+      <c r="AA15" s="86"/>
+      <c r="AB15" s="86"/>
+      <c r="AC15" s="86"/>
+      <c r="AD15" s="86"/>
+      <c r="AE15" s="84"/>
+      <c r="AF15" s="84"/>
+      <c r="AG15" s="85"/>
     </row>
     <row r="16" spans="1:33" s="2" customFormat="1" ht="75.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="151" t="s">
+      <c r="B16" s="149" t="s">
         <v>41</v>
       </c>
       <c r="C16" s="15"/>
@@ -3022,48 +3022,48 @@
       <c r="G16" s="20"/>
       <c r="H16" s="16"/>
       <c r="I16" s="33"/>
-      <c r="J16" s="149" t="s">
+      <c r="J16" s="147" t="s">
         <v>25</v>
       </c>
-      <c r="K16" s="150"/>
-      <c r="L16" s="60"/>
-      <c r="M16" s="133" t="s">
+      <c r="K16" s="148"/>
+      <c r="L16" s="59"/>
+      <c r="M16" s="132" t="s">
         <v>75</v>
       </c>
-      <c r="N16" s="125"/>
-      <c r="O16" s="126"/>
-      <c r="P16" s="132" t="s">
+      <c r="N16" s="124"/>
+      <c r="O16" s="125"/>
+      <c r="P16" s="131" t="s">
         <v>28</v>
       </c>
-      <c r="Q16" s="127"/>
-      <c r="R16" s="128" t="s">
+      <c r="Q16" s="126"/>
+      <c r="R16" s="127" t="s">
         <v>27</v>
       </c>
-      <c r="S16" s="128"/>
-      <c r="T16" s="128"/>
-      <c r="U16" s="128"/>
-      <c r="V16" s="128"/>
-      <c r="W16" s="128"/>
-      <c r="X16" s="128"/>
-      <c r="Y16" s="128"/>
-      <c r="Z16" s="129" t="s">
+      <c r="S16" s="127"/>
+      <c r="T16" s="127"/>
+      <c r="U16" s="127"/>
+      <c r="V16" s="127"/>
+      <c r="W16" s="127"/>
+      <c r="X16" s="127"/>
+      <c r="Y16" s="127"/>
+      <c r="Z16" s="128" t="s">
         <v>70</v>
       </c>
-      <c r="AA16" s="130"/>
-      <c r="AB16" s="130"/>
-      <c r="AC16" s="130"/>
-      <c r="AD16" s="131"/>
-      <c r="AE16" s="148" t="s">
+      <c r="AA16" s="129"/>
+      <c r="AB16" s="129"/>
+      <c r="AC16" s="129"/>
+      <c r="AD16" s="130"/>
+      <c r="AE16" s="146" t="s">
         <v>55</v>
       </c>
-      <c r="AF16" s="148"/>
-      <c r="AG16" s="41" t="s">
+      <c r="AF16" s="146"/>
+      <c r="AG16" s="40" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" spans="2:33" s="2" customFormat="1" ht="138.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="152"/>
-      <c r="C17" s="70" t="s">
+      <c r="B17" s="150"/>
+      <c r="C17" s="69" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="17" t="s">
@@ -3081,7 +3081,7 @@
       <c r="H17" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="I17" s="43" t="s">
+      <c r="I17" s="42" t="s">
         <v>24</v>
       </c>
       <c r="J17" s="14" t="s">
@@ -3132,13 +3132,13 @@
       <c r="Y17" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="Z17" s="112" t="s">
+      <c r="Z17" s="111" t="s">
         <v>31</v>
       </c>
-      <c r="AA17" s="113" t="s">
+      <c r="AA17" s="112" t="s">
         <v>29</v>
       </c>
-      <c r="AB17" s="113" t="s">
+      <c r="AB17" s="112" t="s">
         <v>30</v>
       </c>
       <c r="AC17" s="13" t="s">
@@ -3153,940 +3153,940 @@
       <c r="AF17" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="AG17" s="42" t="s">
+      <c r="AG17" s="41" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="18" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="89">
+      <c r="B18" s="88">
         <v>1</v>
       </c>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="61"/>
-      <c r="G18" s="61"/>
-      <c r="H18" s="61"/>
-      <c r="I18" s="61"/>
-      <c r="J18" s="90"/>
-      <c r="K18" s="91"/>
-      <c r="L18" s="91"/>
-      <c r="M18" s="91"/>
-      <c r="N18" s="91"/>
-      <c r="O18" s="91"/>
-      <c r="P18" s="91"/>
-      <c r="Q18" s="91"/>
-      <c r="R18" s="91"/>
-      <c r="S18" s="91"/>
-      <c r="T18" s="91"/>
-      <c r="U18" s="91"/>
-      <c r="V18" s="91"/>
-      <c r="W18" s="91"/>
-      <c r="X18" s="91"/>
-      <c r="Y18" s="91"/>
-      <c r="Z18" s="91"/>
-      <c r="AA18" s="91"/>
-      <c r="AB18" s="91"/>
-      <c r="AC18" s="91"/>
-      <c r="AD18" s="91"/>
-      <c r="AE18" s="91"/>
-      <c r="AF18" s="91"/>
-      <c r="AG18" s="92"/>
+      <c r="C18" s="60"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="60"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="89"/>
+      <c r="K18" s="90"/>
+      <c r="L18" s="90"/>
+      <c r="M18" s="90"/>
+      <c r="N18" s="90"/>
+      <c r="O18" s="90"/>
+      <c r="P18" s="90"/>
+      <c r="Q18" s="90"/>
+      <c r="R18" s="90"/>
+      <c r="S18" s="90"/>
+      <c r="T18" s="90"/>
+      <c r="U18" s="90"/>
+      <c r="V18" s="90"/>
+      <c r="W18" s="90"/>
+      <c r="X18" s="90"/>
+      <c r="Y18" s="90"/>
+      <c r="Z18" s="90"/>
+      <c r="AA18" s="90"/>
+      <c r="AB18" s="90"/>
+      <c r="AC18" s="90"/>
+      <c r="AD18" s="90"/>
+      <c r="AE18" s="90"/>
+      <c r="AF18" s="90"/>
+      <c r="AG18" s="91"/>
     </row>
     <row r="19" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="93">
+      <c r="B19" s="92">
         <v>2</v>
       </c>
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="62"/>
-      <c r="H19" s="62"/>
-      <c r="I19" s="62"/>
-      <c r="J19" s="94"/>
-      <c r="K19" s="95"/>
-      <c r="L19" s="91"/>
-      <c r="M19" s="91"/>
-      <c r="N19" s="91"/>
-      <c r="O19" s="95"/>
-      <c r="P19" s="95"/>
-      <c r="Q19" s="95"/>
-      <c r="R19" s="95"/>
-      <c r="S19" s="95"/>
-      <c r="T19" s="95"/>
-      <c r="U19" s="95"/>
-      <c r="V19" s="95"/>
-      <c r="W19" s="95"/>
-      <c r="X19" s="95"/>
-      <c r="Y19" s="95"/>
-      <c r="Z19" s="95"/>
-      <c r="AA19" s="95"/>
-      <c r="AB19" s="95"/>
-      <c r="AC19" s="95"/>
-      <c r="AD19" s="95"/>
-      <c r="AE19" s="95"/>
-      <c r="AF19" s="95"/>
-      <c r="AG19" s="96"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="61"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="61"/>
+      <c r="H19" s="61"/>
+      <c r="I19" s="61"/>
+      <c r="J19" s="93"/>
+      <c r="K19" s="94"/>
+      <c r="L19" s="90"/>
+      <c r="M19" s="90"/>
+      <c r="N19" s="90"/>
+      <c r="O19" s="94"/>
+      <c r="P19" s="94"/>
+      <c r="Q19" s="94"/>
+      <c r="R19" s="94"/>
+      <c r="S19" s="94"/>
+      <c r="T19" s="94"/>
+      <c r="U19" s="94"/>
+      <c r="V19" s="94"/>
+      <c r="W19" s="94"/>
+      <c r="X19" s="94"/>
+      <c r="Y19" s="94"/>
+      <c r="Z19" s="94"/>
+      <c r="AA19" s="94"/>
+      <c r="AB19" s="94"/>
+      <c r="AC19" s="94"/>
+      <c r="AD19" s="94"/>
+      <c r="AE19" s="94"/>
+      <c r="AF19" s="94"/>
+      <c r="AG19" s="95"/>
     </row>
     <row r="20" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="93">
+      <c r="B20" s="92">
         <v>3</v>
       </c>
-      <c r="C20" s="62"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="94"/>
-      <c r="K20" s="95"/>
-      <c r="L20" s="91"/>
-      <c r="M20" s="91"/>
-      <c r="N20" s="91"/>
-      <c r="O20" s="95"/>
-      <c r="P20" s="95"/>
-      <c r="Q20" s="95"/>
-      <c r="R20" s="95"/>
-      <c r="S20" s="95"/>
-      <c r="T20" s="95"/>
-      <c r="U20" s="95"/>
-      <c r="V20" s="95"/>
-      <c r="W20" s="95"/>
-      <c r="X20" s="95"/>
-      <c r="Y20" s="95"/>
-      <c r="Z20" s="95"/>
-      <c r="AA20" s="95"/>
-      <c r="AB20" s="95"/>
-      <c r="AC20" s="95"/>
-      <c r="AD20" s="95"/>
-      <c r="AE20" s="95"/>
-      <c r="AF20" s="95"/>
-      <c r="AG20" s="96"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="61"/>
+      <c r="I20" s="61"/>
+      <c r="J20" s="93"/>
+      <c r="K20" s="94"/>
+      <c r="L20" s="90"/>
+      <c r="M20" s="90"/>
+      <c r="N20" s="90"/>
+      <c r="O20" s="94"/>
+      <c r="P20" s="94"/>
+      <c r="Q20" s="94"/>
+      <c r="R20" s="94"/>
+      <c r="S20" s="94"/>
+      <c r="T20" s="94"/>
+      <c r="U20" s="94"/>
+      <c r="V20" s="94"/>
+      <c r="W20" s="94"/>
+      <c r="X20" s="94"/>
+      <c r="Y20" s="94"/>
+      <c r="Z20" s="94"/>
+      <c r="AA20" s="94"/>
+      <c r="AB20" s="94"/>
+      <c r="AC20" s="94"/>
+      <c r="AD20" s="94"/>
+      <c r="AE20" s="94"/>
+      <c r="AF20" s="94"/>
+      <c r="AG20" s="95"/>
     </row>
     <row r="21" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="89">
+      <c r="B21" s="88">
         <v>4</v>
       </c>
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="62"/>
-      <c r="I21" s="62"/>
-      <c r="J21" s="94"/>
-      <c r="K21" s="95"/>
-      <c r="L21" s="91"/>
-      <c r="M21" s="91"/>
-      <c r="N21" s="91"/>
-      <c r="O21" s="95"/>
-      <c r="P21" s="95"/>
-      <c r="Q21" s="95"/>
-      <c r="R21" s="95"/>
-      <c r="S21" s="95"/>
-      <c r="T21" s="95"/>
-      <c r="U21" s="95"/>
-      <c r="V21" s="95"/>
-      <c r="W21" s="95"/>
-      <c r="X21" s="95"/>
-      <c r="Y21" s="95"/>
-      <c r="Z21" s="95"/>
-      <c r="AA21" s="95"/>
-      <c r="AB21" s="95"/>
-      <c r="AC21" s="95"/>
-      <c r="AD21" s="95"/>
-      <c r="AE21" s="95"/>
-      <c r="AF21" s="95"/>
-      <c r="AG21" s="96"/>
+      <c r="C21" s="61"/>
+      <c r="D21" s="61"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="61"/>
+      <c r="I21" s="61"/>
+      <c r="J21" s="93"/>
+      <c r="K21" s="94"/>
+      <c r="L21" s="90"/>
+      <c r="M21" s="90"/>
+      <c r="N21" s="90"/>
+      <c r="O21" s="94"/>
+      <c r="P21" s="94"/>
+      <c r="Q21" s="94"/>
+      <c r="R21" s="94"/>
+      <c r="S21" s="94"/>
+      <c r="T21" s="94"/>
+      <c r="U21" s="94"/>
+      <c r="V21" s="94"/>
+      <c r="W21" s="94"/>
+      <c r="X21" s="94"/>
+      <c r="Y21" s="94"/>
+      <c r="Z21" s="94"/>
+      <c r="AA21" s="94"/>
+      <c r="AB21" s="94"/>
+      <c r="AC21" s="94"/>
+      <c r="AD21" s="94"/>
+      <c r="AE21" s="94"/>
+      <c r="AF21" s="94"/>
+      <c r="AG21" s="95"/>
     </row>
     <row r="22" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="93">
+      <c r="B22" s="92">
         <v>5</v>
       </c>
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="62"/>
-      <c r="I22" s="62"/>
-      <c r="J22" s="94"/>
-      <c r="K22" s="95"/>
-      <c r="L22" s="91"/>
-      <c r="M22" s="91"/>
-      <c r="N22" s="91"/>
-      <c r="O22" s="95"/>
-      <c r="P22" s="95"/>
-      <c r="Q22" s="95"/>
-      <c r="R22" s="95"/>
-      <c r="S22" s="95"/>
-      <c r="T22" s="95"/>
-      <c r="U22" s="95"/>
-      <c r="V22" s="95"/>
-      <c r="W22" s="95"/>
-      <c r="X22" s="95"/>
-      <c r="Y22" s="95"/>
-      <c r="Z22" s="95"/>
-      <c r="AA22" s="95"/>
-      <c r="AB22" s="95"/>
-      <c r="AC22" s="95"/>
-      <c r="AD22" s="95"/>
-      <c r="AE22" s="95"/>
-      <c r="AF22" s="95"/>
-      <c r="AG22" s="96"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="61"/>
+      <c r="I22" s="61"/>
+      <c r="J22" s="93"/>
+      <c r="K22" s="94"/>
+      <c r="L22" s="90"/>
+      <c r="M22" s="90"/>
+      <c r="N22" s="90"/>
+      <c r="O22" s="94"/>
+      <c r="P22" s="94"/>
+      <c r="Q22" s="94"/>
+      <c r="R22" s="94"/>
+      <c r="S22" s="94"/>
+      <c r="T22" s="94"/>
+      <c r="U22" s="94"/>
+      <c r="V22" s="94"/>
+      <c r="W22" s="94"/>
+      <c r="X22" s="94"/>
+      <c r="Y22" s="94"/>
+      <c r="Z22" s="94"/>
+      <c r="AA22" s="94"/>
+      <c r="AB22" s="94"/>
+      <c r="AC22" s="94"/>
+      <c r="AD22" s="94"/>
+      <c r="AE22" s="94"/>
+      <c r="AF22" s="94"/>
+      <c r="AG22" s="95"/>
     </row>
     <row r="23" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="93">
+      <c r="B23" s="92">
         <v>6</v>
       </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="94"/>
-      <c r="K23" s="63"/>
-      <c r="L23" s="91"/>
-      <c r="M23" s="91"/>
-      <c r="N23" s="91"/>
-      <c r="O23" s="63"/>
-      <c r="P23" s="63"/>
-      <c r="Q23" s="63"/>
-      <c r="R23" s="63"/>
-      <c r="S23" s="63"/>
-      <c r="T23" s="63"/>
-      <c r="U23" s="63"/>
-      <c r="V23" s="63"/>
-      <c r="W23" s="63"/>
-      <c r="X23" s="63"/>
-      <c r="Y23" s="63"/>
-      <c r="Z23" s="63"/>
-      <c r="AA23" s="63"/>
-      <c r="AB23" s="63"/>
-      <c r="AC23" s="63"/>
-      <c r="AD23" s="63"/>
-      <c r="AE23" s="63"/>
-      <c r="AF23" s="63"/>
-      <c r="AG23" s="64"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="61"/>
+      <c r="E23" s="61"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="61"/>
+      <c r="I23" s="61"/>
+      <c r="J23" s="93"/>
+      <c r="K23" s="62"/>
+      <c r="L23" s="90"/>
+      <c r="M23" s="90"/>
+      <c r="N23" s="90"/>
+      <c r="O23" s="62"/>
+      <c r="P23" s="62"/>
+      <c r="Q23" s="62"/>
+      <c r="R23" s="62"/>
+      <c r="S23" s="62"/>
+      <c r="T23" s="62"/>
+      <c r="U23" s="62"/>
+      <c r="V23" s="62"/>
+      <c r="W23" s="62"/>
+      <c r="X23" s="62"/>
+      <c r="Y23" s="62"/>
+      <c r="Z23" s="62"/>
+      <c r="AA23" s="62"/>
+      <c r="AB23" s="62"/>
+      <c r="AC23" s="62"/>
+      <c r="AD23" s="62"/>
+      <c r="AE23" s="62"/>
+      <c r="AF23" s="62"/>
+      <c r="AG23" s="63"/>
     </row>
     <row r="24" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="89">
+      <c r="B24" s="88">
         <v>7</v>
       </c>
-      <c r="C24" s="62"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="62"/>
-      <c r="I24" s="62"/>
-      <c r="J24" s="94"/>
-      <c r="K24" s="95"/>
-      <c r="L24" s="91"/>
-      <c r="M24" s="91"/>
-      <c r="N24" s="91"/>
-      <c r="O24" s="95"/>
-      <c r="P24" s="95"/>
-      <c r="Q24" s="95"/>
-      <c r="R24" s="95"/>
-      <c r="S24" s="95"/>
-      <c r="T24" s="95"/>
-      <c r="U24" s="95"/>
-      <c r="V24" s="95"/>
-      <c r="W24" s="95"/>
-      <c r="X24" s="95"/>
-      <c r="Y24" s="95"/>
-      <c r="Z24" s="95"/>
-      <c r="AA24" s="95"/>
-      <c r="AB24" s="95"/>
-      <c r="AC24" s="95"/>
-      <c r="AD24" s="95"/>
-      <c r="AE24" s="95"/>
-      <c r="AF24" s="95"/>
-      <c r="AG24" s="96"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="61"/>
+      <c r="I24" s="61"/>
+      <c r="J24" s="93"/>
+      <c r="K24" s="94"/>
+      <c r="L24" s="90"/>
+      <c r="M24" s="90"/>
+      <c r="N24" s="90"/>
+      <c r="O24" s="94"/>
+      <c r="P24" s="94"/>
+      <c r="Q24" s="94"/>
+      <c r="R24" s="94"/>
+      <c r="S24" s="94"/>
+      <c r="T24" s="94"/>
+      <c r="U24" s="94"/>
+      <c r="V24" s="94"/>
+      <c r="W24" s="94"/>
+      <c r="X24" s="94"/>
+      <c r="Y24" s="94"/>
+      <c r="Z24" s="94"/>
+      <c r="AA24" s="94"/>
+      <c r="AB24" s="94"/>
+      <c r="AC24" s="94"/>
+      <c r="AD24" s="94"/>
+      <c r="AE24" s="94"/>
+      <c r="AF24" s="94"/>
+      <c r="AG24" s="95"/>
     </row>
     <row r="25" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="93">
+      <c r="B25" s="92">
         <v>8</v>
       </c>
-      <c r="C25" s="62"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="62"/>
-      <c r="G25" s="62"/>
-      <c r="H25" s="62"/>
-      <c r="I25" s="62"/>
-      <c r="J25" s="94"/>
-      <c r="K25" s="95"/>
-      <c r="L25" s="91"/>
-      <c r="M25" s="91"/>
-      <c r="N25" s="91"/>
-      <c r="O25" s="95"/>
-      <c r="P25" s="95"/>
-      <c r="Q25" s="95"/>
-      <c r="R25" s="95"/>
-      <c r="S25" s="95"/>
-      <c r="T25" s="95"/>
-      <c r="U25" s="95"/>
-      <c r="V25" s="95"/>
-      <c r="W25" s="95"/>
-      <c r="X25" s="95"/>
-      <c r="Y25" s="95"/>
-      <c r="Z25" s="95"/>
-      <c r="AA25" s="95"/>
-      <c r="AB25" s="95"/>
-      <c r="AC25" s="95"/>
-      <c r="AD25" s="95"/>
-      <c r="AE25" s="95"/>
-      <c r="AF25" s="95"/>
-      <c r="AG25" s="96"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="61"/>
+      <c r="E25" s="61"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="61"/>
+      <c r="I25" s="61"/>
+      <c r="J25" s="93"/>
+      <c r="K25" s="94"/>
+      <c r="L25" s="90"/>
+      <c r="M25" s="90"/>
+      <c r="N25" s="90"/>
+      <c r="O25" s="94"/>
+      <c r="P25" s="94"/>
+      <c r="Q25" s="94"/>
+      <c r="R25" s="94"/>
+      <c r="S25" s="94"/>
+      <c r="T25" s="94"/>
+      <c r="U25" s="94"/>
+      <c r="V25" s="94"/>
+      <c r="W25" s="94"/>
+      <c r="X25" s="94"/>
+      <c r="Y25" s="94"/>
+      <c r="Z25" s="94"/>
+      <c r="AA25" s="94"/>
+      <c r="AB25" s="94"/>
+      <c r="AC25" s="94"/>
+      <c r="AD25" s="94"/>
+      <c r="AE25" s="94"/>
+      <c r="AF25" s="94"/>
+      <c r="AG25" s="95"/>
     </row>
     <row r="26" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="93">
+      <c r="B26" s="92">
         <v>9</v>
       </c>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="62"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="62"/>
-      <c r="J26" s="94"/>
-      <c r="K26" s="95"/>
-      <c r="L26" s="91"/>
-      <c r="M26" s="91"/>
-      <c r="N26" s="91"/>
-      <c r="O26" s="95"/>
-      <c r="P26" s="95"/>
-      <c r="Q26" s="95"/>
-      <c r="R26" s="95"/>
-      <c r="S26" s="95"/>
-      <c r="T26" s="95"/>
-      <c r="U26" s="95"/>
-      <c r="V26" s="95"/>
-      <c r="W26" s="95"/>
-      <c r="X26" s="95"/>
-      <c r="Y26" s="95"/>
-      <c r="Z26" s="95"/>
-      <c r="AA26" s="95"/>
-      <c r="AB26" s="95"/>
-      <c r="AC26" s="95"/>
-      <c r="AD26" s="95"/>
-      <c r="AE26" s="95"/>
-      <c r="AF26" s="95"/>
-      <c r="AG26" s="96"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="61"/>
+      <c r="I26" s="61"/>
+      <c r="J26" s="93"/>
+      <c r="K26" s="94"/>
+      <c r="L26" s="90"/>
+      <c r="M26" s="90"/>
+      <c r="N26" s="90"/>
+      <c r="O26" s="94"/>
+      <c r="P26" s="94"/>
+      <c r="Q26" s="94"/>
+      <c r="R26" s="94"/>
+      <c r="S26" s="94"/>
+      <c r="T26" s="94"/>
+      <c r="U26" s="94"/>
+      <c r="V26" s="94"/>
+      <c r="W26" s="94"/>
+      <c r="X26" s="94"/>
+      <c r="Y26" s="94"/>
+      <c r="Z26" s="94"/>
+      <c r="AA26" s="94"/>
+      <c r="AB26" s="94"/>
+      <c r="AC26" s="94"/>
+      <c r="AD26" s="94"/>
+      <c r="AE26" s="94"/>
+      <c r="AF26" s="94"/>
+      <c r="AG26" s="95"/>
     </row>
     <row r="27" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="89">
+      <c r="B27" s="88">
         <v>10</v>
       </c>
-      <c r="C27" s="62"/>
-      <c r="D27" s="62"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="62"/>
-      <c r="H27" s="62"/>
-      <c r="I27" s="62"/>
-      <c r="J27" s="94"/>
-      <c r="K27" s="95"/>
-      <c r="L27" s="91"/>
-      <c r="M27" s="91"/>
-      <c r="N27" s="91"/>
-      <c r="O27" s="95"/>
-      <c r="P27" s="95"/>
-      <c r="Q27" s="95"/>
-      <c r="R27" s="95"/>
-      <c r="S27" s="95"/>
-      <c r="T27" s="95"/>
-      <c r="U27" s="95"/>
-      <c r="V27" s="95"/>
-      <c r="W27" s="95"/>
-      <c r="X27" s="95"/>
-      <c r="Y27" s="95"/>
-      <c r="Z27" s="95"/>
-      <c r="AA27" s="95"/>
-      <c r="AB27" s="95"/>
-      <c r="AC27" s="95"/>
-      <c r="AD27" s="95"/>
-      <c r="AE27" s="95"/>
-      <c r="AF27" s="95"/>
-      <c r="AG27" s="96"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="61"/>
+      <c r="I27" s="61"/>
+      <c r="J27" s="93"/>
+      <c r="K27" s="94"/>
+      <c r="L27" s="90"/>
+      <c r="M27" s="90"/>
+      <c r="N27" s="90"/>
+      <c r="O27" s="94"/>
+      <c r="P27" s="94"/>
+      <c r="Q27" s="94"/>
+      <c r="R27" s="94"/>
+      <c r="S27" s="94"/>
+      <c r="T27" s="94"/>
+      <c r="U27" s="94"/>
+      <c r="V27" s="94"/>
+      <c r="W27" s="94"/>
+      <c r="X27" s="94"/>
+      <c r="Y27" s="94"/>
+      <c r="Z27" s="94"/>
+      <c r="AA27" s="94"/>
+      <c r="AB27" s="94"/>
+      <c r="AC27" s="94"/>
+      <c r="AD27" s="94"/>
+      <c r="AE27" s="94"/>
+      <c r="AF27" s="94"/>
+      <c r="AG27" s="95"/>
     </row>
     <row r="28" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="93">
+      <c r="B28" s="92">
         <v>11</v>
       </c>
-      <c r="C28" s="62"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="62"/>
-      <c r="H28" s="62"/>
-      <c r="I28" s="62"/>
-      <c r="J28" s="94"/>
-      <c r="K28" s="95"/>
-      <c r="L28" s="91"/>
-      <c r="M28" s="91"/>
-      <c r="N28" s="91"/>
-      <c r="O28" s="95"/>
-      <c r="P28" s="95"/>
-      <c r="Q28" s="95"/>
-      <c r="R28" s="95"/>
-      <c r="S28" s="95"/>
-      <c r="T28" s="95"/>
-      <c r="U28" s="95"/>
-      <c r="V28" s="95"/>
-      <c r="W28" s="95"/>
-      <c r="X28" s="95"/>
-      <c r="Y28" s="95"/>
-      <c r="Z28" s="95"/>
-      <c r="AA28" s="95"/>
-      <c r="AB28" s="95"/>
-      <c r="AC28" s="95"/>
-      <c r="AD28" s="95"/>
-      <c r="AE28" s="95"/>
-      <c r="AF28" s="95"/>
-      <c r="AG28" s="96"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="61"/>
+      <c r="E28" s="61"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="61"/>
+      <c r="H28" s="61"/>
+      <c r="I28" s="61"/>
+      <c r="J28" s="93"/>
+      <c r="K28" s="94"/>
+      <c r="L28" s="90"/>
+      <c r="M28" s="90"/>
+      <c r="N28" s="90"/>
+      <c r="O28" s="94"/>
+      <c r="P28" s="94"/>
+      <c r="Q28" s="94"/>
+      <c r="R28" s="94"/>
+      <c r="S28" s="94"/>
+      <c r="T28" s="94"/>
+      <c r="U28" s="94"/>
+      <c r="V28" s="94"/>
+      <c r="W28" s="94"/>
+      <c r="X28" s="94"/>
+      <c r="Y28" s="94"/>
+      <c r="Z28" s="94"/>
+      <c r="AA28" s="94"/>
+      <c r="AB28" s="94"/>
+      <c r="AC28" s="94"/>
+      <c r="AD28" s="94"/>
+      <c r="AE28" s="94"/>
+      <c r="AF28" s="94"/>
+      <c r="AG28" s="95"/>
     </row>
     <row r="29" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="93">
+      <c r="B29" s="92">
         <v>12</v>
       </c>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="62"/>
-      <c r="G29" s="62"/>
-      <c r="H29" s="62"/>
-      <c r="I29" s="62"/>
-      <c r="J29" s="94"/>
-      <c r="K29" s="95"/>
-      <c r="L29" s="91"/>
-      <c r="M29" s="91"/>
-      <c r="N29" s="91"/>
-      <c r="O29" s="95"/>
-      <c r="P29" s="95"/>
-      <c r="Q29" s="95"/>
-      <c r="R29" s="95"/>
-      <c r="S29" s="95"/>
-      <c r="T29" s="95"/>
-      <c r="U29" s="95"/>
-      <c r="V29" s="95"/>
-      <c r="W29" s="95"/>
-      <c r="X29" s="95"/>
-      <c r="Y29" s="95"/>
-      <c r="Z29" s="95"/>
-      <c r="AA29" s="95"/>
-      <c r="AB29" s="95"/>
-      <c r="AC29" s="95"/>
-      <c r="AD29" s="95"/>
-      <c r="AE29" s="95"/>
-      <c r="AF29" s="95"/>
-      <c r="AG29" s="96"/>
+      <c r="C29" s="61"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="61"/>
+      <c r="G29" s="61"/>
+      <c r="H29" s="61"/>
+      <c r="I29" s="61"/>
+      <c r="J29" s="93"/>
+      <c r="K29" s="94"/>
+      <c r="L29" s="90"/>
+      <c r="M29" s="90"/>
+      <c r="N29" s="90"/>
+      <c r="O29" s="94"/>
+      <c r="P29" s="94"/>
+      <c r="Q29" s="94"/>
+      <c r="R29" s="94"/>
+      <c r="S29" s="94"/>
+      <c r="T29" s="94"/>
+      <c r="U29" s="94"/>
+      <c r="V29" s="94"/>
+      <c r="W29" s="94"/>
+      <c r="X29" s="94"/>
+      <c r="Y29" s="94"/>
+      <c r="Z29" s="94"/>
+      <c r="AA29" s="94"/>
+      <c r="AB29" s="94"/>
+      <c r="AC29" s="94"/>
+      <c r="AD29" s="94"/>
+      <c r="AE29" s="94"/>
+      <c r="AF29" s="94"/>
+      <c r="AG29" s="95"/>
     </row>
     <row r="30" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="89">
+      <c r="B30" s="88">
         <v>13</v>
       </c>
-      <c r="C30" s="62"/>
-      <c r="D30" s="62"/>
-      <c r="E30" s="62"/>
-      <c r="F30" s="62"/>
-      <c r="G30" s="62"/>
-      <c r="H30" s="62"/>
-      <c r="I30" s="62"/>
-      <c r="J30" s="94"/>
-      <c r="K30" s="95"/>
-      <c r="L30" s="91"/>
-      <c r="M30" s="91"/>
-      <c r="N30" s="91"/>
-      <c r="O30" s="95"/>
-      <c r="P30" s="95"/>
-      <c r="Q30" s="95"/>
-      <c r="R30" s="95"/>
-      <c r="S30" s="95"/>
-      <c r="T30" s="95"/>
-      <c r="U30" s="95"/>
-      <c r="V30" s="95"/>
-      <c r="W30" s="95"/>
-      <c r="X30" s="95"/>
-      <c r="Y30" s="95"/>
-      <c r="Z30" s="95"/>
-      <c r="AA30" s="95"/>
-      <c r="AB30" s="95"/>
-      <c r="AC30" s="95"/>
-      <c r="AD30" s="95"/>
-      <c r="AE30" s="95"/>
-      <c r="AF30" s="95"/>
-      <c r="AG30" s="96"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="61"/>
+      <c r="F30" s="61"/>
+      <c r="G30" s="61"/>
+      <c r="H30" s="61"/>
+      <c r="I30" s="61"/>
+      <c r="J30" s="93"/>
+      <c r="K30" s="94"/>
+      <c r="L30" s="90"/>
+      <c r="M30" s="90"/>
+      <c r="N30" s="90"/>
+      <c r="O30" s="94"/>
+      <c r="P30" s="94"/>
+      <c r="Q30" s="94"/>
+      <c r="R30" s="94"/>
+      <c r="S30" s="94"/>
+      <c r="T30" s="94"/>
+      <c r="U30" s="94"/>
+      <c r="V30" s="94"/>
+      <c r="W30" s="94"/>
+      <c r="X30" s="94"/>
+      <c r="Y30" s="94"/>
+      <c r="Z30" s="94"/>
+      <c r="AA30" s="94"/>
+      <c r="AB30" s="94"/>
+      <c r="AC30" s="94"/>
+      <c r="AD30" s="94"/>
+      <c r="AE30" s="94"/>
+      <c r="AF30" s="94"/>
+      <c r="AG30" s="95"/>
     </row>
     <row r="31" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="93">
+      <c r="B31" s="92">
         <v>14</v>
       </c>
-      <c r="C31" s="62"/>
-      <c r="D31" s="62"/>
-      <c r="E31" s="62"/>
-      <c r="F31" s="62"/>
-      <c r="G31" s="62"/>
-      <c r="H31" s="62"/>
-      <c r="I31" s="62"/>
-      <c r="J31" s="94"/>
-      <c r="K31" s="95"/>
-      <c r="L31" s="91"/>
-      <c r="M31" s="91"/>
-      <c r="N31" s="91"/>
-      <c r="O31" s="95"/>
-      <c r="P31" s="95"/>
-      <c r="Q31" s="95"/>
-      <c r="R31" s="95"/>
-      <c r="S31" s="95"/>
-      <c r="T31" s="95"/>
-      <c r="U31" s="95"/>
-      <c r="V31" s="95"/>
-      <c r="W31" s="95"/>
-      <c r="X31" s="95"/>
-      <c r="Y31" s="95"/>
-      <c r="Z31" s="95"/>
-      <c r="AA31" s="95"/>
-      <c r="AB31" s="95"/>
-      <c r="AC31" s="95"/>
-      <c r="AD31" s="95"/>
-      <c r="AE31" s="95"/>
-      <c r="AF31" s="95"/>
-      <c r="AG31" s="96"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="61"/>
+      <c r="G31" s="61"/>
+      <c r="H31" s="61"/>
+      <c r="I31" s="61"/>
+      <c r="J31" s="93"/>
+      <c r="K31" s="94"/>
+      <c r="L31" s="90"/>
+      <c r="M31" s="90"/>
+      <c r="N31" s="90"/>
+      <c r="O31" s="94"/>
+      <c r="P31" s="94"/>
+      <c r="Q31" s="94"/>
+      <c r="R31" s="94"/>
+      <c r="S31" s="94"/>
+      <c r="T31" s="94"/>
+      <c r="U31" s="94"/>
+      <c r="V31" s="94"/>
+      <c r="W31" s="94"/>
+      <c r="X31" s="94"/>
+      <c r="Y31" s="94"/>
+      <c r="Z31" s="94"/>
+      <c r="AA31" s="94"/>
+      <c r="AB31" s="94"/>
+      <c r="AC31" s="94"/>
+      <c r="AD31" s="94"/>
+      <c r="AE31" s="94"/>
+      <c r="AF31" s="94"/>
+      <c r="AG31" s="95"/>
     </row>
     <row r="32" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="93">
+      <c r="B32" s="92">
         <v>15</v>
       </c>
-      <c r="C32" s="62"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="62"/>
-      <c r="F32" s="62"/>
-      <c r="G32" s="62"/>
-      <c r="H32" s="62"/>
-      <c r="I32" s="62"/>
-      <c r="J32" s="94"/>
-      <c r="K32" s="95"/>
-      <c r="L32" s="91"/>
-      <c r="M32" s="91"/>
-      <c r="N32" s="91"/>
-      <c r="O32" s="95"/>
-      <c r="P32" s="95"/>
-      <c r="Q32" s="95"/>
-      <c r="R32" s="95"/>
-      <c r="S32" s="95"/>
-      <c r="T32" s="95"/>
-      <c r="U32" s="95"/>
-      <c r="V32" s="95"/>
-      <c r="W32" s="95"/>
-      <c r="X32" s="95"/>
-      <c r="Y32" s="95"/>
-      <c r="Z32" s="95"/>
-      <c r="AA32" s="95"/>
-      <c r="AB32" s="95"/>
-      <c r="AC32" s="95"/>
-      <c r="AD32" s="95"/>
-      <c r="AE32" s="95"/>
-      <c r="AF32" s="95"/>
-      <c r="AG32" s="96"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="61"/>
+      <c r="E32" s="61"/>
+      <c r="F32" s="61"/>
+      <c r="G32" s="61"/>
+      <c r="H32" s="61"/>
+      <c r="I32" s="61"/>
+      <c r="J32" s="93"/>
+      <c r="K32" s="94"/>
+      <c r="L32" s="90"/>
+      <c r="M32" s="90"/>
+      <c r="N32" s="90"/>
+      <c r="O32" s="94"/>
+      <c r="P32" s="94"/>
+      <c r="Q32" s="94"/>
+      <c r="R32" s="94"/>
+      <c r="S32" s="94"/>
+      <c r="T32" s="94"/>
+      <c r="U32" s="94"/>
+      <c r="V32" s="94"/>
+      <c r="W32" s="94"/>
+      <c r="X32" s="94"/>
+      <c r="Y32" s="94"/>
+      <c r="Z32" s="94"/>
+      <c r="AA32" s="94"/>
+      <c r="AB32" s="94"/>
+      <c r="AC32" s="94"/>
+      <c r="AD32" s="94"/>
+      <c r="AE32" s="94"/>
+      <c r="AF32" s="94"/>
+      <c r="AG32" s="95"/>
     </row>
     <row r="33" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="89">
+      <c r="B33" s="88">
         <v>16</v>
       </c>
-      <c r="C33" s="62"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="62"/>
-      <c r="F33" s="62"/>
-      <c r="G33" s="62"/>
-      <c r="H33" s="62"/>
-      <c r="I33" s="62"/>
-      <c r="J33" s="94"/>
-      <c r="K33" s="95"/>
-      <c r="L33" s="91"/>
-      <c r="M33" s="91"/>
-      <c r="N33" s="91"/>
-      <c r="O33" s="95"/>
-      <c r="P33" s="95"/>
-      <c r="Q33" s="95"/>
-      <c r="R33" s="95"/>
-      <c r="S33" s="95"/>
-      <c r="T33" s="95"/>
-      <c r="U33" s="95"/>
-      <c r="V33" s="95"/>
-      <c r="W33" s="95"/>
-      <c r="X33" s="95"/>
-      <c r="Y33" s="95"/>
-      <c r="Z33" s="95"/>
-      <c r="AA33" s="95"/>
-      <c r="AB33" s="95"/>
-      <c r="AC33" s="95"/>
-      <c r="AD33" s="95"/>
-      <c r="AE33" s="95"/>
-      <c r="AF33" s="95"/>
-      <c r="AG33" s="96"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="61"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="61"/>
+      <c r="H33" s="61"/>
+      <c r="I33" s="61"/>
+      <c r="J33" s="93"/>
+      <c r="K33" s="94"/>
+      <c r="L33" s="90"/>
+      <c r="M33" s="90"/>
+      <c r="N33" s="90"/>
+      <c r="O33" s="94"/>
+      <c r="P33" s="94"/>
+      <c r="Q33" s="94"/>
+      <c r="R33" s="94"/>
+      <c r="S33" s="94"/>
+      <c r="T33" s="94"/>
+      <c r="U33" s="94"/>
+      <c r="V33" s="94"/>
+      <c r="W33" s="94"/>
+      <c r="X33" s="94"/>
+      <c r="Y33" s="94"/>
+      <c r="Z33" s="94"/>
+      <c r="AA33" s="94"/>
+      <c r="AB33" s="94"/>
+      <c r="AC33" s="94"/>
+      <c r="AD33" s="94"/>
+      <c r="AE33" s="94"/>
+      <c r="AF33" s="94"/>
+      <c r="AG33" s="95"/>
     </row>
     <row r="34" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="93">
+      <c r="B34" s="92">
         <v>17</v>
       </c>
-      <c r="C34" s="62"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="62"/>
-      <c r="G34" s="62"/>
-      <c r="H34" s="62"/>
-      <c r="I34" s="62"/>
-      <c r="J34" s="97"/>
-      <c r="K34" s="97"/>
-      <c r="L34" s="91"/>
-      <c r="M34" s="91"/>
-      <c r="N34" s="91"/>
-      <c r="O34" s="95"/>
-      <c r="P34" s="95"/>
-      <c r="Q34" s="95"/>
-      <c r="R34" s="95"/>
-      <c r="S34" s="95"/>
-      <c r="T34" s="95"/>
-      <c r="U34" s="95"/>
-      <c r="V34" s="95"/>
-      <c r="W34" s="95"/>
-      <c r="X34" s="95"/>
-      <c r="Y34" s="95"/>
-      <c r="Z34" s="95"/>
-      <c r="AA34" s="95"/>
-      <c r="AB34" s="95"/>
-      <c r="AC34" s="95"/>
-      <c r="AD34" s="95"/>
-      <c r="AE34" s="95"/>
-      <c r="AF34" s="95"/>
-      <c r="AG34" s="96"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="61"/>
+      <c r="E34" s="61"/>
+      <c r="F34" s="61"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="61"/>
+      <c r="I34" s="61"/>
+      <c r="J34" s="96"/>
+      <c r="K34" s="96"/>
+      <c r="L34" s="90"/>
+      <c r="M34" s="90"/>
+      <c r="N34" s="90"/>
+      <c r="O34" s="94"/>
+      <c r="P34" s="94"/>
+      <c r="Q34" s="94"/>
+      <c r="R34" s="94"/>
+      <c r="S34" s="94"/>
+      <c r="T34" s="94"/>
+      <c r="U34" s="94"/>
+      <c r="V34" s="94"/>
+      <c r="W34" s="94"/>
+      <c r="X34" s="94"/>
+      <c r="Y34" s="94"/>
+      <c r="Z34" s="94"/>
+      <c r="AA34" s="94"/>
+      <c r="AB34" s="94"/>
+      <c r="AC34" s="94"/>
+      <c r="AD34" s="94"/>
+      <c r="AE34" s="94"/>
+      <c r="AF34" s="94"/>
+      <c r="AG34" s="95"/>
     </row>
     <row r="35" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="93">
+      <c r="B35" s="92">
         <v>18</v>
       </c>
-      <c r="C35" s="62"/>
-      <c r="D35" s="62"/>
-      <c r="E35" s="62"/>
-      <c r="F35" s="62"/>
-      <c r="G35" s="62"/>
-      <c r="H35" s="62"/>
-      <c r="I35" s="62"/>
-      <c r="J35" s="97"/>
-      <c r="K35" s="97"/>
-      <c r="L35" s="91"/>
-      <c r="M35" s="91"/>
-      <c r="N35" s="91"/>
-      <c r="O35" s="95"/>
-      <c r="P35" s="95"/>
-      <c r="Q35" s="95"/>
-      <c r="R35" s="95"/>
-      <c r="S35" s="95"/>
-      <c r="T35" s="95"/>
-      <c r="U35" s="95"/>
-      <c r="V35" s="95"/>
-      <c r="W35" s="95"/>
-      <c r="X35" s="95"/>
-      <c r="Y35" s="95"/>
-      <c r="Z35" s="95"/>
-      <c r="AA35" s="95"/>
-      <c r="AB35" s="95"/>
-      <c r="AC35" s="95"/>
-      <c r="AD35" s="95"/>
-      <c r="AE35" s="95"/>
-      <c r="AF35" s="95"/>
-      <c r="AG35" s="96"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="61"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="61"/>
+      <c r="H35" s="61"/>
+      <c r="I35" s="61"/>
+      <c r="J35" s="96"/>
+      <c r="K35" s="96"/>
+      <c r="L35" s="90"/>
+      <c r="M35" s="90"/>
+      <c r="N35" s="90"/>
+      <c r="O35" s="94"/>
+      <c r="P35" s="94"/>
+      <c r="Q35" s="94"/>
+      <c r="R35" s="94"/>
+      <c r="S35" s="94"/>
+      <c r="T35" s="94"/>
+      <c r="U35" s="94"/>
+      <c r="V35" s="94"/>
+      <c r="W35" s="94"/>
+      <c r="X35" s="94"/>
+      <c r="Y35" s="94"/>
+      <c r="Z35" s="94"/>
+      <c r="AA35" s="94"/>
+      <c r="AB35" s="94"/>
+      <c r="AC35" s="94"/>
+      <c r="AD35" s="94"/>
+      <c r="AE35" s="94"/>
+      <c r="AF35" s="94"/>
+      <c r="AG35" s="95"/>
     </row>
     <row r="36" spans="2:33" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="89">
+      <c r="B36" s="88">
         <v>19</v>
       </c>
-      <c r="C36" s="62"/>
-      <c r="D36" s="65"/>
-      <c r="E36" s="65"/>
-      <c r="F36" s="65"/>
-      <c r="G36" s="65"/>
-      <c r="H36" s="65"/>
-      <c r="I36" s="65"/>
-      <c r="J36" s="98"/>
-      <c r="K36" s="98"/>
-      <c r="L36" s="91"/>
-      <c r="M36" s="120"/>
-      <c r="N36" s="120"/>
-      <c r="O36" s="99"/>
-      <c r="P36" s="99"/>
-      <c r="Q36" s="99"/>
-      <c r="R36" s="99"/>
-      <c r="S36" s="99"/>
-      <c r="T36" s="99"/>
-      <c r="U36" s="99"/>
-      <c r="V36" s="99"/>
-      <c r="W36" s="99"/>
-      <c r="X36" s="99"/>
-      <c r="Y36" s="99"/>
-      <c r="Z36" s="99"/>
-      <c r="AA36" s="99"/>
-      <c r="AB36" s="99"/>
-      <c r="AC36" s="99"/>
-      <c r="AD36" s="99"/>
-      <c r="AE36" s="99"/>
-      <c r="AF36" s="99"/>
-      <c r="AG36" s="100"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="64"/>
+      <c r="G36" s="64"/>
+      <c r="H36" s="64"/>
+      <c r="I36" s="64"/>
+      <c r="J36" s="97"/>
+      <c r="K36" s="97"/>
+      <c r="L36" s="90"/>
+      <c r="M36" s="119"/>
+      <c r="N36" s="119"/>
+      <c r="O36" s="98"/>
+      <c r="P36" s="98"/>
+      <c r="Q36" s="98"/>
+      <c r="R36" s="98"/>
+      <c r="S36" s="98"/>
+      <c r="T36" s="98"/>
+      <c r="U36" s="98"/>
+      <c r="V36" s="98"/>
+      <c r="W36" s="98"/>
+      <c r="X36" s="98"/>
+      <c r="Y36" s="98"/>
+      <c r="Z36" s="98"/>
+      <c r="AA36" s="98"/>
+      <c r="AB36" s="98"/>
+      <c r="AC36" s="98"/>
+      <c r="AD36" s="98"/>
+      <c r="AE36" s="98"/>
+      <c r="AF36" s="98"/>
+      <c r="AG36" s="99"/>
     </row>
     <row r="37" spans="2:33" ht="26.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="101">
+      <c r="B37" s="100">
         <v>20</v>
       </c>
-      <c r="C37" s="66"/>
-      <c r="D37" s="66"/>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
-      <c r="G37" s="66"/>
-      <c r="H37" s="66"/>
-      <c r="I37" s="66"/>
-      <c r="J37" s="102"/>
-      <c r="K37" s="102"/>
-      <c r="L37" s="103"/>
-      <c r="M37" s="103"/>
-      <c r="N37" s="103"/>
-      <c r="O37" s="104"/>
-      <c r="P37" s="104"/>
-      <c r="Q37" s="104"/>
-      <c r="R37" s="104"/>
-      <c r="S37" s="104"/>
-      <c r="T37" s="104"/>
-      <c r="U37" s="104"/>
-      <c r="V37" s="104"/>
-      <c r="W37" s="104"/>
-      <c r="X37" s="104"/>
-      <c r="Y37" s="104"/>
-      <c r="Z37" s="104"/>
-      <c r="AA37" s="104"/>
-      <c r="AB37" s="104"/>
-      <c r="AC37" s="104"/>
-      <c r="AD37" s="104"/>
-      <c r="AE37" s="104"/>
-      <c r="AF37" s="104"/>
-      <c r="AG37" s="105"/>
+      <c r="C37" s="65"/>
+      <c r="D37" s="65"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
+      <c r="G37" s="65"/>
+      <c r="H37" s="65"/>
+      <c r="I37" s="65"/>
+      <c r="J37" s="101"/>
+      <c r="K37" s="101"/>
+      <c r="L37" s="102"/>
+      <c r="M37" s="102"/>
+      <c r="N37" s="102"/>
+      <c r="O37" s="103"/>
+      <c r="P37" s="103"/>
+      <c r="Q37" s="103"/>
+      <c r="R37" s="103"/>
+      <c r="S37" s="103"/>
+      <c r="T37" s="103"/>
+      <c r="U37" s="103"/>
+      <c r="V37" s="103"/>
+      <c r="W37" s="103"/>
+      <c r="X37" s="103"/>
+      <c r="Y37" s="103"/>
+      <c r="Z37" s="103"/>
+      <c r="AA37" s="103"/>
+      <c r="AB37" s="103"/>
+      <c r="AC37" s="103"/>
+      <c r="AD37" s="103"/>
+      <c r="AE37" s="103"/>
+      <c r="AF37" s="103"/>
+      <c r="AG37" s="104"/>
     </row>
     <row r="38" spans="2:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="141" t="s">
+      <c r="B38" s="140" t="s">
         <v>80</v>
       </c>
-      <c r="C38" s="106"/>
-      <c r="D38" s="106"/>
-      <c r="E38" s="106"/>
-      <c r="F38" s="106"/>
-      <c r="G38" s="106"/>
-      <c r="H38" s="106"/>
-      <c r="I38" s="106"/>
-      <c r="J38" s="106"/>
-      <c r="K38" s="106"/>
-      <c r="L38" s="106"/>
-      <c r="M38" s="106"/>
-      <c r="N38" s="106"/>
-      <c r="O38" s="107"/>
-      <c r="P38" s="107"/>
-      <c r="Q38" s="107"/>
-      <c r="R38" s="107"/>
-      <c r="S38" s="107"/>
-      <c r="T38" s="107"/>
-      <c r="U38" s="107"/>
-      <c r="V38" s="107"/>
-      <c r="W38" s="107"/>
-      <c r="X38" s="107"/>
-      <c r="Y38" s="107"/>
-      <c r="Z38" s="107"/>
-      <c r="AA38" s="107"/>
-      <c r="AB38" s="107"/>
-      <c r="AC38" s="107"/>
-      <c r="AD38" s="107"/>
-      <c r="AE38" s="107"/>
-      <c r="AF38" s="107"/>
-      <c r="AG38" s="106"/>
+      <c r="C38" s="105"/>
+      <c r="D38" s="105"/>
+      <c r="E38" s="105"/>
+      <c r="F38" s="105"/>
+      <c r="G38" s="105"/>
+      <c r="H38" s="105"/>
+      <c r="I38" s="105"/>
+      <c r="J38" s="105"/>
+      <c r="K38" s="105"/>
+      <c r="L38" s="105"/>
+      <c r="M38" s="105"/>
+      <c r="N38" s="105"/>
+      <c r="O38" s="106"/>
+      <c r="P38" s="106"/>
+      <c r="Q38" s="106"/>
+      <c r="R38" s="106"/>
+      <c r="S38" s="106"/>
+      <c r="T38" s="106"/>
+      <c r="U38" s="106"/>
+      <c r="V38" s="106"/>
+      <c r="W38" s="106"/>
+      <c r="X38" s="106"/>
+      <c r="Y38" s="106"/>
+      <c r="Z38" s="106"/>
+      <c r="AA38" s="106"/>
+      <c r="AB38" s="106"/>
+      <c r="AC38" s="106"/>
+      <c r="AD38" s="106"/>
+      <c r="AE38" s="106"/>
+      <c r="AF38" s="106"/>
+      <c r="AG38" s="105"/>
     </row>
     <row r="39" spans="2:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="106"/>
-      <c r="C39" s="106"/>
-      <c r="D39" s="106"/>
-      <c r="E39" s="106"/>
-      <c r="F39" s="106"/>
-      <c r="G39" s="106"/>
-      <c r="H39" s="106"/>
-      <c r="I39" s="106"/>
-      <c r="J39" s="106"/>
-      <c r="K39" s="106"/>
-      <c r="L39" s="106"/>
-      <c r="M39" s="106"/>
-      <c r="N39" s="106"/>
-      <c r="O39" s="107"/>
-      <c r="P39" s="107"/>
-      <c r="Q39" s="107"/>
-      <c r="R39" s="107"/>
-      <c r="S39" s="107"/>
-      <c r="T39" s="107"/>
-      <c r="U39" s="107"/>
-      <c r="V39" s="107"/>
-      <c r="W39" s="107"/>
-      <c r="X39" s="107"/>
-      <c r="Y39" s="107"/>
-      <c r="Z39" s="107"/>
-      <c r="AA39" s="107"/>
-      <c r="AB39" s="107"/>
-      <c r="AC39" s="107"/>
-      <c r="AD39" s="107"/>
-      <c r="AE39" s="107"/>
-      <c r="AF39" s="107"/>
-      <c r="AG39" s="106"/>
+      <c r="B39" s="105"/>
+      <c r="C39" s="105"/>
+      <c r="D39" s="105"/>
+      <c r="E39" s="105"/>
+      <c r="F39" s="105"/>
+      <c r="G39" s="105"/>
+      <c r="H39" s="105"/>
+      <c r="I39" s="105"/>
+      <c r="J39" s="105"/>
+      <c r="K39" s="105"/>
+      <c r="L39" s="105"/>
+      <c r="M39" s="105"/>
+      <c r="N39" s="105"/>
+      <c r="O39" s="106"/>
+      <c r="P39" s="106"/>
+      <c r="Q39" s="106"/>
+      <c r="R39" s="106"/>
+      <c r="S39" s="106"/>
+      <c r="T39" s="106"/>
+      <c r="U39" s="106"/>
+      <c r="V39" s="106"/>
+      <c r="W39" s="106"/>
+      <c r="X39" s="106"/>
+      <c r="Y39" s="106"/>
+      <c r="Z39" s="106"/>
+      <c r="AA39" s="106"/>
+      <c r="AB39" s="106"/>
+      <c r="AC39" s="106"/>
+      <c r="AD39" s="106"/>
+      <c r="AE39" s="106"/>
+      <c r="AF39" s="106"/>
+      <c r="AG39" s="105"/>
     </row>
     <row r="40" spans="2:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="106"/>
-      <c r="C40" s="106"/>
-      <c r="D40" s="106"/>
-      <c r="E40" s="106"/>
-      <c r="F40" s="106"/>
-      <c r="G40" s="106"/>
-      <c r="H40" s="106"/>
-      <c r="I40" s="106"/>
-      <c r="J40" s="106"/>
-      <c r="K40" s="106"/>
-      <c r="L40" s="106"/>
-      <c r="M40" s="106"/>
-      <c r="N40" s="106"/>
-      <c r="O40" s="107"/>
-      <c r="P40" s="107"/>
-      <c r="Q40" s="107"/>
-      <c r="R40" s="107"/>
-      <c r="S40" s="107"/>
-      <c r="T40" s="107"/>
-      <c r="U40" s="107"/>
-      <c r="V40" s="107"/>
-      <c r="W40" s="107"/>
-      <c r="X40" s="107"/>
-      <c r="Y40" s="107"/>
-      <c r="Z40" s="107"/>
-      <c r="AA40" s="107"/>
-      <c r="AB40" s="107"/>
-      <c r="AC40" s="107"/>
-      <c r="AD40" s="107"/>
-      <c r="AE40" s="107"/>
-      <c r="AF40" s="107"/>
-      <c r="AG40" s="106"/>
+      <c r="B40" s="105"/>
+      <c r="C40" s="105"/>
+      <c r="D40" s="105"/>
+      <c r="E40" s="105"/>
+      <c r="F40" s="105"/>
+      <c r="G40" s="105"/>
+      <c r="H40" s="105"/>
+      <c r="I40" s="105"/>
+      <c r="J40" s="105"/>
+      <c r="K40" s="105"/>
+      <c r="L40" s="105"/>
+      <c r="M40" s="105"/>
+      <c r="N40" s="105"/>
+      <c r="O40" s="106"/>
+      <c r="P40" s="106"/>
+      <c r="Q40" s="106"/>
+      <c r="R40" s="106"/>
+      <c r="S40" s="106"/>
+      <c r="T40" s="106"/>
+      <c r="U40" s="106"/>
+      <c r="V40" s="106"/>
+      <c r="W40" s="106"/>
+      <c r="X40" s="106"/>
+      <c r="Y40" s="106"/>
+      <c r="Z40" s="106"/>
+      <c r="AA40" s="106"/>
+      <c r="AB40" s="106"/>
+      <c r="AC40" s="106"/>
+      <c r="AD40" s="106"/>
+      <c r="AE40" s="106"/>
+      <c r="AF40" s="106"/>
+      <c r="AG40" s="105"/>
     </row>
     <row r="41" spans="2:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="106"/>
-      <c r="C41" s="67"/>
-      <c r="D41" s="67"/>
-      <c r="E41" s="67"/>
-      <c r="F41" s="106"/>
-      <c r="G41" s="106"/>
-      <c r="H41" s="106"/>
-      <c r="I41" s="106"/>
-      <c r="J41" s="106"/>
-      <c r="K41" s="106"/>
-      <c r="L41" s="106"/>
-      <c r="M41" s="106"/>
-      <c r="N41" s="106"/>
-      <c r="O41" s="107"/>
-      <c r="P41" s="107"/>
-      <c r="Q41" s="107"/>
-      <c r="R41" s="107"/>
-      <c r="S41" s="107"/>
-      <c r="T41" s="107"/>
-      <c r="U41" s="107"/>
-      <c r="V41" s="107"/>
-      <c r="W41" s="107"/>
-      <c r="X41" s="107"/>
-      <c r="Y41" s="107"/>
-      <c r="Z41" s="107"/>
-      <c r="AA41" s="107"/>
-      <c r="AB41" s="107"/>
-      <c r="AC41" s="107"/>
-      <c r="AD41" s="107"/>
-      <c r="AE41" s="107"/>
-      <c r="AF41" s="107"/>
-      <c r="AG41" s="106"/>
+      <c r="B41" s="105"/>
+      <c r="C41" s="66"/>
+      <c r="D41" s="66"/>
+      <c r="E41" s="66"/>
+      <c r="F41" s="105"/>
+      <c r="G41" s="105"/>
+      <c r="H41" s="105"/>
+      <c r="I41" s="105"/>
+      <c r="J41" s="105"/>
+      <c r="K41" s="105"/>
+      <c r="L41" s="105"/>
+      <c r="M41" s="105"/>
+      <c r="N41" s="105"/>
+      <c r="O41" s="106"/>
+      <c r="P41" s="106"/>
+      <c r="Q41" s="106"/>
+      <c r="R41" s="106"/>
+      <c r="S41" s="106"/>
+      <c r="T41" s="106"/>
+      <c r="U41" s="106"/>
+      <c r="V41" s="106"/>
+      <c r="W41" s="106"/>
+      <c r="X41" s="106"/>
+      <c r="Y41" s="106"/>
+      <c r="Z41" s="106"/>
+      <c r="AA41" s="106"/>
+      <c r="AB41" s="106"/>
+      <c r="AC41" s="106"/>
+      <c r="AD41" s="106"/>
+      <c r="AE41" s="106"/>
+      <c r="AF41" s="106"/>
+      <c r="AG41" s="105"/>
     </row>
     <row r="42" spans="2:33" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="67"/>
-      <c r="C42" s="67"/>
-      <c r="D42" s="67"/>
-      <c r="E42" s="67"/>
-      <c r="F42" s="157" t="s">
+      <c r="B42" s="66"/>
+      <c r="C42" s="66"/>
+      <c r="D42" s="66"/>
+      <c r="E42" s="66"/>
+      <c r="F42" s="155" t="s">
         <v>48</v>
       </c>
-      <c r="G42" s="157"/>
-      <c r="H42" s="68"/>
-      <c r="I42" s="69"/>
-      <c r="J42" s="106"/>
-      <c r="K42" s="138"/>
-      <c r="L42" s="138"/>
-      <c r="M42" s="138"/>
-      <c r="N42" s="138"/>
-      <c r="O42" s="68" t="s">
+      <c r="G42" s="155"/>
+      <c r="H42" s="67"/>
+      <c r="I42" s="68"/>
+      <c r="J42" s="105"/>
+      <c r="K42" s="137"/>
+      <c r="L42" s="137"/>
+      <c r="M42" s="137"/>
+      <c r="N42" s="137"/>
+      <c r="O42" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="P42" s="77"/>
-      <c r="Q42" s="77"/>
-      <c r="R42" s="77"/>
-      <c r="S42" s="77"/>
-      <c r="T42" s="77"/>
-      <c r="U42" s="77"/>
-      <c r="V42" s="77"/>
-      <c r="W42" s="77"/>
-      <c r="X42" s="138"/>
-      <c r="Y42" s="138"/>
-      <c r="Z42" s="138"/>
-      <c r="AA42" s="138"/>
-      <c r="AB42" s="138"/>
-      <c r="AC42" s="138"/>
-      <c r="AD42" s="138"/>
-      <c r="AE42" s="138"/>
-      <c r="AF42" s="138"/>
-      <c r="AG42" s="138"/>
+      <c r="P42" s="76"/>
+      <c r="Q42" s="76"/>
+      <c r="R42" s="76"/>
+      <c r="S42" s="76"/>
+      <c r="T42" s="76"/>
+      <c r="U42" s="76"/>
+      <c r="V42" s="76"/>
+      <c r="W42" s="76"/>
+      <c r="X42" s="137"/>
+      <c r="Y42" s="137"/>
+      <c r="Z42" s="137"/>
+      <c r="AA42" s="137"/>
+      <c r="AB42" s="137"/>
+      <c r="AC42" s="137"/>
+      <c r="AD42" s="137"/>
+      <c r="AE42" s="137"/>
+      <c r="AF42" s="137"/>
+      <c r="AG42" s="137"/>
     </row>
     <row r="43" spans="2:33" ht="42.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="67"/>
-      <c r="C43" s="67"/>
-      <c r="D43" s="67"/>
-      <c r="E43" s="67"/>
-      <c r="F43" s="75"/>
-      <c r="G43" s="69"/>
-      <c r="H43" s="69"/>
-      <c r="I43" s="69"/>
-      <c r="J43" s="106"/>
-      <c r="K43" s="76"/>
-      <c r="L43" s="76"/>
-      <c r="M43" s="76"/>
-      <c r="N43" s="76"/>
-      <c r="O43" s="76"/>
-      <c r="P43" s="76"/>
-      <c r="Q43" s="76"/>
-      <c r="R43" s="76"/>
-      <c r="S43" s="76"/>
-      <c r="T43" s="76"/>
-      <c r="U43" s="76"/>
-      <c r="V43" s="158" t="s">
+      <c r="B43" s="66"/>
+      <c r="C43" s="66"/>
+      <c r="D43" s="66"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="74"/>
+      <c r="G43" s="68"/>
+      <c r="H43" s="68"/>
+      <c r="I43" s="68"/>
+      <c r="J43" s="105"/>
+      <c r="K43" s="75"/>
+      <c r="L43" s="75"/>
+      <c r="M43" s="75"/>
+      <c r="N43" s="75"/>
+      <c r="O43" s="75"/>
+      <c r="P43" s="75"/>
+      <c r="Q43" s="75"/>
+      <c r="R43" s="75"/>
+      <c r="S43" s="75"/>
+      <c r="T43" s="75"/>
+      <c r="U43" s="75"/>
+      <c r="V43" s="156" t="s">
         <v>49</v>
       </c>
-      <c r="W43" s="158"/>
-      <c r="X43" s="158"/>
-      <c r="Y43" s="158"/>
-      <c r="Z43" s="140" t="s">
+      <c r="W43" s="156"/>
+      <c r="X43" s="156"/>
+      <c r="Y43" s="156"/>
+      <c r="Z43" s="139" t="s">
         <v>71</v>
       </c>
-      <c r="AA43" s="139"/>
-      <c r="AB43" s="76"/>
-      <c r="AC43" s="76"/>
-      <c r="AD43" s="76"/>
+      <c r="AA43" s="138"/>
+      <c r="AB43" s="75"/>
+      <c r="AC43" s="75"/>
+      <c r="AD43" s="75"/>
     </row>
     <row r="44" spans="2:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B44" s="5" t="s">
@@ -4094,73 +4094,73 @@
       </c>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
-      <c r="E44" s="106"/>
-      <c r="F44" s="106"/>
-      <c r="G44" s="106"/>
-      <c r="H44" s="106"/>
-      <c r="I44" s="106"/>
-      <c r="J44" s="106"/>
-      <c r="K44" s="106"/>
-      <c r="L44" s="106"/>
-      <c r="M44" s="106"/>
-      <c r="N44" s="106"/>
-      <c r="O44" s="107"/>
-      <c r="P44" s="107"/>
-      <c r="Q44" s="107"/>
-      <c r="R44" s="107"/>
-      <c r="S44" s="107"/>
-      <c r="T44" s="107"/>
-      <c r="U44" s="107"/>
-      <c r="V44" s="107"/>
-      <c r="W44" s="107"/>
-      <c r="X44" s="107"/>
-      <c r="Y44" s="107"/>
-      <c r="Z44" s="107"/>
-      <c r="AA44" s="107"/>
-      <c r="AB44" s="107"/>
-      <c r="AC44" s="107"/>
-      <c r="AD44" s="107"/>
-      <c r="AE44" s="107"/>
-      <c r="AF44" s="107"/>
-      <c r="AG44" s="106"/>
+      <c r="E44" s="105"/>
+      <c r="F44" s="105"/>
+      <c r="G44" s="105"/>
+      <c r="H44" s="105"/>
+      <c r="I44" s="105"/>
+      <c r="J44" s="105"/>
+      <c r="K44" s="105"/>
+      <c r="L44" s="105"/>
+      <c r="M44" s="105"/>
+      <c r="N44" s="105"/>
+      <c r="O44" s="106"/>
+      <c r="P44" s="106"/>
+      <c r="Q44" s="106"/>
+      <c r="R44" s="106"/>
+      <c r="S44" s="106"/>
+      <c r="T44" s="106"/>
+      <c r="U44" s="106"/>
+      <c r="V44" s="106"/>
+      <c r="W44" s="106"/>
+      <c r="X44" s="106"/>
+      <c r="Y44" s="106"/>
+      <c r="Z44" s="106"/>
+      <c r="AA44" s="106"/>
+      <c r="AB44" s="106"/>
+      <c r="AC44" s="106"/>
+      <c r="AD44" s="106"/>
+      <c r="AE44" s="106"/>
+      <c r="AF44" s="106"/>
+      <c r="AG44" s="105"/>
     </row>
     <row r="45" spans="2:33" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="147" t="s">
+      <c r="B45" s="145" t="s">
         <v>51</v>
       </c>
-      <c r="C45" s="147"/>
+      <c r="C45" s="145"/>
       <c r="D45" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="E45" s="108"/>
-      <c r="F45" s="108"/>
-      <c r="G45" s="108"/>
-      <c r="H45" s="108"/>
-      <c r="I45" s="108"/>
-      <c r="J45" s="108"/>
-      <c r="K45" s="108"/>
-      <c r="L45" s="108"/>
-      <c r="M45" s="108"/>
-      <c r="N45" s="108"/>
-      <c r="O45" s="108"/>
-      <c r="P45" s="108"/>
-      <c r="Q45" s="108"/>
-      <c r="R45" s="108"/>
-      <c r="S45" s="108"/>
-      <c r="T45" s="108"/>
-      <c r="U45" s="108"/>
-      <c r="V45" s="108"/>
-      <c r="W45" s="108"/>
-      <c r="X45" s="108"/>
-      <c r="Y45" s="108"/>
-      <c r="Z45" s="108"/>
-      <c r="AA45" s="108"/>
-      <c r="AB45" s="108"/>
-      <c r="AC45" s="108"/>
-      <c r="AD45" s="108"/>
-      <c r="AE45" s="108"/>
-      <c r="AF45" s="108"/>
-      <c r="AG45" s="108"/>
+      <c r="E45" s="107"/>
+      <c r="F45" s="107"/>
+      <c r="G45" s="107"/>
+      <c r="H45" s="107"/>
+      <c r="I45" s="107"/>
+      <c r="J45" s="107"/>
+      <c r="K45" s="107"/>
+      <c r="L45" s="107"/>
+      <c r="M45" s="107"/>
+      <c r="N45" s="107"/>
+      <c r="O45" s="107"/>
+      <c r="P45" s="107"/>
+      <c r="Q45" s="107"/>
+      <c r="R45" s="107"/>
+      <c r="S45" s="107"/>
+      <c r="T45" s="107"/>
+      <c r="U45" s="107"/>
+      <c r="V45" s="107"/>
+      <c r="W45" s="107"/>
+      <c r="X45" s="107"/>
+      <c r="Y45" s="107"/>
+      <c r="Z45" s="107"/>
+      <c r="AA45" s="107"/>
+      <c r="AB45" s="107"/>
+      <c r="AC45" s="107"/>
+      <c r="AD45" s="107"/>
+      <c r="AE45" s="107"/>
+      <c r="AF45" s="107"/>
+      <c r="AG45" s="107"/>
     </row>
     <row r="46" spans="2:33" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B46" s="6"/>
@@ -4168,35 +4168,35 @@
       <c r="D46" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E46" s="106"/>
-      <c r="F46" s="106"/>
-      <c r="G46" s="106"/>
-      <c r="H46" s="106"/>
-      <c r="I46" s="106"/>
-      <c r="J46" s="106"/>
-      <c r="K46" s="106"/>
-      <c r="L46" s="106"/>
-      <c r="M46" s="106"/>
-      <c r="N46" s="106"/>
-      <c r="O46" s="107"/>
-      <c r="P46" s="107"/>
-      <c r="Q46" s="107"/>
-      <c r="R46" s="107"/>
-      <c r="S46" s="107"/>
-      <c r="T46" s="107"/>
-      <c r="U46" s="107"/>
-      <c r="V46" s="107"/>
-      <c r="W46" s="107"/>
-      <c r="X46" s="107"/>
-      <c r="Y46" s="107"/>
-      <c r="Z46" s="107"/>
-      <c r="AA46" s="107"/>
-      <c r="AB46" s="107"/>
-      <c r="AC46" s="107"/>
-      <c r="AD46" s="107"/>
-      <c r="AE46" s="107"/>
-      <c r="AF46" s="107"/>
-      <c r="AG46" s="106"/>
+      <c r="E46" s="105"/>
+      <c r="F46" s="105"/>
+      <c r="G46" s="105"/>
+      <c r="H46" s="105"/>
+      <c r="I46" s="105"/>
+      <c r="J46" s="105"/>
+      <c r="K46" s="105"/>
+      <c r="L46" s="105"/>
+      <c r="M46" s="105"/>
+      <c r="N46" s="105"/>
+      <c r="O46" s="106"/>
+      <c r="P46" s="106"/>
+      <c r="Q46" s="106"/>
+      <c r="R46" s="106"/>
+      <c r="S46" s="106"/>
+      <c r="T46" s="106"/>
+      <c r="U46" s="106"/>
+      <c r="V46" s="106"/>
+      <c r="W46" s="106"/>
+      <c r="X46" s="106"/>
+      <c r="Y46" s="106"/>
+      <c r="Z46" s="106"/>
+      <c r="AA46" s="106"/>
+      <c r="AB46" s="106"/>
+      <c r="AC46" s="106"/>
+      <c r="AD46" s="106"/>
+      <c r="AE46" s="106"/>
+      <c r="AF46" s="106"/>
+      <c r="AG46" s="105"/>
     </row>
     <row r="47" spans="2:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B47" s="6"/>
@@ -4204,72 +4204,79 @@
       <c r="D47" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E47" s="106"/>
-      <c r="F47" s="106"/>
-      <c r="G47" s="106"/>
-      <c r="H47" s="106"/>
-      <c r="I47" s="106"/>
-      <c r="J47" s="106"/>
-      <c r="K47" s="106"/>
-      <c r="L47" s="106"/>
-      <c r="M47" s="106"/>
-      <c r="N47" s="106"/>
-      <c r="O47" s="107"/>
-      <c r="P47" s="107"/>
-      <c r="Q47" s="107"/>
-      <c r="R47" s="107"/>
-      <c r="S47" s="107"/>
-      <c r="T47" s="107"/>
-      <c r="U47" s="107"/>
-      <c r="V47" s="107"/>
-      <c r="W47" s="107"/>
-      <c r="X47" s="107"/>
-      <c r="Y47" s="107"/>
-      <c r="Z47" s="107"/>
-      <c r="AA47" s="107"/>
-      <c r="AB47" s="107"/>
-      <c r="AC47" s="107"/>
-      <c r="AD47" s="107"/>
-      <c r="AE47" s="107"/>
-      <c r="AF47" s="107"/>
-      <c r="AG47" s="106"/>
+      <c r="E47" s="105"/>
+      <c r="F47" s="105"/>
+      <c r="G47" s="105"/>
+      <c r="H47" s="105"/>
+      <c r="I47" s="105"/>
+      <c r="J47" s="105"/>
+      <c r="K47" s="105"/>
+      <c r="L47" s="105"/>
+      <c r="M47" s="105"/>
+      <c r="N47" s="105"/>
+      <c r="O47" s="106"/>
+      <c r="P47" s="106"/>
+      <c r="Q47" s="106"/>
+      <c r="R47" s="106"/>
+      <c r="S47" s="106"/>
+      <c r="T47" s="106"/>
+      <c r="U47" s="106"/>
+      <c r="V47" s="106"/>
+      <c r="W47" s="106"/>
+      <c r="X47" s="106"/>
+      <c r="Y47" s="106"/>
+      <c r="Z47" s="106"/>
+      <c r="AA47" s="106"/>
+      <c r="AB47" s="106"/>
+      <c r="AC47" s="106"/>
+      <c r="AD47" s="106"/>
+      <c r="AE47" s="106"/>
+      <c r="AF47" s="106"/>
+      <c r="AG47" s="105"/>
     </row>
     <row r="48" spans="2:33" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B48" s="106"/>
-      <c r="C48" s="106"/>
-      <c r="D48" s="106"/>
-      <c r="E48" s="106"/>
-      <c r="F48" s="106"/>
-      <c r="G48" s="106"/>
-      <c r="H48" s="106"/>
-      <c r="I48" s="106"/>
-      <c r="J48" s="106"/>
-      <c r="K48" s="106"/>
-      <c r="L48" s="106"/>
-      <c r="M48" s="106"/>
-      <c r="N48" s="106"/>
-      <c r="O48" s="107"/>
-      <c r="P48" s="107"/>
-      <c r="Q48" s="107"/>
-      <c r="R48" s="107"/>
-      <c r="S48" s="107"/>
-      <c r="T48" s="107"/>
-      <c r="U48" s="107"/>
-      <c r="V48" s="107"/>
-      <c r="W48" s="107"/>
-      <c r="X48" s="107"/>
-      <c r="Y48" s="107"/>
-      <c r="Z48" s="107"/>
-      <c r="AA48" s="107"/>
-      <c r="AB48" s="107"/>
-      <c r="AC48" s="107"/>
-      <c r="AD48" s="107"/>
-      <c r="AE48" s="107"/>
-      <c r="AF48" s="107"/>
-      <c r="AG48" s="106"/>
+      <c r="B48" s="105"/>
+      <c r="C48" s="105"/>
+      <c r="D48" s="105"/>
+      <c r="E48" s="105"/>
+      <c r="F48" s="105"/>
+      <c r="G48" s="105"/>
+      <c r="H48" s="105"/>
+      <c r="I48" s="105"/>
+      <c r="J48" s="105"/>
+      <c r="K48" s="105"/>
+      <c r="L48" s="105"/>
+      <c r="M48" s="105"/>
+      <c r="N48" s="105"/>
+      <c r="O48" s="106"/>
+      <c r="P48" s="106"/>
+      <c r="Q48" s="106"/>
+      <c r="R48" s="106"/>
+      <c r="S48" s="106"/>
+      <c r="T48" s="106"/>
+      <c r="U48" s="106"/>
+      <c r="V48" s="106"/>
+      <c r="W48" s="106"/>
+      <c r="X48" s="106"/>
+      <c r="Y48" s="106"/>
+      <c r="Z48" s="106"/>
+      <c r="AA48" s="106"/>
+      <c r="AB48" s="106"/>
+      <c r="AC48" s="106"/>
+      <c r="AD48" s="106"/>
+      <c r="AE48" s="106"/>
+      <c r="AF48" s="106"/>
+      <c r="AG48" s="105"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B10:AG10"/>
+    <mergeCell ref="H11:L11"/>
+    <mergeCell ref="B3:AG3"/>
+    <mergeCell ref="B4:AG4"/>
+    <mergeCell ref="B5:AG5"/>
+    <mergeCell ref="B6:AG6"/>
+    <mergeCell ref="B7:AG7"/>
     <mergeCell ref="B45:C45"/>
     <mergeCell ref="AE16:AF16"/>
     <mergeCell ref="J16:K16"/>
@@ -4279,13 +4286,6 @@
     <mergeCell ref="J14:L14"/>
     <mergeCell ref="F42:G42"/>
     <mergeCell ref="V43:Y43"/>
-    <mergeCell ref="B10:AG10"/>
-    <mergeCell ref="H11:L11"/>
-    <mergeCell ref="B3:AG3"/>
-    <mergeCell ref="B4:AG4"/>
-    <mergeCell ref="B5:AG5"/>
-    <mergeCell ref="B6:AG6"/>
-    <mergeCell ref="B7:AG7"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="1.299212598425197" right="0.70866141732283472" top="0.35433070866141736" bottom="0.35433070866141736" header="0.51181102362204722" footer="0.31496062992125984"/>

</xml_diff>